<commit_message>
Auto: update momentum data - 2025-11-05 04:01 UTC
</commit_message>
<xml_diff>
--- a/data/trending_momentum_stocks.xlsx
+++ b/data/trending_momentum_stocks.xlsx
@@ -546,11 +546,11 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
-        <v>-2.7</v>
+        <v>-3.6</v>
       </c>
     </row>
     <row r="5">
@@ -572,11 +572,11 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>9.77</v>
+        <v>9.4</v>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
-        <v>-5.15</v>
+        <v>-8.74</v>
       </c>
     </row>
     <row r="6">
@@ -598,11 +598,11 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>34230</v>
+        <v>35780</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
-        <v>3.54</v>
+        <v>8.23</v>
       </c>
     </row>
     <row r="7">
@@ -624,11 +624,11 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>19292</v>
+        <v>20341</v>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
-        <v>0.43</v>
+        <v>5.89</v>
       </c>
     </row>
     <row r="8">
@@ -650,11 +650,11 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>13.04</v>
+        <v>12.8</v>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
-        <v>-3.26</v>
+        <v>-5.04</v>
       </c>
     </row>
     <row r="9">
@@ -676,11 +676,11 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>251.31</v>
+        <v>254.6</v>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
-        <v>0.12</v>
+        <v>1.43</v>
       </c>
     </row>
     <row r="10">
@@ -702,11 +702,11 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>271.1</v>
+        <v>271</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
-        <v>-6.15</v>
+        <v>-6.18</v>
       </c>
     </row>
     <row r="11">
@@ -728,11 +728,11 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>249.4</v>
+        <v>244</v>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="n">
-        <v>-1.81</v>
+        <v>-3.94</v>
       </c>
     </row>
     <row r="12">
@@ -754,11 +754,11 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>342</v>
+        <v>330.95</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="n">
-        <v>4.91</v>
+        <v>1.52</v>
       </c>
     </row>
     <row r="13">
@@ -806,11 +806,11 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>41</v>
+        <v>41.4</v>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="n">
-        <v>-4.07</v>
+        <v>-3.14</v>
       </c>
     </row>
     <row r="15">
@@ -884,11 +884,11 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>176</v>
+        <v>184.43</v>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="n">
-        <v>-4.57</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -936,11 +936,11 @@
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>236</v>
+        <v>230.9</v>
       </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="n">
-        <v>-1.1</v>
+        <v>-3.24</v>
       </c>
     </row>
     <row r="20">
@@ -962,11 +962,11 @@
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>70.34999999999999</v>
+        <v>69</v>
       </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>-1.92</v>
       </c>
     </row>
     <row r="21">
@@ -988,11 +988,11 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>76</v>
+        <v>76.28</v>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
-        <v>-0.55</v>
+        <v>-0.18</v>
       </c>
     </row>
     <row r="22">
@@ -1014,11 +1014,11 @@
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>54.75</v>
+        <v>54.8</v>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="n">
-        <v>-0.09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1066,11 +1066,11 @@
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>921.5</v>
+        <v>895.75</v>
       </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="n">
-        <v>-1.22</v>
+        <v>-3.98</v>
       </c>
     </row>
     <row r="25">
@@ -1170,11 +1170,11 @@
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>1725</v>
+        <v>1729</v>
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="n">
-        <v>1.17</v>
+        <v>1.41</v>
       </c>
     </row>
     <row r="29">
@@ -1222,11 +1222,11 @@
         <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>1589.2</v>
+        <v>1585</v>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="n">
-        <v>1.87</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="31">
@@ -1248,11 +1248,11 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>585.7</v>
+        <v>574.05</v>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="n">
-        <v>-4.76</v>
+        <v>-6.66</v>
       </c>
     </row>
     <row r="32">
@@ -1274,11 +1274,11 @@
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>273.65</v>
+        <v>272.6</v>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="n">
-        <v>-3.64</v>
+        <v>-4.01</v>
       </c>
     </row>
     <row r="33">
@@ -1300,11 +1300,11 @@
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>7.99</v>
+        <v>8.630000000000001</v>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="n">
-        <v>5.41</v>
+        <v>13.85</v>
       </c>
     </row>
     <row r="34">
@@ -1326,11 +1326,11 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>14.51</v>
+        <v>14</v>
       </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="n">
-        <v>-2.81</v>
+        <v>-6.23</v>
       </c>
     </row>
     <row r="35">
@@ -1352,11 +1352,11 @@
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>224.28</v>
+        <v>221.26</v>
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="n">
-        <v>-2.91</v>
+        <v>-4.22</v>
       </c>
     </row>
     <row r="36">
@@ -1378,11 +1378,11 @@
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>2890</v>
+        <v>3033</v>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="n">
-        <v>6.68</v>
+        <v>11.96</v>
       </c>
     </row>
     <row r="37">
@@ -1404,11 +1404,11 @@
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>475</v>
+        <v>412.6</v>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="n">
-        <v>2.37</v>
+        <v>-11.08</v>
       </c>
     </row>
     <row r="38">
@@ -1430,11 +1430,11 @@
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>43.5</v>
+        <v>43.89</v>
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="n">
-        <v>0.23</v>
+        <v>1.13</v>
       </c>
     </row>
     <row r="39">
@@ -1456,11 +1456,11 @@
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>786.9</v>
+        <v>785.85</v>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="n">
-        <v>-1.88</v>
+        <v>-2.01</v>
       </c>
     </row>
     <row r="40">
@@ -1508,11 +1508,11 @@
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>899.65</v>
+        <v>869.9</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="n">
-        <v>1.2</v>
+        <v>-2.15</v>
       </c>
     </row>
     <row r="42">
@@ -1534,11 +1534,11 @@
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>241.57</v>
+        <v>230.75</v>
       </c>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="n">
-        <v>-0.77</v>
+        <v>-5.22</v>
       </c>
     </row>
     <row r="43">
@@ -1560,11 +1560,11 @@
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>105.79</v>
+        <v>104.55</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="n">
-        <v>-2.94</v>
+        <v>-4.08</v>
       </c>
     </row>
     <row r="44">
@@ -1586,11 +1586,11 @@
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>136.56</v>
+        <v>138</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="n">
-        <v>-3.83</v>
+        <v>-2.82</v>
       </c>
     </row>
     <row r="45">
@@ -1634,11 +1634,11 @@
         <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>464.95</v>
+        <v>436.7</v>
       </c>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="n">
-        <v>-2.1</v>
+        <v>-8.039999999999999</v>
       </c>
     </row>
     <row r="47">
@@ -1660,11 +1660,11 @@
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>11.56</v>
+        <v>11.44</v>
       </c>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="n">
-        <v>-2.45</v>
+        <v>-3.46</v>
       </c>
     </row>
     <row r="48">
@@ -1686,11 +1686,11 @@
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>2.18</v>
+        <v>2.15</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="n">
-        <v>-0.46</v>
+        <v>-1.83</v>
       </c>
     </row>
     <row r="49">
@@ -1738,11 +1738,11 @@
         <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>309.05</v>
+        <v>306.6</v>
       </c>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="n">
-        <v>-1.86</v>
+        <v>-2.64</v>
       </c>
     </row>
     <row r="51">
@@ -1790,11 +1790,11 @@
         <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>18.97</v>
+        <v>17.85</v>
       </c>
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="n">
-        <v>-1.04</v>
+        <v>-6.89</v>
       </c>
     </row>
     <row r="53">
@@ -1816,11 +1816,11 @@
         <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>29.8</v>
+        <v>29.15</v>
       </c>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="n">
-        <v>-1.81</v>
+        <v>-3.95</v>
       </c>
     </row>
     <row r="54">
@@ -1842,11 +1842,11 @@
         <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>7.03</v>
+        <v>7.08</v>
       </c>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="n">
-        <v>-3.96</v>
+        <v>-3.28</v>
       </c>
     </row>
     <row r="55">
@@ -1868,11 +1868,11 @@
         <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>348.7</v>
+        <v>344</v>
       </c>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="n">
-        <v>-2.41</v>
+        <v>-3.72</v>
       </c>
     </row>
     <row r="56">
@@ -1894,11 +1894,11 @@
         <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>67.13</v>
+        <v>68.40000000000001</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="n">
-        <v>-4.1</v>
+        <v>-2.29</v>
       </c>
     </row>
     <row r="57">
@@ -1920,11 +1920,11 @@
         <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>15137</v>
+        <v>15183</v>
       </c>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="n">
-        <v>-2.32</v>
+        <v>-2.02</v>
       </c>
     </row>
     <row r="58">
@@ -1946,11 +1946,11 @@
         <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>251.69</v>
+        <v>246.5</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="n">
-        <v>-1.3</v>
+        <v>-3.33</v>
       </c>
     </row>
     <row r="59">
@@ -1972,11 +1972,11 @@
         <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>557</v>
+        <v>557.4</v>
       </c>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="n">
-        <v>2.01</v>
+        <v>2.09</v>
       </c>
     </row>
     <row r="60">
@@ -1998,11 +1998,11 @@
         <v>0</v>
       </c>
       <c r="F60" t="n">
-        <v>606.3</v>
+        <v>609.75</v>
       </c>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="n">
-        <v>-2.05</v>
+        <v>-1.49</v>
       </c>
     </row>
     <row r="61">
@@ -2024,11 +2024,11 @@
         <v>0</v>
       </c>
       <c r="F61" t="n">
-        <v>714.95</v>
+        <v>709.9</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="n">
-        <v>2.28</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="62">
@@ -2050,11 +2050,11 @@
         <v>0</v>
       </c>
       <c r="F62" t="n">
-        <v>1033</v>
+        <v>1000.3</v>
       </c>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="n">
-        <v>0</v>
+        <v>-3.17</v>
       </c>
     </row>
     <row r="63">
@@ -2076,11 +2076,11 @@
         <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>58.6</v>
+        <v>57.2</v>
       </c>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="n">
-        <v>-2.01</v>
+        <v>-4.35</v>
       </c>
     </row>
     <row r="64">
@@ -2102,11 +2102,11 @@
         <v>0</v>
       </c>
       <c r="F64" t="n">
-        <v>1.55</v>
+        <v>1.54</v>
       </c>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="n">
-        <v>0</v>
+        <v>-0.65</v>
       </c>
     </row>
     <row r="65">
@@ -2128,11 +2128,11 @@
         <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>29.95</v>
+        <v>28.9</v>
       </c>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="n">
-        <v>-0.83</v>
+        <v>-4.3</v>
       </c>
     </row>
     <row r="66">
@@ -2154,11 +2154,11 @@
         <v>0</v>
       </c>
       <c r="F66" t="n">
-        <v>156.82</v>
+        <v>154</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="n">
-        <v>-0.49</v>
+        <v>-2.28</v>
       </c>
     </row>
     <row r="67">
@@ -2180,11 +2180,11 @@
         <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>219.99</v>
+        <v>212.65</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="n">
-        <v>0</v>
+        <v>-3.34</v>
       </c>
     </row>
     <row r="68">
@@ -2206,11 +2206,11 @@
         <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>76.37</v>
+        <v>76.40000000000001</v>
       </c>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="n">
-        <v>-0.82</v>
+        <v>-0.78</v>
       </c>
     </row>
     <row r="69">
@@ -2232,11 +2232,11 @@
         <v>0</v>
       </c>
       <c r="F69" t="n">
-        <v>200.24</v>
+        <v>193.9</v>
       </c>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="n">
-        <v>-1.26</v>
+        <v>-4.39</v>
       </c>
     </row>
     <row r="70">
@@ -2258,11 +2258,11 @@
         <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>480.5</v>
+        <v>469.6</v>
       </c>
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="n">
-        <v>-0.65</v>
+        <v>-2.9</v>
       </c>
     </row>
     <row r="71">
@@ -2284,11 +2284,11 @@
         <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>8.279999999999999</v>
+        <v>8.050000000000001</v>
       </c>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="n">
-        <v>-0.72</v>
+        <v>-3.48</v>
       </c>
     </row>
     <row r="72">
@@ -2310,11 +2310,11 @@
         <v>0</v>
       </c>
       <c r="F72" t="n">
-        <v>53.71</v>
+        <v>52.5</v>
       </c>
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="n">
-        <v>-1.27</v>
+        <v>-3.49</v>
       </c>
     </row>
     <row r="73">
@@ -2336,11 +2336,11 @@
         <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>392.85</v>
+        <v>392.3</v>
       </c>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="n">
-        <v>0.22</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="74">
@@ -2362,11 +2362,11 @@
         <v>0</v>
       </c>
       <c r="F74" t="n">
-        <v>29.7</v>
+        <v>27.95</v>
       </c>
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="n">
-        <v>0</v>
+        <v>-5.89</v>
       </c>
     </row>
     <row r="75">
@@ -2388,11 +2388,11 @@
         <v>0</v>
       </c>
       <c r="F75" t="n">
-        <v>170.46</v>
+        <v>171</v>
       </c>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="n">
-        <v>-3.69</v>
+        <v>-3.39</v>
       </c>
     </row>
     <row r="76">
@@ -2414,11 +2414,11 @@
         <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>350.5</v>
+        <v>343.65</v>
       </c>
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="n">
-        <v>2.97</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="77">
@@ -2440,11 +2440,11 @@
         <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>973.85</v>
+        <v>952</v>
       </c>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="n">
-        <v>-1.33</v>
+        <v>-3.55</v>
       </c>
     </row>
     <row r="78">
@@ -2466,11 +2466,11 @@
         <v>0</v>
       </c>
       <c r="F78" t="n">
-        <v>1410.3</v>
+        <v>1389.3</v>
       </c>
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="n">
-        <v>-0.93</v>
+        <v>-2.41</v>
       </c>
     </row>
     <row r="79">
@@ -2492,11 +2492,11 @@
         <v>0</v>
       </c>
       <c r="F79" t="n">
-        <v>78.44</v>
+        <v>80.05</v>
       </c>
       <c r="G79" t="inlineStr"/>
       <c r="H79" t="n">
-        <v>0.5600000000000001</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="80">
@@ -2518,11 +2518,11 @@
         <v>0</v>
       </c>
       <c r="F80" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="n">
-        <v>-2.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -2544,11 +2544,11 @@
         <v>0</v>
       </c>
       <c r="F81" t="n">
-        <v>598.3</v>
+        <v>609</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="n">
-        <v>-1.55</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="82">
@@ -2570,11 +2570,11 @@
         <v>0</v>
       </c>
       <c r="F82" t="n">
-        <v>10.34</v>
+        <v>10.07</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="n">
-        <v>-0.86</v>
+        <v>-3.45</v>
       </c>
     </row>
     <row r="83">
@@ -2622,11 +2622,11 @@
         <v>0</v>
       </c>
       <c r="F84" t="n">
-        <v>222.95</v>
+        <v>219.05</v>
       </c>
       <c r="G84" t="inlineStr"/>
       <c r="H84" t="n">
-        <v>-0.89</v>
+        <v>-2.62</v>
       </c>
     </row>
     <row r="85">
@@ -2648,11 +2648,11 @@
         <v>0</v>
       </c>
       <c r="F85" t="n">
-        <v>178.45</v>
+        <v>180</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="n">
-        <v>-0.86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -2674,11 +2674,11 @@
         <v>0</v>
       </c>
       <c r="F86" t="n">
-        <v>105.99</v>
+        <v>105.69</v>
       </c>
       <c r="G86" t="inlineStr"/>
       <c r="H86" t="n">
-        <v>0.42</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="87">
@@ -2700,11 +2700,11 @@
         <v>0</v>
       </c>
       <c r="F87" t="n">
-        <v>8.57</v>
+        <v>8.5</v>
       </c>
       <c r="G87" t="inlineStr"/>
       <c r="H87" t="n">
-        <v>-1.04</v>
+        <v>-1.85</v>
       </c>
     </row>
     <row r="88">
@@ -2726,11 +2726,11 @@
         <v>0</v>
       </c>
       <c r="F88" t="n">
-        <v>195</v>
+        <v>188.5</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="n">
-        <v>-1.22</v>
+        <v>-4.51</v>
       </c>
     </row>
     <row r="89">
@@ -2752,11 +2752,11 @@
         <v>0</v>
       </c>
       <c r="F89" t="n">
-        <v>157.27</v>
+        <v>153.38</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="n">
-        <v>-1.37</v>
+        <v>-3.81</v>
       </c>
     </row>
     <row r="90">
@@ -2778,11 +2778,11 @@
         <v>0</v>
       </c>
       <c r="F90" t="n">
-        <v>6.84</v>
+        <v>6.8</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="n">
-        <v>-2.01</v>
+        <v>-2.58</v>
       </c>
     </row>
     <row r="91">
@@ -2804,11 +2804,11 @@
         <v>0</v>
       </c>
       <c r="F91" t="n">
-        <v>4.65</v>
+        <v>4.47</v>
       </c>
       <c r="G91" t="inlineStr"/>
       <c r="H91" t="n">
-        <v>-0.21</v>
+        <v>-4.08</v>
       </c>
     </row>
     <row r="92">
@@ -2830,11 +2830,11 @@
         <v>0</v>
       </c>
       <c r="F92" t="n">
-        <v>1.86</v>
+        <v>1.79</v>
       </c>
       <c r="G92" t="inlineStr"/>
       <c r="H92" t="n">
-        <v>-1.06</v>
+        <v>-4.79</v>
       </c>
     </row>
     <row r="93">
@@ -2856,11 +2856,11 @@
         <v>0</v>
       </c>
       <c r="F93" t="n">
-        <v>157.79</v>
+        <v>157.71</v>
       </c>
       <c r="G93" t="inlineStr"/>
       <c r="H93" t="n">
-        <v>-1.07</v>
+        <v>-1.12</v>
       </c>
     </row>
     <row r="94">
@@ -2882,11 +2882,11 @@
         <v>0</v>
       </c>
       <c r="F94" t="n">
-        <v>446.45</v>
+        <v>457.5</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="n">
-        <v>-0.77</v>
+        <v>1.69</v>
       </c>
     </row>
     <row r="95">
@@ -2908,11 +2908,11 @@
         <v>0</v>
       </c>
       <c r="F95" t="n">
-        <v>49.5</v>
+        <v>49.16</v>
       </c>
       <c r="G95" t="inlineStr"/>
       <c r="H95" t="n">
-        <v>-0.9</v>
+        <v>-1.58</v>
       </c>
     </row>
     <row r="96">
@@ -2934,11 +2934,11 @@
         <v>0</v>
       </c>
       <c r="F96" t="n">
-        <v>15.66</v>
+        <v>14.9</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="n">
-        <v>-0.89</v>
+        <v>-5.7</v>
       </c>
     </row>
     <row r="97">
@@ -2960,11 +2960,11 @@
         <v>0</v>
       </c>
       <c r="F97" t="n">
-        <v>71.37</v>
+        <v>73</v>
       </c>
       <c r="G97" t="inlineStr"/>
       <c r="H97" t="n">
-        <v>-2.88</v>
+        <v>-0.67</v>
       </c>
     </row>
     <row r="98">
@@ -2986,11 +2986,11 @@
         <v>0</v>
       </c>
       <c r="F98" t="n">
-        <v>189.91</v>
+        <v>186.4</v>
       </c>
       <c r="G98" t="inlineStr"/>
       <c r="H98" t="n">
-        <v>-1.4</v>
+        <v>-3.22</v>
       </c>
     </row>
     <row r="99">
@@ -3012,11 +3012,11 @@
         <v>0</v>
       </c>
       <c r="F99" t="n">
-        <v>8</v>
+        <v>8.1</v>
       </c>
       <c r="G99" t="inlineStr"/>
       <c r="H99" t="n">
-        <v>-1.6</v>
+        <v>-0.37</v>
       </c>
     </row>
     <row r="100">
@@ -3038,11 +3038,11 @@
         <v>0</v>
       </c>
       <c r="F100" t="n">
-        <v>19.85</v>
+        <v>19.35</v>
       </c>
       <c r="G100" t="inlineStr"/>
       <c r="H100" t="n">
-        <v>-0.75</v>
+        <v>-3.25</v>
       </c>
     </row>
     <row r="101">
@@ -3064,11 +3064,11 @@
         <v>0</v>
       </c>
       <c r="F101" t="n">
-        <v>9.640000000000001</v>
+        <v>9.380000000000001</v>
       </c>
       <c r="G101" t="inlineStr"/>
       <c r="H101" t="n">
-        <v>-0.92</v>
+        <v>-3.6</v>
       </c>
     </row>
     <row r="102">
@@ -3090,11 +3090,11 @@
         <v>0</v>
       </c>
       <c r="F102" t="n">
-        <v>30.09</v>
+        <v>29.11</v>
       </c>
       <c r="G102" t="inlineStr"/>
       <c r="H102" t="n">
-        <v>-0.86</v>
+        <v>-4.09</v>
       </c>
     </row>
     <row r="103">
@@ -3116,11 +3116,11 @@
         <v>0</v>
       </c>
       <c r="F103" t="n">
-        <v>162.25</v>
+        <v>161.05</v>
       </c>
       <c r="G103" t="inlineStr"/>
       <c r="H103" t="n">
-        <v>-1.67</v>
+        <v>-2.39</v>
       </c>
     </row>
     <row r="104">
@@ -3142,11 +3142,11 @@
         <v>0</v>
       </c>
       <c r="F104" t="n">
-        <v>173.81</v>
+        <v>164.3</v>
       </c>
       <c r="G104" t="inlineStr"/>
       <c r="H104" t="n">
-        <v>6.31</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="105">
@@ -3168,11 +3168,11 @@
         <v>0</v>
       </c>
       <c r="F105" t="n">
-        <v>91.73999999999999</v>
+        <v>92</v>
       </c>
       <c r="G105" t="inlineStr"/>
       <c r="H105" t="n">
-        <v>-2.2</v>
+        <v>-1.92</v>
       </c>
     </row>
     <row r="106">
@@ -3194,11 +3194,11 @@
         <v>0</v>
       </c>
       <c r="F106" t="n">
-        <v>26.07</v>
+        <v>26.29</v>
       </c>
       <c r="G106" t="inlineStr"/>
       <c r="H106" t="n">
-        <v>-1.55</v>
+        <v>-0.72</v>
       </c>
     </row>
     <row r="107">
@@ -3220,11 +3220,11 @@
         <v>0</v>
       </c>
       <c r="F107" t="n">
-        <v>148.59</v>
+        <v>147</v>
       </c>
       <c r="G107" t="inlineStr"/>
       <c r="H107" t="n">
-        <v>-0.9399999999999999</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="108">
@@ -3246,11 +3246,11 @@
         <v>0</v>
       </c>
       <c r="F108" t="n">
-        <v>25.03</v>
+        <v>24.31</v>
       </c>
       <c r="G108" t="inlineStr"/>
       <c r="H108" t="n">
-        <v>-0.48</v>
+        <v>-3.34</v>
       </c>
     </row>
     <row r="109">
@@ -3272,11 +3272,11 @@
         <v>0</v>
       </c>
       <c r="F109" t="n">
-        <v>1202.8</v>
+        <v>1190</v>
       </c>
       <c r="G109" t="inlineStr"/>
       <c r="H109" t="n">
-        <v>-1</v>
+        <v>-2.06</v>
       </c>
     </row>
     <row r="110">
@@ -3298,11 +3298,11 @@
         <v>0</v>
       </c>
       <c r="F110" t="n">
-        <v>35.61</v>
+        <v>35.85</v>
       </c>
       <c r="G110" t="inlineStr"/>
       <c r="H110" t="n">
-        <v>-0.25</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="111">
@@ -3324,11 +3324,11 @@
         <v>0</v>
       </c>
       <c r="F111" t="n">
-        <v>114</v>
+        <v>112.19</v>
       </c>
       <c r="G111" t="inlineStr"/>
       <c r="H111" t="n">
-        <v>-1.04</v>
+        <v>-2.61</v>
       </c>
     </row>
     <row r="112">
@@ -3350,11 +3350,11 @@
         <v>0</v>
       </c>
       <c r="F112" t="n">
-        <v>208.57</v>
+        <v>210</v>
       </c>
       <c r="G112" t="inlineStr"/>
       <c r="H112" t="n">
-        <v>-2.08</v>
+        <v>-1.41</v>
       </c>
     </row>
     <row r="113">
@@ -3376,11 +3376,11 @@
         <v>0</v>
       </c>
       <c r="F113" t="n">
-        <v>85.31999999999999</v>
+        <v>84.27</v>
       </c>
       <c r="G113" t="inlineStr"/>
       <c r="H113" t="n">
-        <v>-1.67</v>
+        <v>-2.88</v>
       </c>
     </row>
     <row r="114">
@@ -3402,11 +3402,11 @@
         <v>0</v>
       </c>
       <c r="F114" t="n">
-        <v>19.34</v>
+        <v>19.35</v>
       </c>
       <c r="G114" t="inlineStr"/>
       <c r="H114" t="n">
-        <v>-1.83</v>
+        <v>-1.78</v>
       </c>
     </row>
     <row r="115">
@@ -3428,11 +3428,11 @@
         <v>0</v>
       </c>
       <c r="F115" t="n">
-        <v>38.6</v>
+        <v>37.9</v>
       </c>
       <c r="G115" t="inlineStr"/>
       <c r="H115" t="n">
-        <v>-2.25</v>
+        <v>-4.03</v>
       </c>
     </row>
     <row r="116">
@@ -3454,11 +3454,11 @@
         <v>0</v>
       </c>
       <c r="F116" t="n">
-        <v>777.5</v>
+        <v>789.95</v>
       </c>
       <c r="G116" t="inlineStr"/>
       <c r="H116" t="n">
-        <v>-0.96</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="117">
@@ -3480,11 +3480,11 @@
         <v>0</v>
       </c>
       <c r="F117" t="n">
-        <v>4.27</v>
+        <v>4.24</v>
       </c>
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="n">
-        <v>-0.47</v>
+        <v>-1.17</v>
       </c>
     </row>
     <row r="118">
@@ -3506,11 +3506,11 @@
         <v>0</v>
       </c>
       <c r="F118" t="n">
-        <v>126.7</v>
+        <v>124.55</v>
       </c>
       <c r="G118" t="inlineStr"/>
       <c r="H118" t="n">
-        <v>-0.16</v>
+        <v>-1.85</v>
       </c>
     </row>
     <row r="119">
@@ -3532,11 +3532,11 @@
         <v>0</v>
       </c>
       <c r="F119" t="n">
-        <v>115.04</v>
+        <v>113.5</v>
       </c>
       <c r="G119" t="inlineStr"/>
       <c r="H119" t="n">
-        <v>-2.52</v>
+        <v>-3.83</v>
       </c>
     </row>
     <row r="120">
@@ -3558,11 +3558,11 @@
         <v>0</v>
       </c>
       <c r="F120" t="n">
-        <v>80.48</v>
+        <v>77.2</v>
       </c>
       <c r="G120" t="inlineStr"/>
       <c r="H120" t="n">
-        <v>-0.26</v>
+        <v>-4.33</v>
       </c>
     </row>
     <row r="121">
@@ -3584,11 +3584,11 @@
         <v>0</v>
       </c>
       <c r="F121" t="n">
-        <v>150.1</v>
+        <v>136.8</v>
       </c>
       <c r="G121" t="inlineStr"/>
       <c r="H121" t="n">
-        <v>-1.57</v>
+        <v>-10.3</v>
       </c>
     </row>
     <row r="122">
@@ -3610,11 +3610,11 @@
         <v>0</v>
       </c>
       <c r="F122" t="n">
-        <v>28.22</v>
+        <v>28.7</v>
       </c>
       <c r="G122" t="inlineStr"/>
       <c r="H122" t="n">
-        <v>-3.36</v>
+        <v>-1.71</v>
       </c>
     </row>
     <row r="123">
@@ -3636,11 +3636,11 @@
         <v>0</v>
       </c>
       <c r="F123" t="n">
-        <v>1205</v>
+        <v>1186.5</v>
       </c>
       <c r="G123" t="inlineStr"/>
       <c r="H123" t="n">
-        <v>-2.81</v>
+        <v>-4.31</v>
       </c>
     </row>
     <row r="124">
@@ -3688,11 +3688,11 @@
         <v>0</v>
       </c>
       <c r="F125" t="n">
-        <v>33</v>
+        <v>32.52</v>
       </c>
       <c r="G125" t="inlineStr"/>
       <c r="H125" t="n">
-        <v>-2.16</v>
+        <v>-3.59</v>
       </c>
     </row>
     <row r="126">
@@ -3714,11 +3714,11 @@
         <v>0</v>
       </c>
       <c r="F126" t="n">
-        <v>4.41</v>
+        <v>4.36</v>
       </c>
       <c r="G126" t="inlineStr"/>
       <c r="H126" t="n">
-        <v>-2</v>
+        <v>-3.11</v>
       </c>
     </row>
     <row r="127">
@@ -3740,11 +3740,11 @@
         <v>0</v>
       </c>
       <c r="F127" t="n">
-        <v>44.38</v>
+        <v>44.2</v>
       </c>
       <c r="G127" t="inlineStr"/>
       <c r="H127" t="n">
-        <v>-1.38</v>
+        <v>-1.78</v>
       </c>
     </row>
     <row r="128">
@@ -3766,11 +3766,11 @@
         <v>0</v>
       </c>
       <c r="F128" t="n">
-        <v>103.26</v>
+        <v>93.90000000000001</v>
       </c>
       <c r="G128" t="inlineStr"/>
       <c r="H128" t="n">
-        <v>-5.27</v>
+        <v>-13.85</v>
       </c>
     </row>
     <row r="129">
@@ -3792,11 +3792,11 @@
         <v>0</v>
       </c>
       <c r="F129" t="n">
-        <v>42.78</v>
+        <v>42.56</v>
       </c>
       <c r="G129" t="inlineStr"/>
       <c r="H129" t="n">
-        <v>-2.44</v>
+        <v>-2.94</v>
       </c>
     </row>
     <row r="130">
@@ -3818,11 +3818,11 @@
         <v>0</v>
       </c>
       <c r="F130" t="n">
-        <v>1449.9</v>
+        <v>1431.4</v>
       </c>
       <c r="G130" t="inlineStr"/>
       <c r="H130" t="n">
-        <v>-1.37</v>
+        <v>-2.63</v>
       </c>
     </row>
     <row r="131">
@@ -3844,11 +3844,11 @@
         <v>0</v>
       </c>
       <c r="F131" t="n">
-        <v>15.95</v>
+        <v>15.83</v>
       </c>
       <c r="G131" t="inlineStr"/>
       <c r="H131" t="n">
-        <v>-0.93</v>
+        <v>-1.68</v>
       </c>
     </row>
     <row r="132">
@@ -3870,11 +3870,11 @@
         <v>0</v>
       </c>
       <c r="F132" t="n">
-        <v>75.25</v>
+        <v>74.89</v>
       </c>
       <c r="G132" t="inlineStr"/>
       <c r="H132" t="n">
-        <v>-2.88</v>
+        <v>-3.34</v>
       </c>
     </row>
     <row r="133">
@@ -3896,11 +3896,11 @@
         <v>0</v>
       </c>
       <c r="F133" t="n">
-        <v>802</v>
+        <v>784</v>
       </c>
       <c r="G133" t="inlineStr"/>
       <c r="H133" t="n">
-        <v>-0.86</v>
+        <v>-3.08</v>
       </c>
     </row>
     <row r="134">
@@ -3922,11 +3922,11 @@
         <v>0</v>
       </c>
       <c r="F134" t="n">
-        <v>2.9</v>
+        <v>2.78</v>
       </c>
       <c r="G134" t="inlineStr"/>
       <c r="H134" t="n">
-        <v>-1.02</v>
+        <v>-5.12</v>
       </c>
     </row>
     <row r="135">
@@ -3948,11 +3948,11 @@
         <v>0</v>
       </c>
       <c r="F135" t="n">
-        <v>58.2</v>
+        <v>58.25</v>
       </c>
       <c r="G135" t="inlineStr"/>
       <c r="H135" t="n">
-        <v>-1.14</v>
+        <v>-1.05</v>
       </c>
     </row>
     <row r="136">
@@ -3974,11 +3974,11 @@
         <v>0</v>
       </c>
       <c r="F136" t="n">
-        <v>8.01</v>
+        <v>7.78</v>
       </c>
       <c r="G136" t="inlineStr"/>
       <c r="H136" t="n">
-        <v>-4.19</v>
+        <v>-6.94</v>
       </c>
     </row>
     <row r="137">
@@ -4000,11 +4000,11 @@
         <v>0</v>
       </c>
       <c r="F137" t="n">
-        <v>255.75</v>
+        <v>259</v>
       </c>
       <c r="G137" t="inlineStr"/>
       <c r="H137" t="n">
-        <v>-1.6</v>
+        <v>-0.35</v>
       </c>
     </row>
     <row r="138">
@@ -4026,11 +4026,11 @@
         <v>0</v>
       </c>
       <c r="F138" t="n">
-        <v>10.06</v>
+        <v>9.92</v>
       </c>
       <c r="G138" t="inlineStr"/>
       <c r="H138" t="n">
-        <v>-1.28</v>
+        <v>-2.65</v>
       </c>
     </row>
     <row r="139">
@@ -4052,11 +4052,11 @@
         <v>0</v>
       </c>
       <c r="F139" t="n">
-        <v>92.66</v>
+        <v>92.5</v>
       </c>
       <c r="G139" t="inlineStr"/>
       <c r="H139" t="n">
-        <v>-1.11</v>
+        <v>-1.28</v>
       </c>
     </row>
     <row r="140">
@@ -4078,11 +4078,11 @@
         <v>0</v>
       </c>
       <c r="F140" t="n">
-        <v>152.9</v>
+        <v>147.59</v>
       </c>
       <c r="G140" t="inlineStr"/>
       <c r="H140" t="n">
-        <v>-2.61</v>
+        <v>-5.99</v>
       </c>
     </row>
     <row r="141">
@@ -4104,11 +4104,11 @@
         <v>0</v>
       </c>
       <c r="F141" t="n">
-        <v>376.15</v>
+        <v>376</v>
       </c>
       <c r="G141" t="inlineStr"/>
       <c r="H141" t="n">
-        <v>-2.3</v>
+        <v>-2.34</v>
       </c>
     </row>
     <row r="142">
@@ -4130,11 +4130,11 @@
         <v>0</v>
       </c>
       <c r="F142" t="n">
-        <v>296.6</v>
+        <v>305.4</v>
       </c>
       <c r="G142" t="inlineStr"/>
       <c r="H142" t="n">
-        <v>-0.77</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="143">
@@ -4156,11 +4156,11 @@
         <v>0</v>
       </c>
       <c r="F143" t="n">
-        <v>27.97</v>
+        <v>27.4</v>
       </c>
       <c r="G143" t="inlineStr"/>
       <c r="H143" t="n">
-        <v>-1.1</v>
+        <v>-3.11</v>
       </c>
     </row>
     <row r="144">
@@ -4204,11 +4204,11 @@
         <v>0</v>
       </c>
       <c r="F145" t="n">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G145" t="inlineStr"/>
       <c r="H145" t="n">
-        <v>-1.22</v>
+        <v>-3.28</v>
       </c>
     </row>
     <row r="146">
@@ -4230,11 +4230,11 @@
         <v>0</v>
       </c>
       <c r="F146" t="n">
-        <v>121</v>
+        <v>116.11</v>
       </c>
       <c r="G146" t="inlineStr"/>
       <c r="H146" t="n">
-        <v>-1.62</v>
+        <v>-5.59</v>
       </c>
     </row>
     <row r="147">
@@ -4256,11 +4256,11 @@
         <v>0</v>
       </c>
       <c r="F147" t="n">
-        <v>1.25</v>
+        <v>1.23</v>
       </c>
       <c r="G147" t="inlineStr"/>
       <c r="H147" t="n">
-        <v>-0.79</v>
+        <v>-2.38</v>
       </c>
     </row>
     <row r="148">
@@ -4282,11 +4282,11 @@
         <v>0</v>
       </c>
       <c r="F148" t="n">
-        <v>172</v>
+        <v>172.95</v>
       </c>
       <c r="G148" t="inlineStr"/>
       <c r="H148" t="n">
-        <v>-1.71</v>
+        <v>-1.17</v>
       </c>
     </row>
     <row r="149">
@@ -4308,11 +4308,11 @@
         <v>0</v>
       </c>
       <c r="F149" t="n">
-        <v>1243.4</v>
+        <v>1197</v>
       </c>
       <c r="G149" t="inlineStr"/>
       <c r="H149" t="n">
-        <v>-2.46</v>
+        <v>-6.1</v>
       </c>
     </row>
     <row r="150">
@@ -4334,11 +4334,11 @@
         <v>0</v>
       </c>
       <c r="F150" t="n">
-        <v>2133.8</v>
+        <v>2110</v>
       </c>
       <c r="G150" t="inlineStr"/>
       <c r="H150" t="n">
-        <v>1.27</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="151">
@@ -4360,11 +4360,11 @@
         <v>0</v>
       </c>
       <c r="F151" t="n">
-        <v>10.52</v>
+        <v>10.51</v>
       </c>
       <c r="G151" t="inlineStr"/>
       <c r="H151" t="n">
-        <v>-3.49</v>
+        <v>-3.58</v>
       </c>
     </row>
     <row r="152">
@@ -4386,11 +4386,11 @@
         <v>0</v>
       </c>
       <c r="F152" t="n">
-        <v>3840</v>
+        <v>3740.7</v>
       </c>
       <c r="G152" t="inlineStr"/>
       <c r="H152" t="n">
-        <v>-0.39</v>
+        <v>-2.96</v>
       </c>
     </row>
     <row r="153">
@@ -4412,11 +4412,11 @@
         <v>0</v>
       </c>
       <c r="F153" t="n">
-        <v>5.17</v>
+        <v>5.15</v>
       </c>
       <c r="G153" t="inlineStr"/>
       <c r="H153" t="n">
-        <v>0</v>
+        <v>-0.39</v>
       </c>
     </row>
     <row r="154">
@@ -4438,11 +4438,11 @@
         <v>0</v>
       </c>
       <c r="F154" t="n">
-        <v>1761</v>
+        <v>1753</v>
       </c>
       <c r="G154" t="inlineStr"/>
       <c r="H154" t="n">
-        <v>0.63</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="155">
@@ -4464,11 +4464,11 @@
         <v>0</v>
       </c>
       <c r="F155" t="n">
-        <v>467.6</v>
+        <v>471.15</v>
       </c>
       <c r="G155" t="inlineStr"/>
       <c r="H155" t="n">
-        <v>-1.54</v>
+        <v>-0.79</v>
       </c>
     </row>
     <row r="156">
@@ -4490,11 +4490,11 @@
         <v>0</v>
       </c>
       <c r="F156" t="n">
-        <v>9.16</v>
+        <v>9.02</v>
       </c>
       <c r="G156" t="inlineStr"/>
       <c r="H156" t="n">
-        <v>-0.43</v>
+        <v>-1.96</v>
       </c>
     </row>
     <row r="157">
@@ -4516,11 +4516,11 @@
         <v>0</v>
       </c>
       <c r="F157" t="n">
-        <v>480</v>
+        <v>477.9</v>
       </c>
       <c r="G157" t="inlineStr"/>
       <c r="H157" t="n">
-        <v>-0.72</v>
+        <v>-1.16</v>
       </c>
     </row>
     <row r="158">
@@ -4542,11 +4542,11 @@
         <v>0</v>
       </c>
       <c r="F158" t="n">
-        <v>24.5</v>
+        <v>24.32</v>
       </c>
       <c r="G158" t="inlineStr"/>
       <c r="H158" t="n">
-        <v>-0.41</v>
+        <v>-1.14</v>
       </c>
     </row>
     <row r="159">
@@ -4568,11 +4568,11 @@
         <v>0</v>
       </c>
       <c r="F159" t="n">
-        <v>53.87</v>
+        <v>54.19</v>
       </c>
       <c r="G159" t="inlineStr"/>
       <c r="H159" t="n">
-        <v>-1.16</v>
+        <v>-0.57</v>
       </c>
     </row>
     <row r="160">
@@ -4594,11 +4594,11 @@
         <v>0</v>
       </c>
       <c r="F160" t="n">
-        <v>34.6</v>
+        <v>33.5</v>
       </c>
       <c r="G160" t="inlineStr"/>
       <c r="H160" t="n">
-        <v>0.58</v>
+        <v>-2.62</v>
       </c>
     </row>
     <row r="161">
@@ -4620,11 +4620,11 @@
         <v>0</v>
       </c>
       <c r="F161" t="n">
-        <v>11.85</v>
+        <v>11.8</v>
       </c>
       <c r="G161" t="inlineStr"/>
       <c r="H161" t="n">
-        <v>-1</v>
+        <v>-1.42</v>
       </c>
     </row>
     <row r="162">
@@ -4646,11 +4646,11 @@
         <v>0</v>
       </c>
       <c r="F162" t="n">
-        <v>20.71</v>
+        <v>20.7</v>
       </c>
       <c r="G162" t="inlineStr"/>
       <c r="H162" t="n">
-        <v>-2.54</v>
+        <v>-2.59</v>
       </c>
     </row>
     <row r="163">
@@ -4672,11 +4672,11 @@
         <v>0</v>
       </c>
       <c r="F163" t="n">
-        <v>322.2</v>
+        <v>319.8</v>
       </c>
       <c r="G163" t="inlineStr"/>
       <c r="H163" t="n">
-        <v>1.1</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="164">
@@ -4698,11 +4698,11 @@
         <v>0</v>
       </c>
       <c r="F164" t="n">
-        <v>479.75</v>
+        <v>480.95</v>
       </c>
       <c r="G164" t="inlineStr"/>
       <c r="H164" t="n">
-        <v>-1.69</v>
+        <v>-1.44</v>
       </c>
     </row>
     <row r="165">
@@ -4724,11 +4724,11 @@
         <v>0</v>
       </c>
       <c r="F165" t="n">
-        <v>333.65</v>
+        <v>342.4</v>
       </c>
       <c r="G165" t="inlineStr"/>
       <c r="H165" t="n">
-        <v>-0.39</v>
+        <v>2.22</v>
       </c>
     </row>
     <row r="166">
@@ -4750,11 +4750,11 @@
         <v>0</v>
       </c>
       <c r="F166" t="n">
-        <v>1205.8</v>
+        <v>1179.1</v>
       </c>
       <c r="G166" t="inlineStr"/>
       <c r="H166" t="n">
-        <v>-1.08</v>
+        <v>-3.27</v>
       </c>
     </row>
     <row r="167">
@@ -4776,11 +4776,11 @@
         <v>0</v>
       </c>
       <c r="F167" t="n">
-        <v>54.5</v>
+        <v>53.44</v>
       </c>
       <c r="G167" t="inlineStr"/>
       <c r="H167" t="n">
-        <v>-2.85</v>
+        <v>-4.74</v>
       </c>
     </row>
     <row r="168">
@@ -4828,11 +4828,11 @@
         <v>0</v>
       </c>
       <c r="F169" t="n">
-        <v>246.29</v>
+        <v>244.2</v>
       </c>
       <c r="G169" t="inlineStr"/>
       <c r="H169" t="n">
-        <v>-1.09</v>
+        <v>-1.93</v>
       </c>
     </row>
     <row r="170">
@@ -4854,11 +4854,11 @@
         <v>0</v>
       </c>
       <c r="F170" t="n">
-        <v>34.74</v>
+        <v>33.71</v>
       </c>
       <c r="G170" t="inlineStr"/>
       <c r="H170" t="n">
-        <v>-0.77</v>
+        <v>-3.71</v>
       </c>
     </row>
     <row r="171">
@@ -4880,11 +4880,11 @@
         <v>0</v>
       </c>
       <c r="F171" t="n">
-        <v>88.40000000000001</v>
+        <v>88.95</v>
       </c>
       <c r="G171" t="inlineStr"/>
       <c r="H171" t="n">
-        <v>-1.12</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="172">
@@ -4906,11 +4906,11 @@
         <v>0</v>
       </c>
       <c r="F172" t="n">
-        <v>6.58</v>
+        <v>6.63</v>
       </c>
       <c r="G172" t="inlineStr"/>
       <c r="H172" t="n">
-        <v>-2.81</v>
+        <v>-2.07</v>
       </c>
     </row>
     <row r="173">
@@ -4932,11 +4932,11 @@
         <v>0</v>
       </c>
       <c r="F173" t="n">
-        <v>17.71</v>
+        <v>17.49</v>
       </c>
       <c r="G173" t="inlineStr"/>
       <c r="H173" t="n">
-        <v>0.06</v>
+        <v>-1.19</v>
       </c>
     </row>
     <row r="174">
@@ -4958,11 +4958,11 @@
         <v>0</v>
       </c>
       <c r="F174" t="n">
-        <v>985.8</v>
+        <v>972</v>
       </c>
       <c r="G174" t="inlineStr"/>
       <c r="H174" t="n">
-        <v>-0.92</v>
+        <v>-2.31</v>
       </c>
     </row>
     <row r="175">
@@ -4984,11 +4984,11 @@
         <v>0</v>
       </c>
       <c r="F175" t="n">
-        <v>216.9</v>
+        <v>224</v>
       </c>
       <c r="G175" t="inlineStr"/>
       <c r="H175" t="n">
-        <v>-0.28</v>
+        <v>2.99</v>
       </c>
     </row>
     <row r="176">
@@ -5010,11 +5010,11 @@
         <v>0</v>
       </c>
       <c r="F176" t="n">
-        <v>29.65</v>
+        <v>29.64</v>
       </c>
       <c r="G176" t="inlineStr"/>
       <c r="H176" t="n">
-        <v>0.85</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="177">
@@ -5036,11 +5036,11 @@
         <v>0</v>
       </c>
       <c r="F177" t="n">
-        <v>48.98</v>
+        <v>48.8</v>
       </c>
       <c r="G177" t="inlineStr"/>
       <c r="H177" t="n">
-        <v>-1.41</v>
+        <v>-1.77</v>
       </c>
     </row>
     <row r="178">
@@ -5062,11 +5062,11 @@
         <v>0</v>
       </c>
       <c r="F178" t="n">
-        <v>186.05</v>
+        <v>192.1</v>
       </c>
       <c r="G178" t="inlineStr"/>
       <c r="H178" t="n">
-        <v>-1.48</v>
+        <v>1.72</v>
       </c>
     </row>
     <row r="179">
@@ -5088,11 +5088,11 @@
         <v>0</v>
       </c>
       <c r="F179" t="n">
-        <v>28.14</v>
+        <v>28.5</v>
       </c>
       <c r="G179" t="inlineStr"/>
       <c r="H179" t="n">
-        <v>-1.61</v>
+        <v>-0.35</v>
       </c>
     </row>
     <row r="180">
@@ -5114,11 +5114,11 @@
         <v>0</v>
       </c>
       <c r="F180" t="n">
-        <v>462</v>
+        <v>447.95</v>
       </c>
       <c r="G180" t="inlineStr"/>
       <c r="H180" t="n">
-        <v>0</v>
+        <v>-3.04</v>
       </c>
     </row>
     <row r="181">
@@ -5140,11 +5140,11 @@
         <v>0</v>
       </c>
       <c r="F181" t="n">
-        <v>183.1</v>
+        <v>179.5</v>
       </c>
       <c r="G181" t="inlineStr"/>
       <c r="H181" t="n">
-        <v>0.6</v>
+        <v>-1.37</v>
       </c>
     </row>
     <row r="182">
@@ -5166,11 +5166,11 @@
         <v>0</v>
       </c>
       <c r="F182" t="n">
-        <v>481.5</v>
+        <v>477</v>
       </c>
       <c r="G182" t="inlineStr"/>
       <c r="H182" t="n">
-        <v>-1.44</v>
+        <v>-2.36</v>
       </c>
     </row>
     <row r="183">
@@ -5192,11 +5192,11 @@
         <v>0</v>
       </c>
       <c r="F183" t="n">
-        <v>648</v>
+        <v>615</v>
       </c>
       <c r="G183" t="inlineStr"/>
       <c r="H183" t="n">
-        <v>0.29</v>
+        <v>-4.81</v>
       </c>
     </row>
     <row r="184">
@@ -5218,11 +5218,11 @@
         <v>0</v>
       </c>
       <c r="F184" t="n">
-        <v>186</v>
+        <v>180.97</v>
       </c>
       <c r="G184" t="inlineStr"/>
       <c r="H184" t="n">
-        <v>0.14</v>
+        <v>-2.57</v>
       </c>
     </row>
     <row r="185">
@@ -5244,11 +5244,11 @@
         <v>0</v>
       </c>
       <c r="F185" t="n">
-        <v>31.39</v>
+        <v>31.09</v>
       </c>
       <c r="G185" t="inlineStr"/>
       <c r="H185" t="n">
-        <v>-1.88</v>
+        <v>-2.81</v>
       </c>
     </row>
     <row r="186">
@@ -5270,11 +5270,11 @@
         <v>0</v>
       </c>
       <c r="F186" t="n">
-        <v>467.45</v>
+        <v>464.75</v>
       </c>
       <c r="G186" t="inlineStr"/>
       <c r="H186" t="n">
-        <v>-2.61</v>
+        <v>-3.18</v>
       </c>
     </row>
     <row r="187">
@@ -5296,11 +5296,11 @@
         <v>0</v>
       </c>
       <c r="F187" t="n">
-        <v>18.54</v>
+        <v>18.59</v>
       </c>
       <c r="G187" t="inlineStr"/>
       <c r="H187" t="n">
-        <v>-1.07</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="188">
@@ -5322,11 +5322,11 @@
         <v>0</v>
       </c>
       <c r="F188" t="n">
-        <v>42.91</v>
+        <v>42.75</v>
       </c>
       <c r="G188" t="inlineStr"/>
       <c r="H188" t="n">
-        <v>-0.9</v>
+        <v>-1.27</v>
       </c>
     </row>
     <row r="189">
@@ -5348,11 +5348,11 @@
         <v>0</v>
       </c>
       <c r="F189" t="n">
-        <v>751.2</v>
+        <v>774.9</v>
       </c>
       <c r="G189" t="inlineStr"/>
       <c r="H189" t="n">
-        <v>-4.31</v>
+        <v>-1.29</v>
       </c>
     </row>
     <row r="190">
@@ -5374,11 +5374,11 @@
         <v>0</v>
       </c>
       <c r="F190" t="n">
-        <v>29.5</v>
+        <v>30.64</v>
       </c>
       <c r="G190" t="inlineStr"/>
       <c r="H190" t="n">
-        <v>-0.61</v>
+        <v>3.23</v>
       </c>
     </row>
     <row r="191">
@@ -5400,11 +5400,11 @@
         <v>0</v>
       </c>
       <c r="F191" t="n">
-        <v>131.85</v>
+        <v>125.3</v>
       </c>
       <c r="G191" t="inlineStr"/>
       <c r="H191" t="n">
-        <v>-0.86</v>
+        <v>-5.79</v>
       </c>
     </row>
     <row r="192">
@@ -5478,11 +5478,11 @@
         <v>0</v>
       </c>
       <c r="F194" t="n">
-        <v>36.48</v>
+        <v>36</v>
       </c>
       <c r="G194" t="inlineStr"/>
       <c r="H194" t="n">
-        <v>-1.38</v>
+        <v>-2.68</v>
       </c>
     </row>
     <row r="195">
@@ -5504,11 +5504,11 @@
         <v>0</v>
       </c>
       <c r="F195" t="n">
-        <v>238.41</v>
+        <v>236.8</v>
       </c>
       <c r="G195" t="inlineStr"/>
       <c r="H195" t="n">
-        <v>-0.6</v>
+        <v>-1.27</v>
       </c>
     </row>
     <row r="196">
@@ -5530,11 +5530,11 @@
         <v>0</v>
       </c>
       <c r="F196" t="n">
-        <v>145.9</v>
+        <v>145</v>
       </c>
       <c r="G196" t="inlineStr"/>
       <c r="H196" t="n">
-        <v>0.76</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="197">
@@ -5556,11 +5556,11 @@
         <v>0</v>
       </c>
       <c r="F197" t="n">
-        <v>11.96</v>
+        <v>11.52</v>
       </c>
       <c r="G197" t="inlineStr"/>
       <c r="H197" t="n">
-        <v>-0.99</v>
+        <v>-4.64</v>
       </c>
     </row>
     <row r="198">
@@ -5582,11 +5582,11 @@
         <v>0</v>
       </c>
       <c r="F198" t="n">
-        <v>187.9</v>
+        <v>185</v>
       </c>
       <c r="G198" t="inlineStr"/>
       <c r="H198" t="n">
-        <v>-1.73</v>
+        <v>-3.24</v>
       </c>
     </row>
     <row r="199">
@@ -5608,11 +5608,11 @@
         <v>0</v>
       </c>
       <c r="F199" t="n">
-        <v>575.4</v>
+        <v>568</v>
       </c>
       <c r="G199" t="inlineStr"/>
       <c r="H199" t="n">
-        <v>0.42</v>
+        <v>-0.87</v>
       </c>
     </row>
     <row r="200">
@@ -5634,11 +5634,11 @@
         <v>0</v>
       </c>
       <c r="F200" t="n">
-        <v>2468.5</v>
+        <v>2441</v>
       </c>
       <c r="G200" t="inlineStr"/>
       <c r="H200" t="n">
-        <v>-2.39</v>
+        <v>-3.48</v>
       </c>
     </row>
     <row r="201">
@@ -5660,11 +5660,11 @@
         <v>0</v>
       </c>
       <c r="F201" t="n">
-        <v>264.25</v>
+        <v>252.55</v>
       </c>
       <c r="G201" t="inlineStr"/>
       <c r="H201" t="n">
-        <v>0.4</v>
+        <v>-4.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto: update momentum data - 2025-12-25 04:26 UTC
</commit_message>
<xml_diff>
--- a/data/trending_momentum_stocks.xlsx
+++ b/data/trending_momentum_stocks.xlsx
@@ -516,11 +516,11 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>72.59999999999999</v>
+        <v>74</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
-        <v>-3.2</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="4">
@@ -542,11 +542,11 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>96.31</v>
+        <v>96.13</v>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
-        <v>0.44</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="5">
@@ -594,11 +594,11 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>426.85</v>
+        <v>419.95</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
-        <v>-6.19</v>
+        <v>-7.7</v>
       </c>
     </row>
     <row r="7">
@@ -620,11 +620,11 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>113.4</v>
+        <v>113.75</v>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
-        <v>5</v>
+        <v>5.32</v>
       </c>
     </row>
     <row r="8">
@@ -646,11 +646,11 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>10.6</v>
+        <v>10.66</v>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
-        <v>-7.02</v>
+        <v>-6.49</v>
       </c>
     </row>
     <row r="9">
@@ -672,11 +672,11 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>142.01</v>
+        <v>152.28</v>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
-        <v>4.43</v>
+        <v>11.98</v>
       </c>
     </row>
     <row r="10">
@@ -724,11 +724,11 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>7.16</v>
+        <v>7.19</v>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="n">
-        <v>-3.89</v>
+        <v>-3.49</v>
       </c>
     </row>
     <row r="12">
@@ -750,11 +750,11 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>30.8</v>
+        <v>30.47</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="n">
-        <v>-4.91</v>
+        <v>-5.93</v>
       </c>
     </row>
     <row r="13">
@@ -776,11 +776,11 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>4.85</v>
+        <v>4.86</v>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
-        <v>-10.02</v>
+        <v>-9.83</v>
       </c>
     </row>
     <row r="14">
@@ -802,11 +802,11 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>14.47</v>
+        <v>13.96</v>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="n">
-        <v>-4.11</v>
+        <v>-7.49</v>
       </c>
     </row>
     <row r="15">
@@ -828,11 +828,11 @@
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>242.5</v>
+        <v>237.3</v>
       </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="n">
-        <v>-3</v>
+        <v>-5.08</v>
       </c>
     </row>
     <row r="16">
@@ -854,11 +854,11 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>24.8</v>
+        <v>24.79</v>
       </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="n">
-        <v>-4.25</v>
+        <v>-4.29</v>
       </c>
     </row>
     <row r="17">
@@ -880,11 +880,11 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>52.5</v>
+        <v>52.95</v>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="n">
-        <v>-3.67</v>
+        <v>-2.84</v>
       </c>
     </row>
     <row r="18">
@@ -1010,11 +1010,11 @@
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>78.90000000000001</v>
+        <v>79.76000000000001</v>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="n">
-        <v>-1.08</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1036,11 +1036,11 @@
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="n">
-        <v>-1.47</v>
+        <v>-3.43</v>
       </c>
     </row>
     <row r="24">
@@ -1062,11 +1062,11 @@
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="n">
-        <v>-1.73</v>
+        <v>-4.61</v>
       </c>
     </row>
     <row r="25">
@@ -1114,11 +1114,11 @@
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>11.8</v>
+        <v>12.05</v>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="n">
-        <v>-2.07</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1192,11 +1192,11 @@
         <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>17</v>
+        <v>17.06</v>
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="n">
-        <v>-1.96</v>
+        <v>-1.61</v>
       </c>
     </row>
     <row r="30">
@@ -1244,11 +1244,11 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>24.38</v>
+        <v>24.55</v>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="n">
-        <v>-1.57</v>
+        <v>-0.89</v>
       </c>
     </row>
     <row r="32">
@@ -1270,11 +1270,11 @@
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>87.3</v>
+        <v>87.40000000000001</v>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="n">
-        <v>-1.52</v>
+        <v>-1.41</v>
       </c>
     </row>
     <row r="33">
@@ -1296,11 +1296,11 @@
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>29.38</v>
+        <v>29.83</v>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="n">
-        <v>-5.2</v>
+        <v>-3.74</v>
       </c>
     </row>
     <row r="34">
@@ -1322,11 +1322,11 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>102.77</v>
+        <v>101.11</v>
       </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="n">
-        <v>-3.91</v>
+        <v>-5.46</v>
       </c>
     </row>
     <row r="35">
@@ -1348,11 +1348,11 @@
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>9.16</v>
+        <v>9.029999999999999</v>
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="n">
-        <v>-5.47</v>
+        <v>-6.81</v>
       </c>
     </row>
     <row r="36">
@@ -1426,11 +1426,11 @@
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>18.44</v>
+        <v>16.8</v>
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="n">
-        <v>9.24</v>
+        <v>-0.47</v>
       </c>
     </row>
     <row r="39">
@@ -1452,11 +1452,11 @@
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>78.25</v>
+        <v>79</v>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="n">
-        <v>-0.57</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="40">
@@ -1478,11 +1478,11 @@
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>25.37</v>
+        <v>25.2</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="n">
-        <v>-0.43</v>
+        <v>-1.1</v>
       </c>
     </row>
     <row r="41">
@@ -1504,11 +1504,11 @@
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>49.5</v>
+        <v>48.95</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="n">
-        <v>-3.88</v>
+        <v>-4.95</v>
       </c>
     </row>
     <row r="42">
@@ -1530,11 +1530,11 @@
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>0.47</v>
+        <v>0.49</v>
       </c>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="n">
-        <v>-4.08</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1556,11 +1556,11 @@
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>9.539999999999999</v>
+        <v>9.5</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="n">
-        <v>-2.65</v>
+        <v>-3.06</v>
       </c>
     </row>
     <row r="44">
@@ -1582,11 +1582,11 @@
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>192.4</v>
+        <v>196.4</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="n">
-        <v>-1.33</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="45">
@@ -1660,11 +1660,11 @@
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>15.3</v>
+        <v>15.2</v>
       </c>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="n">
-        <v>-2.86</v>
+        <v>-3.49</v>
       </c>
     </row>
     <row r="48">
@@ -1686,11 +1686,11 @@
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>0.8</v>
+        <v>0.83</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="n">
-        <v>6.67</v>
+        <v>10.67</v>
       </c>
     </row>
     <row r="49">
@@ -1738,11 +1738,11 @@
         <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>12.26</v>
+        <v>12.29</v>
       </c>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="n">
-        <v>-3.99</v>
+        <v>-3.76</v>
       </c>
     </row>
     <row r="51">
@@ -1764,11 +1764,11 @@
         <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>112.91</v>
+        <v>112.9</v>
       </c>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="n">
-        <v>-2.24</v>
+        <v>-2.25</v>
       </c>
     </row>
     <row r="52">
@@ -1790,11 +1790,11 @@
         <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>0.5</v>
+        <v>0.51</v>
       </c>
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="n">
-        <v>-3.85</v>
+        <v>-1.92</v>
       </c>
     </row>
     <row r="53">
@@ -1842,11 +1842,11 @@
         <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>54.66</v>
+        <v>55.2</v>
       </c>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="n">
-        <v>-2.39</v>
+        <v>-1.43</v>
       </c>
     </row>
     <row r="55">
@@ -1868,11 +1868,11 @@
         <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="n">
-        <v>-3.21</v>
+        <v>-4.43</v>
       </c>
     </row>
     <row r="56">
@@ -1920,11 +1920,11 @@
         <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>6.3</v>
+        <v>5.93</v>
       </c>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="n">
-        <v>5.88</v>
+        <v>-0.34</v>
       </c>
     </row>
     <row r="58">
@@ -1946,11 +1946,11 @@
         <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>32.42</v>
+        <v>31.1</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="n">
-        <v>-0.09</v>
+        <v>-4.16</v>
       </c>
     </row>
     <row r="59">
@@ -1998,11 +1998,11 @@
         <v>0</v>
       </c>
       <c r="F60" t="n">
-        <v>8.109999999999999</v>
+        <v>8</v>
       </c>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="n">
-        <v>-5.04</v>
+        <v>-6.32</v>
       </c>
     </row>
     <row r="61">
@@ -2024,11 +2024,11 @@
         <v>0</v>
       </c>
       <c r="F61" t="n">
-        <v>71.93000000000001</v>
+        <v>69.86</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="n">
-        <v>-1.83</v>
+        <v>-4.65</v>
       </c>
     </row>
     <row r="62">
@@ -2072,11 +2072,11 @@
         <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>9.44</v>
+        <v>9.26</v>
       </c>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="n">
-        <v>-0.53</v>
+        <v>-2.42</v>
       </c>
     </row>
     <row r="64">
@@ -2098,11 +2098,11 @@
         <v>0</v>
       </c>
       <c r="F64" t="n">
-        <v>3.69</v>
+        <v>3.61</v>
       </c>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="n">
-        <v>-2.64</v>
+        <v>-4.75</v>
       </c>
     </row>
     <row r="65">
@@ -2124,11 +2124,11 @@
         <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>109.98</v>
+        <v>113.9</v>
       </c>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="n">
-        <v>-3.51</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="66">
@@ -2150,11 +2150,11 @@
         <v>0</v>
       </c>
       <c r="F66" t="n">
-        <v>14</v>
+        <v>14.28</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="n">
-        <v>-5.08</v>
+        <v>-3.19</v>
       </c>
     </row>
     <row r="67">
@@ -2176,11 +2176,11 @@
         <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="n">
-        <v>-1.81</v>
+        <v>-3.42</v>
       </c>
     </row>
     <row r="68">
@@ -2202,11 +2202,11 @@
         <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>8.67</v>
+        <v>8.74</v>
       </c>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="n">
-        <v>-3.13</v>
+        <v>-2.35</v>
       </c>
     </row>
     <row r="69">
@@ -2228,11 +2228,11 @@
         <v>0</v>
       </c>
       <c r="F69" t="n">
-        <v>219</v>
+        <v>213.34</v>
       </c>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="n">
-        <v>0</v>
+        <v>-2.58</v>
       </c>
     </row>
     <row r="70">
@@ -2254,11 +2254,11 @@
         <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>87.09999999999999</v>
+        <v>86.98999999999999</v>
       </c>
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="n">
-        <v>-3.11</v>
+        <v>-3.24</v>
       </c>
     </row>
     <row r="71">
@@ -2280,11 +2280,11 @@
         <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>1.83</v>
+        <v>1.86</v>
       </c>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="n">
-        <v>-1.61</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -2306,11 +2306,11 @@
         <v>0</v>
       </c>
       <c r="F72" t="n">
-        <v>76.06</v>
+        <v>75.69</v>
       </c>
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="n">
-        <v>-3.45</v>
+        <v>-3.92</v>
       </c>
     </row>
     <row r="73">
@@ -2332,11 +2332,11 @@
         <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>43.74</v>
+        <v>42.6</v>
       </c>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="n">
-        <v>-0.59</v>
+        <v>-3.18</v>
       </c>
     </row>
     <row r="74">
@@ -2358,11 +2358,11 @@
         <v>0</v>
       </c>
       <c r="F74" t="n">
-        <v>0.68</v>
+        <v>0.67</v>
       </c>
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="n">
-        <v>-1.45</v>
+        <v>-2.9</v>
       </c>
     </row>
     <row r="75">
@@ -2384,11 +2384,11 @@
         <v>0</v>
       </c>
       <c r="F75" t="n">
-        <v>2781.2</v>
+        <v>2719.9</v>
       </c>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="n">
-        <v>1.24</v>
+        <v>-0.99</v>
       </c>
     </row>
     <row r="76">
@@ -2410,11 +2410,11 @@
         <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>18.7</v>
+        <v>18.12</v>
       </c>
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="n">
-        <v>-1.06</v>
+        <v>-4.13</v>
       </c>
     </row>
     <row r="77">
@@ -2436,11 +2436,11 @@
         <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>13.93</v>
+        <v>14.08</v>
       </c>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="n">
-        <v>0.9399999999999999</v>
+        <v>2.03</v>
       </c>
     </row>
     <row r="78">
@@ -2462,11 +2462,11 @@
         <v>0</v>
       </c>
       <c r="F78" t="n">
-        <v>208.15</v>
+        <v>208.16</v>
       </c>
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="n">
-        <v>2.03</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="79">
@@ -2488,11 +2488,11 @@
         <v>0</v>
       </c>
       <c r="F79" t="n">
-        <v>61.65</v>
+        <v>62.7</v>
       </c>
       <c r="G79" t="inlineStr"/>
       <c r="H79" t="n">
-        <v>-0.5</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="80">
@@ -2514,11 +2514,11 @@
         <v>0</v>
       </c>
       <c r="F80" t="n">
-        <v>6.33</v>
+        <v>6.25</v>
       </c>
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="n">
-        <v>-1.56</v>
+        <v>-2.8</v>
       </c>
     </row>
     <row r="81">
@@ -2540,11 +2540,11 @@
         <v>0</v>
       </c>
       <c r="F81" t="n">
-        <v>161</v>
+        <v>163.08</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="n">
-        <v>-2.36</v>
+        <v>-1.1</v>
       </c>
     </row>
     <row r="82">
@@ -2566,11 +2566,11 @@
         <v>0</v>
       </c>
       <c r="F82" t="n">
-        <v>81.05</v>
+        <v>77.5</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="n">
-        <v>-1.04</v>
+        <v>-5.37</v>
       </c>
     </row>
     <row r="83">
@@ -2592,11 +2592,11 @@
         <v>0</v>
       </c>
       <c r="F83" t="n">
-        <v>2.47</v>
+        <v>2.45</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="n">
-        <v>-3.52</v>
+        <v>-4.3</v>
       </c>
     </row>
     <row r="84">
@@ -2618,11 +2618,11 @@
         <v>0</v>
       </c>
       <c r="F84" t="n">
-        <v>52.54</v>
+        <v>52</v>
       </c>
       <c r="G84" t="inlineStr"/>
       <c r="H84" t="n">
-        <v>-2.56</v>
+        <v>-3.56</v>
       </c>
     </row>
     <row r="85">
@@ -2644,11 +2644,11 @@
         <v>0</v>
       </c>
       <c r="F85" t="n">
-        <v>25.89</v>
+        <v>25.29</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="n">
-        <v>-0.42</v>
+        <v>-2.73</v>
       </c>
     </row>
     <row r="86">
@@ -2670,11 +2670,11 @@
         <v>0</v>
       </c>
       <c r="F86" t="n">
-        <v>846</v>
+        <v>818.5</v>
       </c>
       <c r="G86" t="inlineStr"/>
       <c r="H86" t="n">
-        <v>-2.31</v>
+        <v>-5.48</v>
       </c>
     </row>
     <row r="87">
@@ -2696,11 +2696,11 @@
         <v>0</v>
       </c>
       <c r="F87" t="n">
-        <v>1.48</v>
+        <v>1.53</v>
       </c>
       <c r="G87" t="inlineStr"/>
       <c r="H87" t="n">
-        <v>-1.33</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88">
@@ -2722,11 +2722,11 @@
         <v>0</v>
       </c>
       <c r="F88" t="n">
-        <v>19.21</v>
+        <v>19.05</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="n">
-        <v>-2.44</v>
+        <v>-3.25</v>
       </c>
     </row>
     <row r="89">
@@ -2748,11 +2748,11 @@
         <v>0</v>
       </c>
       <c r="F89" t="n">
-        <v>105.5</v>
+        <v>106.35</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="n">
-        <v>-4.09</v>
+        <v>-3.32</v>
       </c>
     </row>
     <row r="90">
@@ -2774,11 +2774,11 @@
         <v>0</v>
       </c>
       <c r="F90" t="n">
-        <v>830</v>
+        <v>804</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="n">
-        <v>-0.92</v>
+        <v>-4.02</v>
       </c>
     </row>
     <row r="91">
@@ -2800,11 +2800,11 @@
         <v>0</v>
       </c>
       <c r="F91" t="n">
-        <v>78.72</v>
+        <v>78.3</v>
       </c>
       <c r="G91" t="inlineStr"/>
       <c r="H91" t="n">
-        <v>-2.8</v>
+        <v>-3.32</v>
       </c>
     </row>
     <row r="92">
@@ -2826,11 +2826,11 @@
         <v>0</v>
       </c>
       <c r="F92" t="n">
-        <v>60.8</v>
+        <v>60.89</v>
       </c>
       <c r="G92" t="inlineStr"/>
       <c r="H92" t="n">
-        <v>-1.62</v>
+        <v>-1.47</v>
       </c>
     </row>
     <row r="93">
@@ -2878,11 +2878,11 @@
         <v>0</v>
       </c>
       <c r="F94" t="n">
-        <v>9.289999999999999</v>
+        <v>9.17</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="n">
-        <v>-2</v>
+        <v>-3.27</v>
       </c>
     </row>
     <row r="95">
@@ -2904,11 +2904,11 @@
         <v>0</v>
       </c>
       <c r="F95" t="n">
-        <v>168.2</v>
+        <v>167.9</v>
       </c>
       <c r="G95" t="inlineStr"/>
       <c r="H95" t="n">
-        <v>-3.32</v>
+        <v>-3.49</v>
       </c>
     </row>
     <row r="96">
@@ -2930,11 +2930,11 @@
         <v>0</v>
       </c>
       <c r="F96" t="n">
-        <v>279.65</v>
+        <v>273</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="n">
-        <v>-2.54</v>
+        <v>-4.86</v>
       </c>
     </row>
     <row r="97">
@@ -2956,11 +2956,11 @@
         <v>0</v>
       </c>
       <c r="F97" t="n">
-        <v>38.37</v>
+        <v>38.15</v>
       </c>
       <c r="G97" t="inlineStr"/>
       <c r="H97" t="n">
-        <v>-2.42</v>
+        <v>-2.98</v>
       </c>
     </row>
     <row r="98">
@@ -3008,11 +3008,11 @@
         <v>0</v>
       </c>
       <c r="F99" t="n">
-        <v>170.95</v>
+        <v>166.05</v>
       </c>
       <c r="G99" t="inlineStr"/>
       <c r="H99" t="n">
-        <v>7.54</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="100">
@@ -3034,11 +3034,11 @@
         <v>0</v>
       </c>
       <c r="F100" t="n">
-        <v>33.74</v>
+        <v>33.75</v>
       </c>
       <c r="G100" t="inlineStr"/>
       <c r="H100" t="n">
-        <v>-2.03</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="101">
@@ -3060,11 +3060,11 @@
         <v>0</v>
       </c>
       <c r="F101" t="n">
-        <v>244.31</v>
+        <v>234.7</v>
       </c>
       <c r="G101" t="inlineStr"/>
       <c r="H101" t="n">
-        <v>1.8</v>
+        <v>-2.21</v>
       </c>
     </row>
     <row r="102">
@@ -3112,11 +3112,11 @@
         <v>0</v>
       </c>
       <c r="F103" t="n">
-        <v>12.51</v>
+        <v>12.58</v>
       </c>
       <c r="G103" t="inlineStr"/>
       <c r="H103" t="n">
-        <v>-1.11</v>
+        <v>-0.55</v>
       </c>
     </row>
     <row r="104">
@@ -3138,11 +3138,11 @@
         <v>0</v>
       </c>
       <c r="F104" t="n">
-        <v>109.95</v>
+        <v>108.85</v>
       </c>
       <c r="G104" t="inlineStr"/>
       <c r="H104" t="n">
-        <v>3.05</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="105">
@@ -3164,11 +3164,11 @@
         <v>0</v>
       </c>
       <c r="F105" t="n">
-        <v>424.3</v>
+        <v>434.95</v>
       </c>
       <c r="G105" t="inlineStr"/>
       <c r="H105" t="n">
-        <v>1.51</v>
+        <v>4.06</v>
       </c>
     </row>
     <row r="106">
@@ -3190,11 +3190,11 @@
         <v>0</v>
       </c>
       <c r="F106" t="n">
-        <v>78.02</v>
+        <v>78.48999999999999</v>
       </c>
       <c r="G106" t="inlineStr"/>
       <c r="H106" t="n">
-        <v>-1.38</v>
+        <v>-0.78</v>
       </c>
     </row>
     <row r="107">
@@ -3216,11 +3216,11 @@
         <v>0</v>
       </c>
       <c r="F107" t="n">
-        <v>7.88</v>
+        <v>7.81</v>
       </c>
       <c r="G107" t="inlineStr"/>
       <c r="H107" t="n">
-        <v>-4.72</v>
+        <v>-5.56</v>
       </c>
     </row>
     <row r="108">
@@ -3242,11 +3242,11 @@
         <v>0</v>
       </c>
       <c r="F108" t="n">
-        <v>8</v>
+        <v>8.06</v>
       </c>
       <c r="G108" t="inlineStr"/>
       <c r="H108" t="n">
-        <v>-3.26</v>
+        <v>-2.54</v>
       </c>
     </row>
     <row r="109">
@@ -3268,11 +3268,11 @@
         <v>0</v>
       </c>
       <c r="F109" t="n">
-        <v>68.88</v>
+        <v>66.98</v>
       </c>
       <c r="G109" t="inlineStr"/>
       <c r="H109" t="n">
-        <v>-0.14</v>
+        <v>-2.9</v>
       </c>
     </row>
     <row r="110">
@@ -3294,10 +3294,12 @@
         <v>0</v>
       </c>
       <c r="F110" t="n">
-        <v>0</v>
+        <v>84.51000000000001</v>
       </c>
       <c r="G110" t="inlineStr"/>
-      <c r="H110" t="inlineStr"/>
+      <c r="H110" t="n">
+        <v>2.56</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -3318,11 +3320,11 @@
         <v>0</v>
       </c>
       <c r="F111" t="n">
-        <v>105.99</v>
+        <v>105.3</v>
       </c>
       <c r="G111" t="inlineStr"/>
       <c r="H111" t="n">
-        <v>-1.4</v>
+        <v>-2.05</v>
       </c>
     </row>
     <row r="112">
@@ -3344,11 +3346,11 @@
         <v>0</v>
       </c>
       <c r="F112" t="n">
-        <v>55</v>
+        <v>56.77</v>
       </c>
       <c r="G112" t="inlineStr"/>
       <c r="H112" t="n">
-        <v>-0.72</v>
+        <v>2.47</v>
       </c>
     </row>
     <row r="113">
@@ -3370,11 +3372,11 @@
         <v>0</v>
       </c>
       <c r="F113" t="n">
-        <v>913</v>
+        <v>929</v>
       </c>
       <c r="G113" t="inlineStr"/>
       <c r="H113" t="n">
-        <v>-1.93</v>
+        <v>-0.21</v>
       </c>
     </row>
     <row r="114">
@@ -3396,11 +3398,11 @@
         <v>0</v>
       </c>
       <c r="F114" t="n">
-        <v>189.5</v>
+        <v>193.5</v>
       </c>
       <c r="G114" t="inlineStr"/>
       <c r="H114" t="n">
-        <v>-2.8</v>
+        <v>-0.74</v>
       </c>
     </row>
     <row r="115">
@@ -3422,11 +3424,11 @@
         <v>0</v>
       </c>
       <c r="F115" t="n">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="G115" t="inlineStr"/>
       <c r="H115" t="n">
-        <v>-0.34</v>
+        <v>3.09</v>
       </c>
     </row>
     <row r="116">
@@ -3448,11 +3450,11 @@
         <v>0</v>
       </c>
       <c r="F116" t="n">
-        <v>39.12</v>
+        <v>39</v>
       </c>
       <c r="G116" t="inlineStr"/>
       <c r="H116" t="n">
-        <v>-2.05</v>
+        <v>-2.35</v>
       </c>
     </row>
     <row r="117">
@@ -3474,11 +3476,11 @@
         <v>0</v>
       </c>
       <c r="F117" t="n">
-        <v>6.48</v>
+        <v>6.37</v>
       </c>
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="n">
-        <v>-0.46</v>
+        <v>-2.15</v>
       </c>
     </row>
     <row r="118">
@@ -3500,11 +3502,11 @@
         <v>0</v>
       </c>
       <c r="F118" t="n">
-        <v>1720</v>
+        <v>1740</v>
       </c>
       <c r="G118" t="inlineStr"/>
       <c r="H118" t="n">
-        <v>-1.71</v>
+        <v>-0.57</v>
       </c>
     </row>
     <row r="119">
@@ -3526,11 +3528,11 @@
         <v>0</v>
       </c>
       <c r="F119" t="n">
-        <v>1583.5</v>
+        <v>1591</v>
       </c>
       <c r="G119" t="inlineStr"/>
       <c r="H119" t="n">
-        <v>-1.95</v>
+        <v>-1.49</v>
       </c>
     </row>
     <row r="120">
@@ -3552,11 +3554,11 @@
         <v>0</v>
       </c>
       <c r="F120" t="n">
-        <v>48.3</v>
+        <v>48.56</v>
       </c>
       <c r="G120" t="inlineStr"/>
       <c r="H120" t="n">
-        <v>-1.83</v>
+        <v>-1.3</v>
       </c>
     </row>
     <row r="121">
@@ -3578,11 +3580,11 @@
         <v>0</v>
       </c>
       <c r="F121" t="n">
-        <v>74.09999999999999</v>
+        <v>74.47</v>
       </c>
       <c r="G121" t="inlineStr"/>
       <c r="H121" t="n">
-        <v>-2.23</v>
+        <v>-1.74</v>
       </c>
     </row>
     <row r="122">
@@ -3604,11 +3606,11 @@
         <v>0</v>
       </c>
       <c r="F122" t="n">
-        <v>16.46</v>
+        <v>16.5</v>
       </c>
       <c r="G122" t="inlineStr"/>
       <c r="H122" t="n">
-        <v>-2.26</v>
+        <v>-2.02</v>
       </c>
     </row>
     <row r="123">
@@ -3630,11 +3632,11 @@
         <v>0</v>
       </c>
       <c r="F123" t="n">
-        <v>6.92</v>
+        <v>6.81</v>
       </c>
       <c r="G123" t="inlineStr"/>
       <c r="H123" t="n">
-        <v>-0.86</v>
+        <v>-2.44</v>
       </c>
     </row>
     <row r="124">
@@ -3656,11 +3658,11 @@
         <v>0</v>
       </c>
       <c r="F124" t="n">
-        <v>1298.5</v>
+        <v>1276.7</v>
       </c>
       <c r="G124" t="inlineStr"/>
       <c r="H124" t="n">
-        <v>-1.7</v>
+        <v>-3.35</v>
       </c>
     </row>
     <row r="125">
@@ -3682,11 +3684,11 @@
         <v>0</v>
       </c>
       <c r="F125" t="n">
-        <v>19.35</v>
+        <v>18.8</v>
       </c>
       <c r="G125" t="inlineStr"/>
       <c r="H125" t="n">
-        <v>-0.77</v>
+        <v>-3.59</v>
       </c>
     </row>
     <row r="126">
@@ -3708,11 +3710,11 @@
         <v>0</v>
       </c>
       <c r="F126" t="n">
-        <v>62.2</v>
+        <v>61.99</v>
       </c>
       <c r="G126" t="inlineStr"/>
       <c r="H126" t="n">
-        <v>-1.14</v>
+        <v>-1.48</v>
       </c>
     </row>
     <row r="127">
@@ -3734,11 +3736,11 @@
         <v>0</v>
       </c>
       <c r="F127" t="n">
-        <v>2.98</v>
+        <v>3</v>
       </c>
       <c r="G127" t="inlineStr"/>
       <c r="H127" t="n">
-        <v>-1.65</v>
+        <v>-0.99</v>
       </c>
     </row>
     <row r="128">
@@ -3760,11 +3762,11 @@
         <v>0</v>
       </c>
       <c r="F128" t="n">
-        <v>9.4</v>
+        <v>9.35</v>
       </c>
       <c r="G128" t="inlineStr"/>
       <c r="H128" t="n">
-        <v>-2.39</v>
+        <v>-2.91</v>
       </c>
     </row>
     <row r="129">
@@ -3786,11 +3788,11 @@
         <v>0</v>
       </c>
       <c r="F129" t="n">
-        <v>29.59</v>
+        <v>29.5</v>
       </c>
       <c r="G129" t="inlineStr"/>
       <c r="H129" t="n">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
     </row>
     <row r="130">
@@ -3812,11 +3814,11 @@
         <v>0</v>
       </c>
       <c r="F130" t="n">
-        <v>6.64</v>
+        <v>6.58</v>
       </c>
       <c r="G130" t="inlineStr"/>
       <c r="H130" t="n">
-        <v>0</v>
+        <v>-0.9</v>
       </c>
     </row>
     <row r="131">
@@ -3838,7 +3840,7 @@
         <v>0</v>
       </c>
       <c r="F131" t="n">
-        <v>130.39</v>
+        <v>130.4</v>
       </c>
       <c r="G131" t="inlineStr"/>
       <c r="H131" t="n">
@@ -3864,11 +3866,11 @@
         <v>0</v>
       </c>
       <c r="F132" t="n">
-        <v>16.36</v>
+        <v>16.3</v>
       </c>
       <c r="G132" t="inlineStr"/>
       <c r="H132" t="n">
-        <v>2.89</v>
+        <v>2.52</v>
       </c>
     </row>
     <row r="133">
@@ -3890,11 +3892,11 @@
         <v>0</v>
       </c>
       <c r="F133" t="n">
-        <v>8.119999999999999</v>
+        <v>7.75</v>
       </c>
       <c r="G133" t="inlineStr"/>
       <c r="H133" t="n">
-        <v>-0.98</v>
+        <v>-5.49</v>
       </c>
     </row>
     <row r="134">
@@ -3916,11 +3918,11 @@
         <v>0</v>
       </c>
       <c r="F134" t="n">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G134" t="inlineStr"/>
       <c r="H134" t="n">
-        <v>0.65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135">
@@ -3942,11 +3944,11 @@
         <v>0</v>
       </c>
       <c r="F135" t="n">
-        <v>37.69</v>
+        <v>37.5</v>
       </c>
       <c r="G135" t="inlineStr"/>
       <c r="H135" t="n">
-        <v>-0.26</v>
+        <v>-0.77</v>
       </c>
     </row>
     <row r="136">
@@ -3994,11 +3996,11 @@
         <v>0</v>
       </c>
       <c r="F137" t="n">
-        <v>5.64</v>
+        <v>5.63</v>
       </c>
       <c r="G137" t="inlineStr"/>
       <c r="H137" t="n">
-        <v>-2.59</v>
+        <v>-2.76</v>
       </c>
     </row>
     <row r="138">
@@ -4020,11 +4022,11 @@
         <v>0</v>
       </c>
       <c r="F138" t="n">
-        <v>105.84</v>
+        <v>103.2</v>
       </c>
       <c r="G138" t="inlineStr"/>
       <c r="H138" t="n">
-        <v>-2</v>
+        <v>-4.44</v>
       </c>
     </row>
     <row r="139">
@@ -4046,11 +4048,11 @@
         <v>0</v>
       </c>
       <c r="F139" t="n">
-        <v>731.4</v>
+        <v>703.5</v>
       </c>
       <c r="G139" t="inlineStr"/>
       <c r="H139" t="n">
-        <v>-1</v>
+        <v>-4.78</v>
       </c>
     </row>
     <row r="140">
@@ -4072,11 +4074,11 @@
         <v>0</v>
       </c>
       <c r="F140" t="n">
-        <v>57.88</v>
+        <v>60.2</v>
       </c>
       <c r="G140" t="inlineStr"/>
       <c r="H140" t="n">
-        <v>-0.21</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="141">
@@ -4098,11 +4100,11 @@
         <v>0</v>
       </c>
       <c r="F141" t="n">
-        <v>41.66</v>
+        <v>40.7</v>
       </c>
       <c r="G141" t="inlineStr"/>
       <c r="H141" t="n">
-        <v>-1.28</v>
+        <v>-3.55</v>
       </c>
     </row>
     <row r="142">
@@ -4124,11 +4126,11 @@
         <v>0</v>
       </c>
       <c r="F142" t="n">
-        <v>10.08</v>
+        <v>9.75</v>
       </c>
       <c r="G142" t="inlineStr"/>
       <c r="H142" t="n">
-        <v>-1.18</v>
+        <v>-4.41</v>
       </c>
     </row>
     <row r="143">
@@ -4150,11 +4152,11 @@
         <v>0</v>
       </c>
       <c r="F143" t="n">
-        <v>50.85</v>
+        <v>53.97</v>
       </c>
       <c r="G143" t="inlineStr"/>
       <c r="H143" t="n">
-        <v>1.7</v>
+        <v>7.94</v>
       </c>
     </row>
     <row r="144">
@@ -4176,11 +4178,11 @@
         <v>0</v>
       </c>
       <c r="F144" t="n">
-        <v>72.39</v>
+        <v>70</v>
       </c>
       <c r="G144" t="inlineStr"/>
       <c r="H144" t="n">
-        <v>-0.84</v>
+        <v>-4.11</v>
       </c>
     </row>
     <row r="145">
@@ -4202,11 +4204,11 @@
         <v>0</v>
       </c>
       <c r="F145" t="n">
-        <v>4.87</v>
+        <v>4.86</v>
       </c>
       <c r="G145" t="inlineStr"/>
       <c r="H145" t="n">
-        <v>-1.22</v>
+        <v>-1.42</v>
       </c>
     </row>
     <row r="146">
@@ -4228,11 +4230,11 @@
         <v>0</v>
       </c>
       <c r="F146" t="n">
-        <v>4.26</v>
+        <v>4.3</v>
       </c>
       <c r="G146" t="inlineStr"/>
       <c r="H146" t="n">
-        <v>-2.96</v>
+        <v>-2.05</v>
       </c>
     </row>
     <row r="147">
@@ -4254,11 +4256,11 @@
         <v>0</v>
       </c>
       <c r="F147" t="n">
-        <v>119.56</v>
+        <v>119</v>
       </c>
       <c r="G147" t="inlineStr"/>
       <c r="H147" t="n">
-        <v>-1.84</v>
+        <v>-2.3</v>
       </c>
     </row>
     <row r="148">
@@ -4280,11 +4282,11 @@
         <v>0</v>
       </c>
       <c r="F148" t="n">
-        <v>75.98999999999999</v>
+        <v>73.90000000000001</v>
       </c>
       <c r="G148" t="inlineStr"/>
       <c r="H148" t="n">
-        <v>-1.95</v>
+        <v>-4.65</v>
       </c>
     </row>
     <row r="149">
@@ -4306,11 +4308,11 @@
         <v>0</v>
       </c>
       <c r="F149" t="n">
-        <v>167.89</v>
+        <v>161</v>
       </c>
       <c r="G149" t="inlineStr"/>
       <c r="H149" t="n">
-        <v>-0.07000000000000001</v>
+        <v>-4.17</v>
       </c>
     </row>
     <row r="150">
@@ -4332,11 +4334,11 @@
         <v>0</v>
       </c>
       <c r="F150" t="n">
-        <v>173.26</v>
+        <v>172.4</v>
       </c>
       <c r="G150" t="inlineStr"/>
       <c r="H150" t="n">
-        <v>3.13</v>
+        <v>2.62</v>
       </c>
     </row>
     <row r="151">
@@ -4358,11 +4360,11 @@
         <v>0</v>
       </c>
       <c r="F151" t="n">
-        <v>486.1</v>
+        <v>496.95</v>
       </c>
       <c r="G151" t="inlineStr"/>
       <c r="H151" t="n">
-        <v>0.54</v>
+        <v>2.78</v>
       </c>
     </row>
     <row r="152">
@@ -4384,11 +4386,11 @@
         <v>0</v>
       </c>
       <c r="F152" t="n">
-        <v>649.55</v>
+        <v>649</v>
       </c>
       <c r="G152" t="inlineStr"/>
       <c r="H152" t="n">
-        <v>0.71</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="153">
@@ -4410,11 +4412,11 @@
         <v>0</v>
       </c>
       <c r="F153" t="n">
-        <v>23.61</v>
+        <v>24</v>
       </c>
       <c r="G153" t="inlineStr"/>
       <c r="H153" t="n">
-        <v>-0.38</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="154">
@@ -4436,11 +4438,11 @@
         <v>0</v>
       </c>
       <c r="F154" t="n">
-        <v>68.15000000000001</v>
+        <v>67</v>
       </c>
       <c r="G154" t="inlineStr"/>
       <c r="H154" t="n">
-        <v>-0.29</v>
+        <v>-1.98</v>
       </c>
     </row>
     <row r="155">
@@ -4462,11 +4464,11 @@
         <v>0</v>
       </c>
       <c r="F155" t="n">
-        <v>342.65</v>
+        <v>346.55</v>
       </c>
       <c r="G155" t="inlineStr"/>
       <c r="H155" t="n">
-        <v>-2.09</v>
+        <v>-0.97</v>
       </c>
     </row>
     <row r="156">
@@ -4488,11 +4490,11 @@
         <v>0</v>
       </c>
       <c r="F156" t="n">
-        <v>442.9</v>
+        <v>419.5</v>
       </c>
       <c r="G156" t="inlineStr"/>
       <c r="H156" t="n">
-        <v>-1.02</v>
+        <v>-6.25</v>
       </c>
     </row>
     <row r="157">
@@ -4514,11 +4516,11 @@
         <v>0</v>
       </c>
       <c r="F157" t="n">
-        <v>1.71</v>
+        <v>1.7</v>
       </c>
       <c r="G157" t="inlineStr"/>
       <c r="H157" t="n">
-        <v>-0.58</v>
+        <v>-1.16</v>
       </c>
     </row>
     <row r="158">
@@ -4540,11 +4542,11 @@
         <v>0</v>
       </c>
       <c r="F158" t="n">
-        <v>795.5</v>
+        <v>750</v>
       </c>
       <c r="G158" t="inlineStr"/>
       <c r="H158" t="n">
-        <v>0.44</v>
+        <v>-5.3</v>
       </c>
     </row>
     <row r="159">
@@ -4566,11 +4568,11 @@
         <v>0</v>
       </c>
       <c r="F159" t="n">
-        <v>116</v>
+        <v>115.75</v>
       </c>
       <c r="G159" t="inlineStr"/>
       <c r="H159" t="n">
-        <v>-2.52</v>
+        <v>-2.73</v>
       </c>
     </row>
     <row r="160">
@@ -4592,11 +4594,11 @@
         <v>0</v>
       </c>
       <c r="F160" t="n">
-        <v>173.5</v>
+        <v>175.55</v>
       </c>
       <c r="G160" t="inlineStr"/>
       <c r="H160" t="n">
-        <v>-3.05</v>
+        <v>-1.9</v>
       </c>
     </row>
     <row r="161">
@@ -4618,11 +4620,11 @@
         <v>0</v>
       </c>
       <c r="F161" t="n">
-        <v>58.5</v>
+        <v>55.89</v>
       </c>
       <c r="G161" t="inlineStr"/>
       <c r="H161" t="n">
-        <v>0</v>
+        <v>-4.46</v>
       </c>
     </row>
     <row r="162">
@@ -4644,11 +4646,11 @@
         <v>0</v>
       </c>
       <c r="F162" t="n">
-        <v>1343</v>
+        <v>1346</v>
       </c>
       <c r="G162" t="inlineStr"/>
       <c r="H162" t="n">
-        <v>-1.76</v>
+        <v>-1.54</v>
       </c>
     </row>
     <row r="163">
@@ -4670,11 +4672,11 @@
         <v>0</v>
       </c>
       <c r="F163" t="n">
-        <v>41.46</v>
+        <v>40.78</v>
       </c>
       <c r="G163" t="inlineStr"/>
       <c r="H163" t="n">
-        <v>-0.79</v>
+        <v>-2.42</v>
       </c>
     </row>
     <row r="164">
@@ -4696,11 +4698,11 @@
         <v>0</v>
       </c>
       <c r="F164" t="n">
-        <v>425</v>
+        <v>441</v>
       </c>
       <c r="G164" t="inlineStr"/>
       <c r="H164" t="n">
-        <v>2.41</v>
+        <v>6.27</v>
       </c>
     </row>
     <row r="165">
@@ -4722,11 +4724,11 @@
         <v>0</v>
       </c>
       <c r="F165" t="n">
-        <v>26.98</v>
+        <v>27.13</v>
       </c>
       <c r="G165" t="inlineStr"/>
       <c r="H165" t="n">
-        <v>1.09</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="166">
@@ -4748,11 +4750,11 @@
         <v>0</v>
       </c>
       <c r="F166" t="n">
-        <v>16.89</v>
+        <v>16.56</v>
       </c>
       <c r="G166" t="inlineStr"/>
       <c r="H166" t="n">
-        <v>0.3</v>
+        <v>-1.66</v>
       </c>
     </row>
     <row r="167">
@@ -4800,11 +4802,11 @@
         <v>0</v>
       </c>
       <c r="F168" t="n">
-        <v>10.1</v>
+        <v>9.970000000000001</v>
       </c>
       <c r="G168" t="inlineStr"/>
       <c r="H168" t="n">
-        <v>-0.98</v>
+        <v>-2.25</v>
       </c>
     </row>
     <row r="169">
@@ -4826,11 +4828,11 @@
         <v>0</v>
       </c>
       <c r="F169" t="n">
-        <v>724.6</v>
+        <v>710</v>
       </c>
       <c r="G169" t="inlineStr"/>
       <c r="H169" t="n">
-        <v>-1.15</v>
+        <v>-3.14</v>
       </c>
     </row>
     <row r="170">
@@ -4852,11 +4854,11 @@
         <v>0</v>
       </c>
       <c r="F170" t="n">
-        <v>6.57</v>
+        <v>6.51</v>
       </c>
       <c r="G170" t="inlineStr"/>
       <c r="H170" t="n">
-        <v>-1.5</v>
+        <v>-2.4</v>
       </c>
     </row>
     <row r="171">
@@ -4878,11 +4880,11 @@
         <v>0</v>
       </c>
       <c r="F171" t="n">
-        <v>18.66</v>
+        <v>18.47</v>
       </c>
       <c r="G171" t="inlineStr"/>
       <c r="H171" t="n">
-        <v>-1.27</v>
+        <v>-2.28</v>
       </c>
     </row>
     <row r="172">
@@ -4904,11 +4906,11 @@
         <v>0</v>
       </c>
       <c r="F172" t="n">
-        <v>26.09</v>
+        <v>25.5</v>
       </c>
       <c r="G172" t="inlineStr"/>
       <c r="H172" t="n">
-        <v>-3.3</v>
+        <v>-5.49</v>
       </c>
     </row>
     <row r="173">
@@ -4930,11 +4932,11 @@
         <v>0</v>
       </c>
       <c r="F173" t="n">
-        <v>84.53</v>
+        <v>81.34</v>
       </c>
       <c r="G173" t="inlineStr"/>
       <c r="H173" t="n">
-        <v>-1.02</v>
+        <v>-4.75</v>
       </c>
     </row>
     <row r="174">
@@ -4956,11 +4958,11 @@
         <v>0</v>
       </c>
       <c r="F174" t="n">
-        <v>174.84</v>
+        <v>172.85</v>
       </c>
       <c r="G174" t="inlineStr"/>
       <c r="H174" t="n">
-        <v>2.25</v>
+        <v>1.09</v>
       </c>
     </row>
     <row r="175">
@@ -4982,11 +4984,11 @@
         <v>0</v>
       </c>
       <c r="F175" t="n">
-        <v>1727</v>
+        <v>1799</v>
       </c>
       <c r="G175" t="inlineStr"/>
       <c r="H175" t="n">
-        <v>-1.93</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="176">
@@ -5008,11 +5010,11 @@
         <v>0</v>
       </c>
       <c r="F176" t="n">
-        <v>25.49</v>
+        <v>25.55</v>
       </c>
       <c r="G176" t="inlineStr"/>
       <c r="H176" t="n">
-        <v>-1.12</v>
+        <v>-0.89</v>
       </c>
     </row>
     <row r="177">
@@ -5034,11 +5036,11 @@
         <v>0</v>
       </c>
       <c r="F177" t="n">
-        <v>17.44</v>
+        <v>17.4</v>
       </c>
       <c r="G177" t="inlineStr"/>
       <c r="H177" t="n">
-        <v>-0.91</v>
+        <v>-1.14</v>
       </c>
     </row>
     <row r="178">
@@ -5060,11 +5062,11 @@
         <v>0</v>
       </c>
       <c r="F178" t="n">
-        <v>591.65</v>
+        <v>595</v>
       </c>
       <c r="G178" t="inlineStr"/>
       <c r="H178" t="n">
-        <v>-0.5600000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179">
@@ -5086,11 +5088,11 @@
         <v>0</v>
       </c>
       <c r="F179" t="n">
-        <v>8.109999999999999</v>
+        <v>8.140000000000001</v>
       </c>
       <c r="G179" t="inlineStr"/>
       <c r="H179" t="n">
-        <v>-1.1</v>
+        <v>-0.73</v>
       </c>
     </row>
     <row r="180">
@@ -5112,11 +5114,11 @@
         <v>0</v>
       </c>
       <c r="F180" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G180" t="inlineStr"/>
       <c r="H180" t="n">
-        <v>-2.12</v>
+        <v>-1.03</v>
       </c>
     </row>
     <row r="181">
@@ -5138,11 +5140,11 @@
         <v>0</v>
       </c>
       <c r="F181" t="n">
-        <v>27.19</v>
+        <v>27.42</v>
       </c>
       <c r="G181" t="inlineStr"/>
       <c r="H181" t="n">
-        <v>-1.38</v>
+        <v>-0.54</v>
       </c>
     </row>
     <row r="182">
@@ -5164,11 +5166,11 @@
         <v>0</v>
       </c>
       <c r="F182" t="n">
-        <v>27.8</v>
+        <v>27.25</v>
       </c>
       <c r="G182" t="inlineStr"/>
       <c r="H182" t="n">
-        <v>-0.14</v>
+        <v>-2.12</v>
       </c>
     </row>
     <row r="183">
@@ -5190,11 +5192,11 @@
         <v>0</v>
       </c>
       <c r="F183" t="n">
-        <v>263.95</v>
+        <v>264.55</v>
       </c>
       <c r="G183" t="inlineStr"/>
       <c r="H183" t="n">
-        <v>-1.46</v>
+        <v>-1.23</v>
       </c>
     </row>
     <row r="184">
@@ -5216,11 +5218,11 @@
         <v>0</v>
       </c>
       <c r="F184" t="n">
-        <v>1043.7</v>
+        <v>1030</v>
       </c>
       <c r="G184" t="inlineStr"/>
       <c r="H184" t="n">
-        <v>-0.79</v>
+        <v>-2.09</v>
       </c>
     </row>
     <row r="185">
@@ -5242,11 +5244,11 @@
         <v>0</v>
       </c>
       <c r="F185" t="n">
-        <v>69.56999999999999</v>
+        <v>69.58</v>
       </c>
       <c r="G185" t="inlineStr"/>
       <c r="H185" t="n">
-        <v>-0.83</v>
+        <v>-0.8100000000000001</v>
       </c>
     </row>
     <row r="186">
@@ -5268,11 +5270,11 @@
         <v>0</v>
       </c>
       <c r="F186" t="n">
-        <v>142.25</v>
+        <v>139.3</v>
       </c>
       <c r="G186" t="inlineStr"/>
       <c r="H186" t="n">
-        <v>1.17</v>
+        <v>-0.92</v>
       </c>
     </row>
     <row r="187">
@@ -5294,11 +5296,11 @@
         <v>0</v>
       </c>
       <c r="F187" t="n">
-        <v>88.84999999999999</v>
+        <v>94</v>
       </c>
       <c r="G187" t="inlineStr"/>
       <c r="H187" t="n">
-        <v>1.78</v>
+        <v>7.67</v>
       </c>
     </row>
     <row r="188">
@@ -5320,11 +5322,11 @@
         <v>0</v>
       </c>
       <c r="F188" t="n">
-        <v>8.59</v>
+        <v>8.619999999999999</v>
       </c>
       <c r="G188" t="inlineStr"/>
       <c r="H188" t="n">
-        <v>-1.6</v>
+        <v>-1.26</v>
       </c>
     </row>
     <row r="189">
@@ -5346,11 +5348,11 @@
         <v>0</v>
       </c>
       <c r="F189" t="n">
-        <v>628.1</v>
+        <v>625.45</v>
       </c>
       <c r="G189" t="inlineStr"/>
       <c r="H189" t="n">
-        <v>1.47</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="190">
@@ -5372,11 +5374,11 @@
         <v>0</v>
       </c>
       <c r="F190" t="n">
-        <v>309.1</v>
+        <v>305</v>
       </c>
       <c r="G190" t="inlineStr"/>
       <c r="H190" t="n">
-        <v>-0.48</v>
+        <v>-1.8</v>
       </c>
     </row>
     <row r="191">
@@ -5398,11 +5400,11 @@
         <v>0</v>
       </c>
       <c r="F191" t="n">
-        <v>820.3</v>
+        <v>816</v>
       </c>
       <c r="G191" t="inlineStr"/>
       <c r="H191" t="n">
-        <v>0.06</v>
+        <v>-0.46</v>
       </c>
     </row>
     <row r="192">
@@ -5424,11 +5426,11 @@
         <v>0</v>
       </c>
       <c r="F192" t="n">
-        <v>4.7</v>
+        <v>5.08</v>
       </c>
       <c r="G192" t="inlineStr"/>
       <c r="H192" t="n">
-        <v>-0.84</v>
+        <v>7.17</v>
       </c>
     </row>
     <row r="193">
@@ -5450,11 +5452,11 @@
         <v>0</v>
       </c>
       <c r="F193" t="n">
-        <v>268.2</v>
+        <v>260.1</v>
       </c>
       <c r="G193" t="inlineStr"/>
       <c r="H193" t="n">
-        <v>-1.12</v>
+        <v>-4.11</v>
       </c>
     </row>
     <row r="194">
@@ -5476,11 +5478,11 @@
         <v>0</v>
       </c>
       <c r="F194" t="n">
-        <v>402.1</v>
+        <v>399.15</v>
       </c>
       <c r="G194" t="inlineStr"/>
       <c r="H194" t="n">
-        <v>-1.64</v>
+        <v>-2.36</v>
       </c>
     </row>
     <row r="195">
@@ -5502,11 +5504,11 @@
         <v>0</v>
       </c>
       <c r="F195" t="n">
-        <v>131.76</v>
+        <v>132.55</v>
       </c>
       <c r="G195" t="inlineStr"/>
       <c r="H195" t="n">
-        <v>-0.82</v>
+        <v>-0.23</v>
       </c>
     </row>
     <row r="196">
@@ -5528,11 +5530,11 @@
         <v>0</v>
       </c>
       <c r="F196" t="n">
-        <v>529.35</v>
+        <v>524.95</v>
       </c>
       <c r="G196" t="inlineStr"/>
       <c r="H196" t="n">
-        <v>-1.1</v>
+        <v>-1.92</v>
       </c>
     </row>
     <row r="197">
@@ -5554,11 +5556,11 @@
         <v>0</v>
       </c>
       <c r="F197" t="n">
-        <v>74.3</v>
+        <v>74.31</v>
       </c>
       <c r="G197" t="inlineStr"/>
       <c r="H197" t="n">
-        <v>-0.93</v>
+        <v>-0.92</v>
       </c>
     </row>
     <row r="198">
@@ -5580,11 +5582,11 @@
         <v>0</v>
       </c>
       <c r="F198" t="n">
-        <v>504.6</v>
+        <v>507.5</v>
       </c>
       <c r="G198" t="inlineStr"/>
       <c r="H198" t="n">
-        <v>-1.79</v>
+        <v>-1.23</v>
       </c>
     </row>
     <row r="199">
@@ -5606,11 +5608,11 @@
         <v>0</v>
       </c>
       <c r="F199" t="n">
-        <v>52.6</v>
+        <v>53.25</v>
       </c>
       <c r="G199" t="inlineStr"/>
       <c r="H199" t="n">
-        <v>-1.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200">
@@ -5632,11 +5634,11 @@
         <v>0</v>
       </c>
       <c r="F200" t="n">
-        <v>272.2</v>
+        <v>271</v>
       </c>
       <c r="G200" t="inlineStr"/>
       <c r="H200" t="n">
-        <v>-1.02</v>
+        <v>-1.45</v>
       </c>
     </row>
     <row r="201">
@@ -5658,11 +5660,11 @@
         <v>0</v>
       </c>
       <c r="F201" t="n">
-        <v>321.2</v>
+        <v>321.05</v>
       </c>
       <c r="G201" t="inlineStr"/>
       <c r="H201" t="n">
-        <v>-0.5</v>
+        <v>-0.54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto: update momentum data - 2026-01-15 04:32 UTC
</commit_message>
<xml_diff>
--- a/data/trending_momentum_stocks.xlsx
+++ b/data/trending_momentum_stocks.xlsx
@@ -494,11 +494,11 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>92.84999999999999</v>
+        <v>83</v>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
-        <v>-0.16</v>
+        <v>-10.75</v>
       </c>
     </row>
     <row r="3">
@@ -520,11 +520,11 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>7.18</v>
+        <v>7.14</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
-        <v>-5.53</v>
+        <v>-6.05</v>
       </c>
     </row>
     <row r="4">
@@ -546,11 +546,11 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>148.84</v>
+        <v>150</v>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
-        <v>-9.789999999999999</v>
+        <v>-9.09</v>
       </c>
     </row>
     <row r="5">
@@ -572,11 +572,11 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>178.51</v>
+        <v>183.75</v>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
-        <v>-7.5</v>
+        <v>-4.79</v>
       </c>
     </row>
     <row r="6">
@@ -598,11 +598,11 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>30.79</v>
+        <v>30.88</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
-        <v>-6.64</v>
+        <v>-6.37</v>
       </c>
     </row>
     <row r="7">
@@ -624,11 +624,11 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>95.75</v>
+        <v>97</v>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
-        <v>-7.04</v>
+        <v>-5.83</v>
       </c>
     </row>
     <row r="8">
@@ -650,11 +650,11 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>52.57</v>
+        <v>48.6</v>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
-        <v>-0.44</v>
+        <v>-7.95</v>
       </c>
     </row>
     <row r="9">
@@ -676,11 +676,11 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>1.89</v>
+        <v>1.85</v>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
-        <v>-7.35</v>
+        <v>-9.31</v>
       </c>
     </row>
     <row r="10">
@@ -702,11 +702,11 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>152.9</v>
+        <v>143</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
-        <v>-3.78</v>
+        <v>-10.01</v>
       </c>
     </row>
     <row r="11">
@@ -728,11 +728,11 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>20.28</v>
+        <v>20.25</v>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="n">
-        <v>-2.97</v>
+        <v>-3.11</v>
       </c>
     </row>
     <row r="12">
@@ -780,11 +780,11 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>7.78</v>
+        <v>7.93</v>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
-        <v>-5.7</v>
+        <v>-3.88</v>
       </c>
     </row>
     <row r="14">
@@ -832,11 +832,11 @@
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>13.2</v>
+        <v>13</v>
       </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="n">
-        <v>-2.22</v>
+        <v>-3.7</v>
       </c>
     </row>
     <row r="16">
@@ -910,11 +910,11 @@
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>30.25</v>
+        <v>29.79</v>
       </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="n">
-        <v>-1.82</v>
+        <v>-3.31</v>
       </c>
     </row>
     <row r="19">
@@ -988,11 +988,11 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>15.6</v>
+        <v>15.4</v>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
-        <v>-4</v>
+        <v>-5.23</v>
       </c>
     </row>
     <row r="22">
@@ -1014,11 +1014,11 @@
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>8.49</v>
+        <v>8.58</v>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="n">
-        <v>-4.07</v>
+        <v>-3.05</v>
       </c>
     </row>
     <row r="23">
@@ -1040,11 +1040,11 @@
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="n">
-        <v>-4.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1066,11 +1066,11 @@
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>139.5</v>
+        <v>139.35</v>
       </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="n">
-        <v>-4.35</v>
+        <v>-4.46</v>
       </c>
     </row>
     <row r="25">
@@ -1092,11 +1092,11 @@
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>9.52</v>
+        <v>9.630000000000001</v>
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="n">
-        <v>-4.8</v>
+        <v>-3.7</v>
       </c>
     </row>
     <row r="26">
@@ -1118,11 +1118,11 @@
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>28.02</v>
+        <v>29</v>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="n">
-        <v>-3.98</v>
+        <v>-0.62</v>
       </c>
     </row>
     <row r="27">
@@ -1144,11 +1144,11 @@
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>13.18</v>
+        <v>13.3</v>
       </c>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="n">
-        <v>-1.49</v>
+        <v>-0.6</v>
       </c>
     </row>
     <row r="28">
@@ -1170,11 +1170,11 @@
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>224.5</v>
+        <v>216.2</v>
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="n">
-        <v>0</v>
+        <v>-3.7</v>
       </c>
     </row>
     <row r="29">
@@ -1196,11 +1196,11 @@
         <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>29.68</v>
+        <v>30.45</v>
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="n">
-        <v>-3.95</v>
+        <v>-1.46</v>
       </c>
     </row>
     <row r="30">
@@ -1248,11 +1248,11 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>128</v>
+        <v>131.4</v>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="n">
-        <v>-0.78</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="32">
@@ -1274,11 +1274,11 @@
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>108.78</v>
+        <v>108.5</v>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="n">
-        <v>-3.95</v>
+        <v>-4.19</v>
       </c>
     </row>
     <row r="33">
@@ -1300,11 +1300,11 @@
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>25.03</v>
+        <v>24.4</v>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="n">
-        <v>-2.76</v>
+        <v>-5.21</v>
       </c>
     </row>
     <row r="34">
@@ -1326,11 +1326,11 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>28.23</v>
+        <v>28.36</v>
       </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="n">
-        <v>-4.31</v>
+        <v>-3.86</v>
       </c>
     </row>
     <row r="35">
@@ -1352,11 +1352,11 @@
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>1599.2</v>
+        <v>1587</v>
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="n">
-        <v>-3.02</v>
+        <v>-3.76</v>
       </c>
     </row>
     <row r="36">
@@ -1378,11 +1378,11 @@
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>8.029999999999999</v>
+        <v>7.98</v>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="n">
-        <v>-2.43</v>
+        <v>-3.04</v>
       </c>
     </row>
     <row r="37">
@@ -1404,11 +1404,11 @@
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>2088.4</v>
+        <v>2080</v>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="n">
-        <v>-2.68</v>
+        <v>-3.07</v>
       </c>
     </row>
     <row r="38">
@@ -1430,11 +1430,11 @@
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>1.7</v>
+        <v>1.75</v>
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="n">
-        <v>-5.56</v>
+        <v>-2.78</v>
       </c>
     </row>
     <row r="39">
@@ -1482,11 +1482,11 @@
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>58.9</v>
+        <v>59</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="n">
-        <v>-6.49</v>
+        <v>-6.33</v>
       </c>
     </row>
     <row r="41">
@@ -1508,11 +1508,11 @@
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>394</v>
+        <v>395.75</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="n">
-        <v>1.29</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="42">
@@ -1534,11 +1534,11 @@
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>22.38</v>
+        <v>21.95</v>
       </c>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="n">
-        <v>-2.06</v>
+        <v>-3.94</v>
       </c>
     </row>
     <row r="43">
@@ -1560,11 +1560,11 @@
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>16.9</v>
+        <v>16.56</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="n">
-        <v>-2.31</v>
+        <v>-4.28</v>
       </c>
     </row>
     <row r="44">
@@ -1586,11 +1586,11 @@
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>39</v>
+        <v>37.2</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="n">
-        <v>-1.66</v>
+        <v>-6.2</v>
       </c>
     </row>
     <row r="45">
@@ -1612,11 +1612,11 @@
         <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>451.05</v>
+        <v>445</v>
       </c>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="n">
-        <v>-4.84</v>
+        <v>-6.12</v>
       </c>
     </row>
     <row r="46">
@@ -1638,11 +1638,11 @@
         <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>29.23</v>
+        <v>29.13</v>
       </c>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="n">
-        <v>-2.53</v>
+        <v>-2.87</v>
       </c>
     </row>
     <row r="47">
@@ -1664,11 +1664,11 @@
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>948.1</v>
+        <v>944</v>
       </c>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="n">
-        <v>-2.45</v>
+        <v>-2.87</v>
       </c>
     </row>
     <row r="48">
@@ -1690,11 +1690,11 @@
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>44</v>
+        <v>45.49</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="n">
-        <v>-1.98</v>
+        <v>1.34</v>
       </c>
     </row>
     <row r="49">
@@ -1716,11 +1716,11 @@
         <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>14.07</v>
+        <v>14.05</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="n">
-        <v>-4.93</v>
+        <v>-5.07</v>
       </c>
     </row>
     <row r="50">
@@ -1768,11 +1768,11 @@
         <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>199.62</v>
+        <v>200</v>
       </c>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="n">
-        <v>-2.36</v>
+        <v>-2.18</v>
       </c>
     </row>
     <row r="52">
@@ -1794,11 +1794,11 @@
         <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>316.8</v>
+        <v>316.15</v>
       </c>
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="n">
-        <v>-2.43</v>
+        <v>-2.63</v>
       </c>
     </row>
     <row r="53">
@@ -1820,11 +1820,11 @@
         <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>0.37</v>
+        <v>0.36</v>
       </c>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="n">
-        <v>0</v>
+        <v>-2.7</v>
       </c>
     </row>
     <row r="54">
@@ -1846,11 +1846,11 @@
         <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>82.51000000000001</v>
+        <v>82.65000000000001</v>
       </c>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="n">
-        <v>-2.82</v>
+        <v>-2.65</v>
       </c>
     </row>
     <row r="55">
@@ -1872,11 +1872,11 @@
         <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>296.45</v>
+        <v>288.35</v>
       </c>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="n">
-        <v>-1.18</v>
+        <v>-3.88</v>
       </c>
     </row>
     <row r="56">
@@ -1898,11 +1898,11 @@
         <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>32.56</v>
+        <v>32.2</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="n">
-        <v>-3.33</v>
+        <v>-4.39</v>
       </c>
     </row>
     <row r="57">
@@ -1924,11 +1924,11 @@
         <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>215.79</v>
+        <v>217.41</v>
       </c>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="n">
-        <v>-2.34</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="58">
@@ -1950,11 +1950,11 @@
         <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>94.52</v>
+        <v>92.51000000000001</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="n">
-        <v>-1.39</v>
+        <v>-3.48</v>
       </c>
     </row>
     <row r="59">
@@ -1976,11 +1976,11 @@
         <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>3358.5</v>
+        <v>3350</v>
       </c>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="n">
-        <v>2.24</v>
+        <v>1.98</v>
       </c>
     </row>
     <row r="60">
@@ -2002,11 +2002,11 @@
         <v>0</v>
       </c>
       <c r="F60" t="n">
-        <v>15.8</v>
+        <v>15.7</v>
       </c>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="n">
-        <v>-3.36</v>
+        <v>-3.98</v>
       </c>
     </row>
     <row r="61">
@@ -2028,11 +2028,11 @@
         <v>0</v>
       </c>
       <c r="F61" t="n">
-        <v>97.73</v>
+        <v>96.53</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="n">
-        <v>-2.27</v>
+        <v>-3.47</v>
       </c>
     </row>
     <row r="62">
@@ -2054,11 +2054,11 @@
         <v>0</v>
       </c>
       <c r="F62" t="n">
-        <v>72.5</v>
+        <v>71.5</v>
       </c>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="n">
-        <v>0.55</v>
+        <v>-0.83</v>
       </c>
     </row>
     <row r="63">
@@ -2080,11 +2080,11 @@
         <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>9.359999999999999</v>
+        <v>9.84</v>
       </c>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="n">
-        <v>-4.49</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="64">
@@ -2106,11 +2106,11 @@
         <v>0</v>
       </c>
       <c r="F64" t="n">
-        <v>7.63</v>
+        <v>7.68</v>
       </c>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="n">
-        <v>-2.43</v>
+        <v>-1.79</v>
       </c>
     </row>
     <row r="65">
@@ -2158,11 +2158,11 @@
         <v>0</v>
       </c>
       <c r="F66" t="n">
-        <v>228.95</v>
+        <v>227.2</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="n">
-        <v>-3.4</v>
+        <v>-4.14</v>
       </c>
     </row>
     <row r="67">
@@ -2184,11 +2184,11 @@
         <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>3.94</v>
+        <v>3.82</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="n">
-        <v>-1.5</v>
+        <v>-4.5</v>
       </c>
     </row>
     <row r="68">
@@ -2210,11 +2210,11 @@
         <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>4.81</v>
+        <v>4.8</v>
       </c>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="n">
-        <v>0</v>
+        <v>-0.21</v>
       </c>
     </row>
     <row r="69">
@@ -2236,11 +2236,11 @@
         <v>0</v>
       </c>
       <c r="F69" t="n">
-        <v>196.05</v>
+        <v>199.9</v>
       </c>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="n">
-        <v>-2.83</v>
+        <v>-0.92</v>
       </c>
     </row>
     <row r="70">
@@ -2262,11 +2262,11 @@
         <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>2.44</v>
+        <v>2.33</v>
       </c>
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="n">
-        <v>-0.8100000000000001</v>
+        <v>-5.28</v>
       </c>
     </row>
     <row r="71">
@@ -2288,11 +2288,11 @@
         <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>15.85</v>
+        <v>16.35</v>
       </c>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="n">
-        <v>-4.4</v>
+        <v>-1.39</v>
       </c>
     </row>
     <row r="72">
@@ -2314,11 +2314,11 @@
         <v>0</v>
       </c>
       <c r="F72" t="n">
-        <v>4.88</v>
+        <v>4.95</v>
       </c>
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="n">
-        <v>-2.2</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="73">
@@ -2340,11 +2340,11 @@
         <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>77.81999999999999</v>
+        <v>78.48</v>
       </c>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="n">
-        <v>-1.49</v>
+        <v>-0.66</v>
       </c>
     </row>
     <row r="74">
@@ -2392,11 +2392,11 @@
         <v>0</v>
       </c>
       <c r="F75" t="n">
-        <v>2.96</v>
+        <v>2.98</v>
       </c>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="n">
-        <v>-0.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -2418,11 +2418,11 @@
         <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>75.87</v>
+        <v>74.8</v>
       </c>
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="n">
-        <v>-1.21</v>
+        <v>-2.6</v>
       </c>
     </row>
     <row r="77">
@@ -2444,11 +2444,11 @@
         <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>20.99</v>
+        <v>19.69</v>
       </c>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="n">
-        <v>0</v>
+        <v>-6.19</v>
       </c>
     </row>
     <row r="78">
@@ -2470,11 +2470,11 @@
         <v>0</v>
       </c>
       <c r="F78" t="n">
-        <v>95.72</v>
+        <v>96.55</v>
       </c>
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="n">
-        <v>-2.33</v>
+        <v>-1.48</v>
       </c>
     </row>
     <row r="79">
@@ -2496,11 +2496,11 @@
         <v>0</v>
       </c>
       <c r="F79" t="n">
-        <v>97.56</v>
+        <v>97</v>
       </c>
       <c r="G79" t="inlineStr"/>
       <c r="H79" t="n">
-        <v>-1.45</v>
+        <v>-2.02</v>
       </c>
     </row>
     <row r="80">
@@ -2522,11 +2522,11 @@
         <v>0</v>
       </c>
       <c r="F80" t="n">
-        <v>1317.8</v>
+        <v>1307</v>
       </c>
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="n">
-        <v>0.6</v>
+        <v>-0.23</v>
       </c>
     </row>
     <row r="81">
@@ -2548,11 +2548,11 @@
         <v>0</v>
       </c>
       <c r="F81" t="n">
-        <v>1.29</v>
+        <v>1.3</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="n">
-        <v>-3.73</v>
+        <v>-2.99</v>
       </c>
     </row>
     <row r="82">
@@ -2574,11 +2574,11 @@
         <v>0</v>
       </c>
       <c r="F82" t="n">
-        <v>3.3</v>
+        <v>3.55</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="n">
-        <v>2.17</v>
+        <v>9.91</v>
       </c>
     </row>
     <row r="83">
@@ -2600,11 +2600,11 @@
         <v>0</v>
       </c>
       <c r="F83" t="n">
-        <v>105.63</v>
+        <v>105.5</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="n">
-        <v>-1.27</v>
+        <v>-1.39</v>
       </c>
     </row>
     <row r="84">
@@ -2648,11 +2648,11 @@
         <v>0</v>
       </c>
       <c r="F85" t="n">
-        <v>893.95</v>
+        <v>854</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="n">
-        <v>-3.36</v>
+        <v>-7.68</v>
       </c>
     </row>
     <row r="86">
@@ -2674,11 +2674,11 @@
         <v>0</v>
       </c>
       <c r="F86" t="n">
-        <v>616.6</v>
+        <v>614.05</v>
       </c>
       <c r="G86" t="inlineStr"/>
       <c r="H86" t="n">
-        <v>-1.77</v>
+        <v>-2.17</v>
       </c>
     </row>
     <row r="87">
@@ -2700,11 +2700,11 @@
         <v>0</v>
       </c>
       <c r="F87" t="n">
-        <v>780.7</v>
+        <v>779.95</v>
       </c>
       <c r="G87" t="inlineStr"/>
       <c r="H87" t="n">
-        <v>2.74</v>
+        <v>2.64</v>
       </c>
     </row>
     <row r="88">
@@ -2752,11 +2752,11 @@
         <v>0</v>
       </c>
       <c r="F89" t="n">
-        <v>42.97</v>
+        <v>44.22</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="n">
-        <v>-0.53</v>
+        <v>2.36</v>
       </c>
     </row>
     <row r="90">
@@ -2778,11 +2778,11 @@
         <v>0</v>
       </c>
       <c r="F90" t="n">
-        <v>9.27</v>
+        <v>9.43</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="n">
-        <v>-0.11</v>
+        <v>1.62</v>
       </c>
     </row>
     <row r="91">
@@ -2804,11 +2804,11 @@
         <v>0</v>
       </c>
       <c r="F91" t="n">
-        <v>0.49</v>
+        <v>0.48</v>
       </c>
       <c r="G91" t="inlineStr"/>
       <c r="H91" t="n">
-        <v>0</v>
+        <v>-2.04</v>
       </c>
     </row>
     <row r="92">
@@ -2830,11 +2830,11 @@
         <v>0</v>
       </c>
       <c r="F92" t="n">
-        <v>38.93</v>
+        <v>34.02</v>
       </c>
       <c r="G92" t="inlineStr"/>
       <c r="H92" t="n">
-        <v>15.28</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="93">
@@ -2856,11 +2856,11 @@
         <v>0</v>
       </c>
       <c r="F93" t="n">
-        <v>22.04</v>
+        <v>22.11</v>
       </c>
       <c r="G93" t="inlineStr"/>
       <c r="H93" t="n">
-        <v>-2</v>
+        <v>-1.69</v>
       </c>
     </row>
     <row r="94">
@@ -2882,11 +2882,11 @@
         <v>0</v>
       </c>
       <c r="F94" t="n">
-        <v>38.4</v>
+        <v>39.25</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="n">
-        <v>-1.71</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="95">
@@ -2908,11 +2908,11 @@
         <v>0</v>
       </c>
       <c r="F95" t="n">
-        <v>25.8</v>
+        <v>26.96</v>
       </c>
       <c r="G95" t="inlineStr"/>
       <c r="H95" t="n">
-        <v>-2.27</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="96">
@@ -2934,11 +2934,11 @@
         <v>0</v>
       </c>
       <c r="F96" t="n">
-        <v>10.36</v>
+        <v>10.2</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="n">
-        <v>-3.27</v>
+        <v>-4.76</v>
       </c>
     </row>
     <row r="97">
@@ -2960,11 +2960,11 @@
         <v>0</v>
       </c>
       <c r="F97" t="n">
-        <v>213.05</v>
+        <v>213.65</v>
       </c>
       <c r="G97" t="inlineStr"/>
       <c r="H97" t="n">
-        <v>-4.58</v>
+        <v>-4.31</v>
       </c>
     </row>
     <row r="98">
@@ -2986,11 +2986,11 @@
         <v>0</v>
       </c>
       <c r="F98" t="n">
-        <v>220.7</v>
+        <v>215</v>
       </c>
       <c r="G98" t="inlineStr"/>
       <c r="H98" t="n">
-        <v>-1.47</v>
+        <v>-4.02</v>
       </c>
     </row>
     <row r="99">
@@ -3012,11 +3012,11 @@
         <v>0</v>
       </c>
       <c r="F99" t="n">
-        <v>33.9</v>
+        <v>33.1</v>
       </c>
       <c r="G99" t="inlineStr"/>
       <c r="H99" t="n">
-        <v>-1.05</v>
+        <v>-3.39</v>
       </c>
     </row>
     <row r="100">
@@ -3038,11 +3038,11 @@
         <v>0</v>
       </c>
       <c r="F100" t="n">
-        <v>325.2</v>
+        <v>320</v>
       </c>
       <c r="G100" t="inlineStr"/>
       <c r="H100" t="n">
-        <v>0.99</v>
+        <v>-0.62</v>
       </c>
     </row>
     <row r="101">
@@ -3064,11 +3064,11 @@
         <v>0</v>
       </c>
       <c r="F101" t="n">
-        <v>8.300000000000001</v>
+        <v>7.92</v>
       </c>
       <c r="G101" t="inlineStr"/>
       <c r="H101" t="n">
-        <v>-0.84</v>
+        <v>-5.38</v>
       </c>
     </row>
     <row r="102">
@@ -3090,11 +3090,11 @@
         <v>0</v>
       </c>
       <c r="F102" t="n">
-        <v>14.8</v>
+        <v>15</v>
       </c>
       <c r="G102" t="inlineStr"/>
       <c r="H102" t="n">
-        <v>-2.37</v>
+        <v>-1.06</v>
       </c>
     </row>
     <row r="103">
@@ -3116,11 +3116,11 @@
         <v>0</v>
       </c>
       <c r="F103" t="n">
-        <v>3.63</v>
+        <v>3.66</v>
       </c>
       <c r="G103" t="inlineStr"/>
       <c r="H103" t="n">
-        <v>-1.89</v>
+        <v>-1.08</v>
       </c>
     </row>
     <row r="104">
@@ -3142,11 +3142,11 @@
         <v>0</v>
       </c>
       <c r="F104" t="n">
-        <v>190.06</v>
+        <v>198.75</v>
       </c>
       <c r="G104" t="inlineStr"/>
       <c r="H104" t="n">
-        <v>-1.52</v>
+        <v>2.98</v>
       </c>
     </row>
     <row r="105">
@@ -3168,11 +3168,11 @@
         <v>0</v>
       </c>
       <c r="F105" t="n">
-        <v>0.53</v>
+        <v>0.52</v>
       </c>
       <c r="G105" t="inlineStr"/>
       <c r="H105" t="n">
-        <v>0</v>
+        <v>-1.89</v>
       </c>
     </row>
     <row r="106">
@@ -3194,11 +3194,11 @@
         <v>0</v>
       </c>
       <c r="F106" t="n">
-        <v>1954.4</v>
+        <v>1902.05</v>
       </c>
       <c r="G106" t="inlineStr"/>
       <c r="H106" t="n">
-        <v>-2.28</v>
+        <v>-4.9</v>
       </c>
     </row>
     <row r="107">
@@ -3220,11 +3220,11 @@
         <v>0</v>
       </c>
       <c r="F107" t="n">
-        <v>151.62</v>
+        <v>155.3</v>
       </c>
       <c r="G107" t="inlineStr"/>
       <c r="H107" t="n">
-        <v>-2.81</v>
+        <v>-0.45</v>
       </c>
     </row>
     <row r="108">
@@ -3246,11 +3246,11 @@
         <v>0</v>
       </c>
       <c r="F108" t="n">
-        <v>2103</v>
+        <v>2033</v>
       </c>
       <c r="G108" t="inlineStr"/>
       <c r="H108" t="n">
-        <v>3.85</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="109">
@@ -3272,11 +3272,11 @@
         <v>0</v>
       </c>
       <c r="F109" t="n">
-        <v>127.11</v>
+        <v>126.95</v>
       </c>
       <c r="G109" t="inlineStr"/>
       <c r="H109" t="n">
-        <v>-2.57</v>
+        <v>-2.69</v>
       </c>
     </row>
     <row r="110">
@@ -3298,11 +3298,11 @@
         <v>0</v>
       </c>
       <c r="F110" t="n">
-        <v>13.01</v>
+        <v>13</v>
       </c>
       <c r="G110" t="inlineStr"/>
       <c r="H110" t="n">
-        <v>-1.74</v>
+        <v>-1.81</v>
       </c>
     </row>
     <row r="111">
@@ -3324,11 +3324,11 @@
         <v>0</v>
       </c>
       <c r="F111" t="n">
-        <v>102.59</v>
+        <v>99.31</v>
       </c>
       <c r="G111" t="inlineStr"/>
       <c r="H111" t="n">
-        <v>-0.39</v>
+        <v>-3.57</v>
       </c>
     </row>
     <row r="112">
@@ -3350,11 +3350,11 @@
         <v>0</v>
       </c>
       <c r="F112" t="n">
-        <v>56.95</v>
+        <v>55.4</v>
       </c>
       <c r="G112" t="inlineStr"/>
       <c r="H112" t="n">
-        <v>1.7</v>
+        <v>-1.07</v>
       </c>
     </row>
     <row r="113">
@@ -3376,11 +3376,11 @@
         <v>0</v>
       </c>
       <c r="F113" t="n">
-        <v>6.39</v>
+        <v>6.27</v>
       </c>
       <c r="G113" t="inlineStr"/>
       <c r="H113" t="n">
-        <v>2.73</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="114">
@@ -3402,11 +3402,11 @@
         <v>0</v>
       </c>
       <c r="F114" t="n">
-        <v>7.84</v>
+        <v>7.71</v>
       </c>
       <c r="G114" t="inlineStr"/>
       <c r="H114" t="n">
-        <v>-0.76</v>
+        <v>-2.41</v>
       </c>
     </row>
     <row r="115">
@@ -3428,11 +3428,11 @@
         <v>0</v>
       </c>
       <c r="F115" t="n">
-        <v>1.64</v>
+        <v>1.68</v>
       </c>
       <c r="G115" t="inlineStr"/>
       <c r="H115" t="n">
-        <v>-3.53</v>
+        <v>-1.18</v>
       </c>
     </row>
     <row r="116">
@@ -3454,11 +3454,11 @@
         <v>0</v>
       </c>
       <c r="F116" t="n">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G116" t="inlineStr"/>
       <c r="H116" t="n">
-        <v>-1.3</v>
+        <v>-0.65</v>
       </c>
     </row>
     <row r="117">
@@ -3480,11 +3480,11 @@
         <v>0</v>
       </c>
       <c r="F117" t="n">
-        <v>64.12</v>
+        <v>63.94</v>
       </c>
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="n">
-        <v>-2.85</v>
+        <v>-3.12</v>
       </c>
     </row>
     <row r="118">
@@ -3506,11 +3506,11 @@
         <v>0</v>
       </c>
       <c r="F118" t="n">
-        <v>0.58</v>
+        <v>0.59</v>
       </c>
       <c r="G118" t="inlineStr"/>
       <c r="H118" t="n">
-        <v>0</v>
+        <v>1.72</v>
       </c>
     </row>
     <row r="119">
@@ -3532,11 +3532,11 @@
         <v>0</v>
       </c>
       <c r="F119" t="n">
-        <v>22.03</v>
+        <v>22.55</v>
       </c>
       <c r="G119" t="inlineStr"/>
       <c r="H119" t="n">
-        <v>-0.63</v>
+        <v>1.71</v>
       </c>
     </row>
     <row r="120">
@@ -3558,11 +3558,11 @@
         <v>0</v>
       </c>
       <c r="F120" t="n">
-        <v>25.57</v>
+        <v>24.65</v>
       </c>
       <c r="G120" t="inlineStr"/>
       <c r="H120" t="n">
-        <v>1.51</v>
+        <v>-2.14</v>
       </c>
     </row>
     <row r="121">
@@ -3584,11 +3584,11 @@
         <v>0</v>
       </c>
       <c r="F121" t="n">
-        <v>2.34</v>
+        <v>2.21</v>
       </c>
       <c r="G121" t="inlineStr"/>
       <c r="H121" t="n">
-        <v>-1.68</v>
+        <v>-7.14</v>
       </c>
     </row>
     <row r="122">
@@ -3610,11 +3610,11 @@
         <v>0</v>
       </c>
       <c r="F122" t="n">
-        <v>7.1</v>
+        <v>7.11</v>
       </c>
       <c r="G122" t="inlineStr"/>
       <c r="H122" t="n">
-        <v>-1.25</v>
+        <v>-1.11</v>
       </c>
     </row>
     <row r="123">
@@ -3636,11 +3636,11 @@
         <v>0</v>
       </c>
       <c r="F123" t="n">
-        <v>346.15</v>
+        <v>349</v>
       </c>
       <c r="G123" t="inlineStr"/>
       <c r="H123" t="n">
-        <v>-2.47</v>
+        <v>-1.66</v>
       </c>
     </row>
     <row r="124">
@@ -3662,11 +3662,11 @@
         <v>0</v>
       </c>
       <c r="F124" t="n">
-        <v>13.29</v>
+        <v>13.59</v>
       </c>
       <c r="G124" t="inlineStr"/>
       <c r="H124" t="n">
-        <v>-0.82</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="125">
@@ -3688,11 +3688,11 @@
         <v>0</v>
       </c>
       <c r="F125" t="n">
-        <v>34.3</v>
+        <v>34.29</v>
       </c>
       <c r="G125" t="inlineStr"/>
       <c r="H125" t="n">
-        <v>-4.19</v>
+        <v>-4.22</v>
       </c>
     </row>
     <row r="126">
@@ -3714,11 +3714,11 @@
         <v>0</v>
       </c>
       <c r="F126" t="n">
-        <v>106.01</v>
+        <v>104</v>
       </c>
       <c r="G126" t="inlineStr"/>
       <c r="H126" t="n">
-        <v>1.93</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127">
@@ -3740,11 +3740,11 @@
         <v>0</v>
       </c>
       <c r="F127" t="n">
-        <v>47.52</v>
+        <v>46.28</v>
       </c>
       <c r="G127" t="inlineStr"/>
       <c r="H127" t="n">
-        <v>-1.72</v>
+        <v>-4.28</v>
       </c>
     </row>
     <row r="128">
@@ -3766,11 +3766,11 @@
         <v>0</v>
       </c>
       <c r="F128" t="n">
-        <v>667.9</v>
+        <v>655</v>
       </c>
       <c r="G128" t="inlineStr"/>
       <c r="H128" t="n">
-        <v>4.36</v>
+        <v>2.34</v>
       </c>
     </row>
     <row r="129">
@@ -3792,11 +3792,11 @@
         <v>0</v>
       </c>
       <c r="F129" t="n">
-        <v>560.8</v>
+        <v>569</v>
       </c>
       <c r="G129" t="inlineStr"/>
       <c r="H129" t="n">
-        <v>2.33</v>
+        <v>3.82</v>
       </c>
     </row>
     <row r="130">
@@ -3818,11 +3818,11 @@
         <v>0</v>
       </c>
       <c r="F130" t="n">
-        <v>0.64</v>
+        <v>0.63</v>
       </c>
       <c r="G130" t="inlineStr"/>
       <c r="H130" t="n">
-        <v>0</v>
+        <v>-1.56</v>
       </c>
     </row>
     <row r="131">
@@ -3844,11 +3844,11 @@
         <v>0</v>
       </c>
       <c r="F131" t="n">
-        <v>262.3</v>
+        <v>259</v>
       </c>
       <c r="G131" t="inlineStr"/>
       <c r="H131" t="n">
-        <v>1.14</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="132">
@@ -3870,11 +3870,11 @@
         <v>0</v>
       </c>
       <c r="F132" t="n">
-        <v>670.2</v>
+        <v>676</v>
       </c>
       <c r="G132" t="inlineStr"/>
       <c r="H132" t="n">
-        <v>3.59</v>
+        <v>4.48</v>
       </c>
     </row>
     <row r="133">
@@ -3922,11 +3922,11 @@
         <v>0</v>
       </c>
       <c r="F134" t="n">
-        <v>51.64</v>
+        <v>50.94</v>
       </c>
       <c r="G134" t="inlineStr"/>
       <c r="H134" t="n">
-        <v>-0.41</v>
+        <v>-1.76</v>
       </c>
     </row>
     <row r="135">
@@ -3948,11 +3948,11 @@
         <v>0</v>
       </c>
       <c r="F135" t="n">
-        <v>257.3</v>
+        <v>257</v>
       </c>
       <c r="G135" t="inlineStr"/>
       <c r="H135" t="n">
-        <v>-3.83</v>
+        <v>-3.94</v>
       </c>
     </row>
     <row r="136">
@@ -3974,11 +3974,11 @@
         <v>0</v>
       </c>
       <c r="F136" t="n">
-        <v>172.26</v>
+        <v>169.5</v>
       </c>
       <c r="G136" t="inlineStr"/>
       <c r="H136" t="n">
-        <v>-1.96</v>
+        <v>-3.53</v>
       </c>
     </row>
     <row r="137">
@@ -4000,11 +4000,11 @@
         <v>0</v>
       </c>
       <c r="F137" t="n">
-        <v>244.15</v>
+        <v>238</v>
       </c>
       <c r="G137" t="inlineStr"/>
       <c r="H137" t="n">
-        <v>-1.39</v>
+        <v>-3.88</v>
       </c>
     </row>
     <row r="138">
@@ -4026,11 +4026,11 @@
         <v>0</v>
       </c>
       <c r="F138" t="n">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G138" t="inlineStr"/>
       <c r="H138" t="n">
-        <v>0.27</v>
+        <v>-1.5</v>
       </c>
     </row>
     <row r="139">
@@ -4052,11 +4052,11 @@
         <v>0</v>
       </c>
       <c r="F139" t="n">
-        <v>38.29</v>
+        <v>38.65</v>
       </c>
       <c r="G139" t="inlineStr"/>
       <c r="H139" t="n">
-        <v>-1.49</v>
+        <v>-0.57</v>
       </c>
     </row>
     <row r="140">
@@ -4078,11 +4078,11 @@
         <v>0</v>
       </c>
       <c r="F140" t="n">
-        <v>48.66</v>
+        <v>54.09</v>
       </c>
       <c r="G140" t="inlineStr"/>
       <c r="H140" t="n">
-        <v>6.36</v>
+        <v>18.23</v>
       </c>
     </row>
     <row r="141">
@@ -4104,11 +4104,11 @@
         <v>0</v>
       </c>
       <c r="F141" t="n">
-        <v>23.68</v>
+        <v>23.45</v>
       </c>
       <c r="G141" t="inlineStr"/>
       <c r="H141" t="n">
-        <v>-0.46</v>
+        <v>-1.43</v>
       </c>
     </row>
     <row r="142">
@@ -4130,11 +4130,11 @@
         <v>0</v>
       </c>
       <c r="F142" t="n">
-        <v>35.42</v>
+        <v>35.12</v>
       </c>
       <c r="G142" t="inlineStr"/>
       <c r="H142" t="n">
-        <v>-1.99</v>
+        <v>-2.82</v>
       </c>
     </row>
     <row r="143">
@@ -4156,11 +4156,11 @@
         <v>0</v>
       </c>
       <c r="F143" t="n">
-        <v>239.33</v>
+        <v>236</v>
       </c>
       <c r="G143" t="inlineStr"/>
       <c r="H143" t="n">
-        <v>-1.51</v>
+        <v>-2.88</v>
       </c>
     </row>
     <row r="144">
@@ -4182,11 +4182,11 @@
         <v>0</v>
       </c>
       <c r="F144" t="n">
-        <v>401.55</v>
+        <v>406.5</v>
       </c>
       <c r="G144" t="inlineStr"/>
       <c r="H144" t="n">
-        <v>-1.58</v>
+        <v>-0.37</v>
       </c>
     </row>
     <row r="145">
@@ -4208,11 +4208,11 @@
         <v>0</v>
       </c>
       <c r="F145" t="n">
-        <v>484</v>
+        <v>481.5</v>
       </c>
       <c r="G145" t="inlineStr"/>
       <c r="H145" t="n">
-        <v>0.86</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="146">
@@ -4234,11 +4234,11 @@
         <v>0</v>
       </c>
       <c r="F146" t="n">
-        <v>915.3</v>
+        <v>894.45</v>
       </c>
       <c r="G146" t="inlineStr"/>
       <c r="H146" t="n">
-        <v>-1.54</v>
+        <v>-3.79</v>
       </c>
     </row>
     <row r="147">
@@ -4260,11 +4260,11 @@
         <v>0</v>
       </c>
       <c r="F147" t="n">
-        <v>64.58</v>
+        <v>65.73999999999999</v>
       </c>
       <c r="G147" t="inlineStr"/>
       <c r="H147" t="n">
-        <v>-2.15</v>
+        <v>-0.39</v>
       </c>
     </row>
     <row r="148">
@@ -4286,11 +4286,11 @@
         <v>0</v>
       </c>
       <c r="F148" t="n">
-        <v>60.1</v>
+        <v>61.5</v>
       </c>
       <c r="G148" t="inlineStr"/>
       <c r="H148" t="n">
-        <v>-2.95</v>
+        <v>-0.6899999999999999</v>
       </c>
     </row>
     <row r="149">
@@ -4312,11 +4312,11 @@
         <v>0</v>
       </c>
       <c r="F149" t="n">
-        <v>75.34999999999999</v>
+        <v>76.5</v>
       </c>
       <c r="G149" t="inlineStr"/>
       <c r="H149" t="n">
-        <v>-1.63</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="150">
@@ -4338,11 +4338,11 @@
         <v>0</v>
       </c>
       <c r="F150" t="n">
-        <v>30.19</v>
+        <v>29.75</v>
       </c>
       <c r="G150" t="inlineStr"/>
       <c r="H150" t="n">
-        <v>-0.98</v>
+        <v>-2.43</v>
       </c>
     </row>
     <row r="151">
@@ -4364,11 +4364,11 @@
         <v>0</v>
       </c>
       <c r="F151" t="n">
-        <v>225.95</v>
+        <v>220.1</v>
       </c>
       <c r="G151" t="inlineStr"/>
       <c r="H151" t="n">
-        <v>-0.02</v>
+        <v>-2.61</v>
       </c>
     </row>
     <row r="152">
@@ -4390,11 +4390,11 @@
         <v>0</v>
       </c>
       <c r="F152" t="n">
-        <v>1162.4</v>
+        <v>1171.8</v>
       </c>
       <c r="G152" t="inlineStr"/>
       <c r="H152" t="n">
-        <v>-1.32</v>
+        <v>-0.53</v>
       </c>
     </row>
     <row r="153">
@@ -4416,11 +4416,11 @@
         <v>0</v>
       </c>
       <c r="F153" t="n">
-        <v>15.51</v>
+        <v>15.42</v>
       </c>
       <c r="G153" t="inlineStr"/>
       <c r="H153" t="n">
-        <v>-1.77</v>
+        <v>-2.34</v>
       </c>
     </row>
     <row r="154">
@@ -4442,11 +4442,11 @@
         <v>0</v>
       </c>
       <c r="F154" t="n">
-        <v>71.90000000000001</v>
+        <v>72</v>
       </c>
       <c r="G154" t="inlineStr"/>
       <c r="H154" t="n">
-        <v>-0.24</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="155">
@@ -4468,11 +4468,11 @@
         <v>0</v>
       </c>
       <c r="F155" t="n">
-        <v>160</v>
+        <v>161.9</v>
       </c>
       <c r="G155" t="inlineStr"/>
       <c r="H155" t="n">
-        <v>0.01</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="156">
@@ -4494,11 +4494,11 @@
         <v>0</v>
       </c>
       <c r="F156" t="n">
-        <v>142.5</v>
+        <v>144.56</v>
       </c>
       <c r="G156" t="inlineStr"/>
       <c r="H156" t="n">
-        <v>0</v>
+        <v>1.45</v>
       </c>
     </row>
     <row r="157">
@@ -4520,11 +4520,11 @@
         <v>0</v>
       </c>
       <c r="F157" t="n">
-        <v>582.55</v>
+        <v>571.95</v>
       </c>
       <c r="G157" t="inlineStr"/>
       <c r="H157" t="n">
-        <v>-0.42</v>
+        <v>-2.23</v>
       </c>
     </row>
     <row r="158">
@@ -4546,11 +4546,11 @@
         <v>0</v>
       </c>
       <c r="F158" t="n">
-        <v>70.45</v>
+        <v>71.94</v>
       </c>
       <c r="G158" t="inlineStr"/>
       <c r="H158" t="n">
-        <v>-1.88</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="159">
@@ -4572,11 +4572,11 @@
         <v>0</v>
       </c>
       <c r="F159" t="n">
-        <v>2.81</v>
+        <v>2.87</v>
       </c>
       <c r="G159" t="inlineStr"/>
       <c r="H159" t="n">
-        <v>-7.87</v>
+        <v>-5.9</v>
       </c>
     </row>
     <row r="160">
@@ -4598,11 +4598,11 @@
         <v>0</v>
       </c>
       <c r="F160" t="n">
-        <v>6.19</v>
+        <v>6.17</v>
       </c>
       <c r="G160" t="inlineStr"/>
       <c r="H160" t="n">
-        <v>0</v>
+        <v>-0.32</v>
       </c>
     </row>
     <row r="161">
@@ -4624,11 +4624,11 @@
         <v>0</v>
       </c>
       <c r="F161" t="n">
-        <v>12.95</v>
+        <v>11.9</v>
       </c>
       <c r="G161" t="inlineStr"/>
       <c r="H161" t="n">
-        <v>-1.89</v>
+        <v>-9.85</v>
       </c>
     </row>
     <row r="162">
@@ -4650,11 +4650,11 @@
         <v>0</v>
       </c>
       <c r="F162" t="n">
-        <v>334.9</v>
+        <v>320</v>
       </c>
       <c r="G162" t="inlineStr"/>
       <c r="H162" t="n">
-        <v>0.21</v>
+        <v>-4.25</v>
       </c>
     </row>
     <row r="163">
@@ -4676,11 +4676,11 @@
         <v>0</v>
       </c>
       <c r="F163" t="n">
-        <v>186.15</v>
+        <v>187.01</v>
       </c>
       <c r="G163" t="inlineStr"/>
       <c r="H163" t="n">
-        <v>-1.67</v>
+        <v>-1.22</v>
       </c>
     </row>
     <row r="164">
@@ -4702,11 +4702,11 @@
         <v>0</v>
       </c>
       <c r="F164" t="n">
-        <v>7625</v>
+        <v>7460</v>
       </c>
       <c r="G164" t="inlineStr"/>
       <c r="H164" t="n">
-        <v>-1.59</v>
+        <v>-3.72</v>
       </c>
     </row>
     <row r="165">
@@ -4728,11 +4728,11 @@
         <v>0</v>
       </c>
       <c r="F165" t="n">
-        <v>19.6</v>
+        <v>19.11</v>
       </c>
       <c r="G165" t="inlineStr"/>
       <c r="H165" t="n">
-        <v>1.29</v>
+        <v>-1.24</v>
       </c>
     </row>
     <row r="166">
@@ -4754,11 +4754,11 @@
         <v>0</v>
       </c>
       <c r="F166" t="n">
-        <v>217</v>
+        <v>220.02</v>
       </c>
       <c r="G166" t="inlineStr"/>
       <c r="H166" t="n">
-        <v>1.07</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="167">
@@ -4780,11 +4780,11 @@
         <v>0</v>
       </c>
       <c r="F167" t="n">
-        <v>73.52</v>
+        <v>72.5</v>
       </c>
       <c r="G167" t="inlineStr"/>
       <c r="H167" t="n">
-        <v>0.03</v>
+        <v>-1.36</v>
       </c>
     </row>
     <row r="168">
@@ -4806,11 +4806,11 @@
         <v>0</v>
       </c>
       <c r="F168" t="n">
-        <v>916.05</v>
+        <v>910.2</v>
       </c>
       <c r="G168" t="inlineStr"/>
       <c r="H168" t="n">
-        <v>-2.88</v>
+        <v>-3.5</v>
       </c>
     </row>
     <row r="169">
@@ -4832,11 +4832,11 @@
         <v>0</v>
       </c>
       <c r="F169" t="n">
-        <v>18</v>
+        <v>17.8</v>
       </c>
       <c r="G169" t="inlineStr"/>
       <c r="H169" t="n">
-        <v>-0.55</v>
+        <v>-1.66</v>
       </c>
     </row>
     <row r="170">
@@ -4858,11 +4858,11 @@
         <v>0</v>
       </c>
       <c r="F170" t="n">
-        <v>26.21</v>
+        <v>26.27</v>
       </c>
       <c r="G170" t="inlineStr"/>
       <c r="H170" t="n">
-        <v>-0.57</v>
+        <v>-0.34</v>
       </c>
     </row>
     <row r="171">
@@ -4884,11 +4884,11 @@
         <v>0</v>
       </c>
       <c r="F171" t="n">
-        <v>35.73</v>
+        <v>37.7</v>
       </c>
       <c r="G171" t="inlineStr"/>
       <c r="H171" t="n">
-        <v>-5.48</v>
+        <v>-0.26</v>
       </c>
     </row>
     <row r="172">
@@ -4910,11 +4910,11 @@
         <v>0</v>
       </c>
       <c r="F172" t="n">
-        <v>45.5</v>
+        <v>45.3</v>
       </c>
       <c r="G172" t="inlineStr"/>
       <c r="H172" t="n">
-        <v>-1.83</v>
+        <v>-2.27</v>
       </c>
     </row>
     <row r="173">
@@ -4936,11 +4936,11 @@
         <v>0</v>
       </c>
       <c r="F173" t="n">
-        <v>202.5</v>
+        <v>199.45</v>
       </c>
       <c r="G173" t="inlineStr"/>
       <c r="H173" t="n">
-        <v>-1.7</v>
+        <v>-3.18</v>
       </c>
     </row>
     <row r="174">
@@ -4962,11 +4962,11 @@
         <v>0</v>
       </c>
       <c r="F174" t="n">
-        <v>3.36</v>
+        <v>3.26</v>
       </c>
       <c r="G174" t="inlineStr"/>
       <c r="H174" t="n">
-        <v>0.6</v>
+        <v>-2.4</v>
       </c>
     </row>
     <row r="175">
@@ -4988,11 +4988,11 @@
         <v>0</v>
       </c>
       <c r="F175" t="n">
-        <v>75.39</v>
+        <v>75.72</v>
       </c>
       <c r="G175" t="inlineStr"/>
       <c r="H175" t="n">
-        <v>2.07</v>
+        <v>2.52</v>
       </c>
     </row>
     <row r="176">
@@ -5014,11 +5014,11 @@
         <v>0</v>
       </c>
       <c r="F176" t="n">
-        <v>4.85</v>
+        <v>4.88</v>
       </c>
       <c r="G176" t="inlineStr"/>
       <c r="H176" t="n">
-        <v>-3.19</v>
+        <v>-2.59</v>
       </c>
     </row>
     <row r="177">
@@ -5040,11 +5040,11 @@
         <v>0</v>
       </c>
       <c r="F177" t="n">
-        <v>35.2</v>
+        <v>37.2</v>
       </c>
       <c r="G177" t="inlineStr"/>
       <c r="H177" t="n">
-        <v>-0.79</v>
+        <v>4.85</v>
       </c>
     </row>
     <row r="178">
@@ -5066,11 +5066,11 @@
         <v>0</v>
       </c>
       <c r="F178" t="n">
-        <v>43.09</v>
+        <v>43</v>
       </c>
       <c r="G178" t="inlineStr"/>
       <c r="H178" t="n">
-        <v>-2.62</v>
+        <v>-2.82</v>
       </c>
     </row>
     <row r="179">
@@ -5092,11 +5092,11 @@
         <v>0</v>
       </c>
       <c r="F179" t="n">
-        <v>38.37</v>
+        <v>38.7</v>
       </c>
       <c r="G179" t="inlineStr"/>
       <c r="H179" t="n">
-        <v>-1.11</v>
+        <v>-0.26</v>
       </c>
     </row>
     <row r="180">
@@ -5118,11 +5118,11 @@
         <v>0</v>
       </c>
       <c r="F180" t="n">
-        <v>117.22</v>
+        <v>116.5</v>
       </c>
       <c r="G180" t="inlineStr"/>
       <c r="H180" t="n">
-        <v>0.58</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="181">
@@ -5144,11 +5144,11 @@
         <v>0</v>
       </c>
       <c r="F181" t="n">
-        <v>229.2</v>
+        <v>227</v>
       </c>
       <c r="G181" t="inlineStr"/>
       <c r="H181" t="n">
-        <v>-3.7</v>
+        <v>-4.62</v>
       </c>
     </row>
     <row r="182">
@@ -5170,11 +5170,11 @@
         <v>0</v>
       </c>
       <c r="F182" t="n">
-        <v>142.09</v>
+        <v>141.45</v>
       </c>
       <c r="G182" t="inlineStr"/>
       <c r="H182" t="n">
-        <v>-0.64</v>
+        <v>-1.08</v>
       </c>
     </row>
     <row r="183">
@@ -5196,11 +5196,11 @@
         <v>0</v>
       </c>
       <c r="F183" t="n">
-        <v>241.85</v>
+        <v>239.4</v>
       </c>
       <c r="G183" t="inlineStr"/>
       <c r="H183" t="n">
-        <v>0</v>
+        <v>-1.01</v>
       </c>
     </row>
     <row r="184">
@@ -5222,11 +5222,11 @@
         <v>0</v>
       </c>
       <c r="F184" t="n">
-        <v>17.37</v>
+        <v>17.23</v>
       </c>
       <c r="G184" t="inlineStr"/>
       <c r="H184" t="n">
-        <v>-0.97</v>
+        <v>-1.77</v>
       </c>
     </row>
     <row r="185">
@@ -5248,11 +5248,11 @@
         <v>0</v>
       </c>
       <c r="F185" t="n">
-        <v>812</v>
+        <v>807.4</v>
       </c>
       <c r="G185" t="inlineStr"/>
       <c r="H185" t="n">
-        <v>-2.04</v>
+        <v>-2.59</v>
       </c>
     </row>
     <row r="186">
@@ -5274,11 +5274,11 @@
         <v>0</v>
       </c>
       <c r="F186" t="n">
-        <v>44.4</v>
+        <v>42.61</v>
       </c>
       <c r="G186" t="inlineStr"/>
       <c r="H186" t="n">
-        <v>0.95</v>
+        <v>-3.12</v>
       </c>
     </row>
     <row r="187">
@@ -5300,11 +5300,11 @@
         <v>0</v>
       </c>
       <c r="F187" t="n">
-        <v>1.78</v>
+        <v>1.79</v>
       </c>
       <c r="G187" t="inlineStr"/>
       <c r="H187" t="n">
-        <v>-0.5600000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188">
@@ -5326,11 +5326,11 @@
         <v>0</v>
       </c>
       <c r="F188" t="n">
-        <v>355</v>
+        <v>354.9</v>
       </c>
       <c r="G188" t="inlineStr"/>
       <c r="H188" t="n">
-        <v>-1.66</v>
+        <v>-1.69</v>
       </c>
     </row>
     <row r="189">
@@ -5352,11 +5352,11 @@
         <v>0</v>
       </c>
       <c r="F189" t="n">
-        <v>127.82</v>
+        <v>126.43</v>
       </c>
       <c r="G189" t="inlineStr"/>
       <c r="H189" t="n">
-        <v>-1.2</v>
+        <v>-2.27</v>
       </c>
     </row>
     <row r="190">
@@ -5378,11 +5378,11 @@
         <v>0</v>
       </c>
       <c r="F190" t="n">
-        <v>64.94</v>
+        <v>64.40000000000001</v>
       </c>
       <c r="G190" t="inlineStr"/>
       <c r="H190" t="n">
-        <v>-1.16</v>
+        <v>-1.98</v>
       </c>
     </row>
     <row r="191">
@@ -5404,11 +5404,11 @@
         <v>0</v>
       </c>
       <c r="F191" t="n">
-        <v>699.9</v>
+        <v>691.9</v>
       </c>
       <c r="G191" t="inlineStr"/>
       <c r="H191" t="n">
-        <v>-1.42</v>
+        <v>-2.55</v>
       </c>
     </row>
     <row r="192">
@@ -5430,11 +5430,11 @@
         <v>0</v>
       </c>
       <c r="F192" t="n">
-        <v>7.41</v>
+        <v>7.44</v>
       </c>
       <c r="G192" t="inlineStr"/>
       <c r="H192" t="n">
-        <v>-1.07</v>
+        <v>-0.67</v>
       </c>
     </row>
     <row r="193">
@@ -5456,11 +5456,11 @@
         <v>0</v>
       </c>
       <c r="F193" t="n">
-        <v>315</v>
+        <v>313.75</v>
       </c>
       <c r="G193" t="inlineStr"/>
       <c r="H193" t="n">
-        <v>0.32</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="194">
@@ -5482,11 +5482,11 @@
         <v>0</v>
       </c>
       <c r="F194" t="n">
-        <v>989.1</v>
+        <v>983</v>
       </c>
       <c r="G194" t="inlineStr"/>
       <c r="H194" t="n">
-        <v>-0.99</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="195">
@@ -5508,11 +5508,11 @@
         <v>0</v>
       </c>
       <c r="F195" t="n">
-        <v>269.65</v>
+        <v>266</v>
       </c>
       <c r="G195" t="inlineStr"/>
       <c r="H195" t="n">
-        <v>-1.55</v>
+        <v>-2.88</v>
       </c>
     </row>
     <row r="196">
@@ -5534,11 +5534,11 @@
         <v>0</v>
       </c>
       <c r="F196" t="n">
-        <v>136.98</v>
+        <v>134.04</v>
       </c>
       <c r="G196" t="inlineStr"/>
       <c r="H196" t="n">
-        <v>0.87</v>
+        <v>-1.3</v>
       </c>
     </row>
     <row r="197">
@@ -5560,11 +5560,11 @@
         <v>0</v>
       </c>
       <c r="F197" t="n">
-        <v>353.05</v>
+        <v>357.5</v>
       </c>
       <c r="G197" t="inlineStr"/>
       <c r="H197" t="n">
-        <v>-1.36</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="198">
@@ -5586,11 +5586,11 @@
         <v>0</v>
       </c>
       <c r="F198" t="n">
-        <v>572</v>
+        <v>575.5</v>
       </c>
       <c r="G198" t="inlineStr"/>
       <c r="H198" t="n">
-        <v>-2.19</v>
+        <v>-1.59</v>
       </c>
     </row>
     <row r="199">
@@ -5612,11 +5612,11 @@
         <v>0</v>
       </c>
       <c r="F199" t="n">
-        <v>150.74</v>
+        <v>150.1</v>
       </c>
       <c r="G199" t="inlineStr"/>
       <c r="H199" t="n">
-        <v>-0.83</v>
+        <v>-1.25</v>
       </c>
     </row>
     <row r="200">
@@ -5638,11 +5638,11 @@
         <v>0</v>
       </c>
       <c r="F200" t="n">
-        <v>417.9</v>
+        <v>413</v>
       </c>
       <c r="G200" t="inlineStr"/>
       <c r="H200" t="n">
-        <v>-1.6</v>
+        <v>-2.75</v>
       </c>
     </row>
     <row r="201">
@@ -5664,11 +5664,11 @@
         <v>0</v>
       </c>
       <c r="F201" t="n">
-        <v>447.05</v>
+        <v>446</v>
       </c>
       <c r="G201" t="inlineStr"/>
       <c r="H201" t="n">
-        <v>-0.96</v>
+        <v>-1.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto: update momentum data - 2026-01-26 04:46 UTC
</commit_message>
<xml_diff>
--- a/data/trending_momentum_stocks.xlsx
+++ b/data/trending_momentum_stocks.xlsx
@@ -482,11 +482,11 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>8.26</v>
+        <v>8.279999999999999</v>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
-        <v>4.56</v>
+        <v>4.81</v>
       </c>
     </row>
     <row r="3">
@@ -508,11 +508,11 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>11.08</v>
+        <v>11.24</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
-        <v>-8.130000000000001</v>
+        <v>-6.8</v>
       </c>
     </row>
     <row r="4">
@@ -534,11 +534,11 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
-        <v>-3.09</v>
+        <v>-11.61</v>
       </c>
     </row>
     <row r="5">
@@ -560,11 +560,11 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>156.4</v>
+        <v>148.1</v>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
-        <v>3.64</v>
+        <v>-1.86</v>
       </c>
     </row>
     <row r="6">
@@ -586,11 +586,11 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>79.5</v>
+        <v>82.95</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
-        <v>-7.02</v>
+        <v>-2.98</v>
       </c>
     </row>
     <row r="7">
@@ -612,11 +612,11 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>27.75</v>
+        <v>26.07</v>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
-        <v>-0.18</v>
+        <v>-6.22</v>
       </c>
     </row>
     <row r="8">
@@ -638,11 +638,11 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>17.36</v>
+        <v>17.15</v>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
-        <v>-1.75</v>
+        <v>-2.94</v>
       </c>
     </row>
     <row r="9">
@@ -664,11 +664,11 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>174.42</v>
+        <v>174.33</v>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
-        <v>-5.72</v>
+        <v>-5.77</v>
       </c>
     </row>
     <row r="10">
@@ -690,11 +690,11 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>192.57</v>
+        <v>185.66</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
-        <v>-3.17</v>
+        <v>-6.65</v>
       </c>
     </row>
     <row r="11">
@@ -716,11 +716,11 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>30.2</v>
+        <v>29.5</v>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="n">
-        <v>-7.65</v>
+        <v>-9.789999999999999</v>
       </c>
     </row>
     <row r="12">
@@ -742,11 +742,11 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>495.9</v>
+        <v>524.3</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="n">
-        <v>6.19</v>
+        <v>12.27</v>
       </c>
     </row>
     <row r="13">
@@ -768,11 +768,11 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>24.11</v>
+        <v>24.23</v>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
-        <v>-1.19</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="14">
@@ -794,11 +794,11 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>107.96</v>
+        <v>106.9</v>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="n">
-        <v>-2.74</v>
+        <v>-3.69</v>
       </c>
     </row>
     <row r="15">
@@ -820,11 +820,11 @@
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>6.34</v>
+        <v>6.15</v>
       </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="n">
-        <v>-1.55</v>
+        <v>-4.5</v>
       </c>
     </row>
     <row r="16">
@@ -846,11 +846,11 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>147.07</v>
+        <v>148.6</v>
       </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="n">
-        <v>-2.08</v>
+        <v>-1.07</v>
       </c>
     </row>
     <row r="17">
@@ -872,11 +872,11 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>4.63</v>
+        <v>4.43</v>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="n">
-        <v>-1.28</v>
+        <v>-5.54</v>
       </c>
     </row>
     <row r="18">
@@ -898,11 +898,11 @@
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>12.38</v>
+        <v>12.4</v>
       </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="n">
-        <v>-4.25</v>
+        <v>-4.1</v>
       </c>
     </row>
     <row r="19">
@@ -924,11 +924,11 @@
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>7.62</v>
+        <v>8</v>
       </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="n">
-        <v>-2.31</v>
+        <v>2.56</v>
       </c>
     </row>
     <row r="20">
@@ -950,11 +950,11 @@
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>339</v>
+        <v>340.9</v>
       </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="n">
-        <v>-0.88</v>
+        <v>-0.32</v>
       </c>
     </row>
     <row r="21">
@@ -976,11 +976,11 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>241.45</v>
+        <v>238</v>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
-        <v>-4.94</v>
+        <v>-6.3</v>
       </c>
     </row>
     <row r="22">
@@ -1002,11 +1002,11 @@
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>500.55</v>
+        <v>472.95</v>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="n">
-        <v>6.27</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="23">
@@ -1028,11 +1028,11 @@
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>4</v>
+        <v>4.14</v>
       </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="n">
-        <v>-4.53</v>
+        <v>-1.19</v>
       </c>
     </row>
     <row r="24">
@@ -1080,11 +1080,11 @@
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>7.58</v>
+        <v>7.66</v>
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="n">
-        <v>-7.56</v>
+        <v>-6.59</v>
       </c>
     </row>
     <row r="26">
@@ -1158,11 +1158,11 @@
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>17.33</v>
+        <v>17.22</v>
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="n">
-        <v>0</v>
+        <v>-0.63</v>
       </c>
     </row>
     <row r="29">
@@ -1210,11 +1210,11 @@
         <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>443.3</v>
+        <v>441.35</v>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="n">
-        <v>0.08</v>
+        <v>-0.36</v>
       </c>
     </row>
     <row r="31">
@@ -1236,11 +1236,11 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>73.34999999999999</v>
+        <v>73</v>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="n">
-        <v>-3.42</v>
+        <v>-3.88</v>
       </c>
     </row>
     <row r="32">
@@ -1262,11 +1262,11 @@
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>7.4</v>
+        <v>7.2</v>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="n">
-        <v>-0.27</v>
+        <v>-2.96</v>
       </c>
     </row>
     <row r="33">
@@ -1288,11 +1288,11 @@
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="n">
-        <v>-4.55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1314,11 +1314,11 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>35.1</v>
+        <v>35.19</v>
       </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="n">
-        <v>-4.62</v>
+        <v>-4.37</v>
       </c>
     </row>
     <row r="35">
@@ -1366,11 +1366,11 @@
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>5.82</v>
+        <v>5.93</v>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="n">
-        <v>-5.06</v>
+        <v>-3.26</v>
       </c>
     </row>
     <row r="37">
@@ -1392,11 +1392,11 @@
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>116.78</v>
+        <v>112</v>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="n">
-        <v>-1.86</v>
+        <v>-5.87</v>
       </c>
     </row>
     <row r="38">
@@ -1444,11 +1444,11 @@
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>72.36</v>
+        <v>68.56</v>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="n">
-        <v>-3.39</v>
+        <v>-8.460000000000001</v>
       </c>
     </row>
     <row r="40">
@@ -1470,11 +1470,11 @@
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>441.65</v>
+        <v>426.6</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="n">
-        <v>-2.93</v>
+        <v>-6.24</v>
       </c>
     </row>
     <row r="41">
@@ -1496,11 +1496,11 @@
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>1.58</v>
+        <v>1.67</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="n">
-        <v>-4.24</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="42">
@@ -1522,11 +1522,11 @@
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>133.07</v>
+        <v>135.5</v>
       </c>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="n">
-        <v>-4.26</v>
+        <v>-2.51</v>
       </c>
     </row>
     <row r="43">
@@ -1548,11 +1548,11 @@
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>122.17</v>
+        <v>122.18</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="n">
-        <v>0.59</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="44">
@@ -1574,11 +1574,11 @@
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>20.58</v>
+        <v>19.94</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="n">
-        <v>-1.06</v>
+        <v>-4.13</v>
       </c>
     </row>
     <row r="45">
@@ -1600,11 +1600,11 @@
         <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>0.95</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="n">
-        <v>-3.06</v>
+        <v>-4.08</v>
       </c>
     </row>
     <row r="46">
@@ -1626,11 +1626,11 @@
         <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>9.57</v>
+        <v>9.449999999999999</v>
       </c>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="n">
-        <v>-0.21</v>
+        <v>-1.46</v>
       </c>
     </row>
     <row r="47">
@@ -1652,11 +1652,11 @@
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>12.62</v>
+        <v>12.2</v>
       </c>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="n">
-        <v>-2.47</v>
+        <v>-5.72</v>
       </c>
     </row>
     <row r="48">
@@ -1678,11 +1678,11 @@
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>28.31</v>
+        <v>27.26</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="n">
-        <v>-1.87</v>
+        <v>-5.51</v>
       </c>
     </row>
     <row r="49">
@@ -1730,11 +1730,11 @@
         <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>1195</v>
+        <v>1179.1</v>
       </c>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="n">
-        <v>-4.4</v>
+        <v>-5.67</v>
       </c>
     </row>
     <row r="51">
@@ -1756,11 +1756,11 @@
         <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>36.94</v>
+        <v>36.3</v>
       </c>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="n">
-        <v>-3.27</v>
+        <v>-4.95</v>
       </c>
     </row>
     <row r="52">
@@ -1808,11 +1808,11 @@
         <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="n">
-        <v>-3.3</v>
+        <v>-3.78</v>
       </c>
     </row>
     <row r="54">
@@ -1834,11 +1834,11 @@
         <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>699.85</v>
+        <v>697</v>
       </c>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="n">
-        <v>0.7</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="55">
@@ -1860,11 +1860,11 @@
         <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>3.89</v>
+        <v>3.8</v>
       </c>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="n">
-        <v>-1.52</v>
+        <v>-3.8</v>
       </c>
     </row>
     <row r="56">
@@ -1886,11 +1886,11 @@
         <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>275.85</v>
+        <v>270.2</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="n">
-        <v>-3.21</v>
+        <v>-5.19</v>
       </c>
     </row>
     <row r="57">
@@ -1912,11 +1912,11 @@
         <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>17.65</v>
+        <v>17.6</v>
       </c>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="n">
-        <v>1.15</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="58">
@@ -1938,11 +1938,11 @@
         <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>147.5</v>
+        <v>145</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="n">
-        <v>-1.67</v>
+        <v>-3.33</v>
       </c>
     </row>
     <row r="59">
@@ -1964,11 +1964,11 @@
         <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>3.17</v>
+        <v>3.29</v>
       </c>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="n">
-        <v>-3.94</v>
+        <v>-0.3</v>
       </c>
     </row>
     <row r="60">
@@ -1990,11 +1990,11 @@
         <v>0</v>
       </c>
       <c r="F60" t="n">
-        <v>643.9</v>
+        <v>700</v>
       </c>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="n">
-        <v>-7.99</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="61">
@@ -2016,11 +2016,11 @@
         <v>0</v>
       </c>
       <c r="F61" t="n">
-        <v>163</v>
+        <v>162.2</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="n">
-        <v>-1.81</v>
+        <v>-2.29</v>
       </c>
     </row>
     <row r="62">
@@ -2042,11 +2042,11 @@
         <v>0</v>
       </c>
       <c r="F62" t="n">
-        <v>10.88</v>
+        <v>11.01</v>
       </c>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="n">
-        <v>-1.09</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="63">
@@ -2068,11 +2068,11 @@
         <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="n">
-        <v>-3.04</v>
+        <v>-3.84</v>
       </c>
     </row>
     <row r="64">
@@ -2094,11 +2094,11 @@
         <v>0</v>
       </c>
       <c r="F64" t="n">
-        <v>2.63</v>
+        <v>2.66</v>
       </c>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="n">
-        <v>-7.07</v>
+        <v>-6.01</v>
       </c>
     </row>
     <row r="65">
@@ -2146,11 +2146,11 @@
         <v>0</v>
       </c>
       <c r="F66" t="n">
-        <v>4.88</v>
+        <v>4.7</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="n">
-        <v>0.83</v>
+        <v>-2.89</v>
       </c>
     </row>
     <row r="67">
@@ -2172,11 +2172,11 @@
         <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>105</v>
+        <v>103.6</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="n">
-        <v>-3.67</v>
+        <v>-4.95</v>
       </c>
     </row>
     <row r="68">
@@ -2198,11 +2198,11 @@
         <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>797</v>
+        <v>780</v>
       </c>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="n">
-        <v>-0.62</v>
+        <v>-2.74</v>
       </c>
     </row>
     <row r="69">
@@ -2224,11 +2224,11 @@
         <v>0</v>
       </c>
       <c r="F69" t="n">
-        <v>17.8</v>
+        <v>17.25</v>
       </c>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="n">
-        <v>-2.63</v>
+        <v>-5.63</v>
       </c>
     </row>
     <row r="70">
@@ -2250,11 +2250,11 @@
         <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>1.41</v>
+        <v>1.4</v>
       </c>
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="n">
-        <v>-4.08</v>
+        <v>-4.76</v>
       </c>
     </row>
     <row r="71">
@@ -2276,11 +2276,11 @@
         <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>1156.2</v>
+        <v>1144.9</v>
       </c>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="n">
-        <v>1.44</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="72">
@@ -2302,11 +2302,11 @@
         <v>0</v>
       </c>
       <c r="F72" t="n">
-        <v>417.5</v>
+        <v>413</v>
       </c>
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="n">
-        <v>3.09</v>
+        <v>1.98</v>
       </c>
     </row>
     <row r="73">
@@ -2328,11 +2328,11 @@
         <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>96</v>
+        <v>94.95</v>
       </c>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="n">
-        <v>-3.99</v>
+        <v>-5.04</v>
       </c>
     </row>
     <row r="74">
@@ -2354,11 +2354,11 @@
         <v>0</v>
       </c>
       <c r="F74" t="n">
-        <v>52.28</v>
+        <v>51.11</v>
       </c>
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="n">
-        <v>-1.34</v>
+        <v>-3.55</v>
       </c>
     </row>
     <row r="75">
@@ -2380,11 +2380,11 @@
         <v>0</v>
       </c>
       <c r="F75" t="n">
-        <v>8.619999999999999</v>
+        <v>8.25</v>
       </c>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="n">
-        <v>-2.82</v>
+        <v>-6.99</v>
       </c>
     </row>
     <row r="76">
@@ -2406,11 +2406,11 @@
         <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>38.43</v>
+        <v>37.5</v>
       </c>
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="n">
-        <v>-3.78</v>
+        <v>-6.11</v>
       </c>
     </row>
     <row r="77">
@@ -2432,11 +2432,11 @@
         <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>396.95</v>
+        <v>394</v>
       </c>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="n">
-        <v>-6.38</v>
+        <v>-7.08</v>
       </c>
     </row>
     <row r="78">
@@ -2458,11 +2458,11 @@
         <v>0</v>
       </c>
       <c r="F78" t="n">
-        <v>147.37</v>
+        <v>149.07</v>
       </c>
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="n">
-        <v>-2.4</v>
+        <v>-1.28</v>
       </c>
     </row>
     <row r="79">
@@ -2484,11 +2484,11 @@
         <v>0</v>
       </c>
       <c r="F79" t="n">
-        <v>8.91</v>
+        <v>9.08</v>
       </c>
       <c r="G79" t="inlineStr"/>
       <c r="H79" t="n">
-        <v>-3.68</v>
+        <v>-1.84</v>
       </c>
     </row>
     <row r="80">
@@ -2510,11 +2510,11 @@
         <v>0</v>
       </c>
       <c r="F80" t="n">
-        <v>53.49</v>
+        <v>54.99</v>
       </c>
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="n">
-        <v>-2.55</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="81">
@@ -2536,11 +2536,11 @@
         <v>0</v>
       </c>
       <c r="F81" t="n">
-        <v>8</v>
+        <v>7.69</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="n">
-        <v>-4.31</v>
+        <v>-8.01</v>
       </c>
     </row>
     <row r="82">
@@ -2562,11 +2562,11 @@
         <v>0</v>
       </c>
       <c r="F82" t="n">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="n">
-        <v>0</v>
+        <v>-3.23</v>
       </c>
     </row>
     <row r="83">
@@ -2588,11 +2588,11 @@
         <v>0</v>
       </c>
       <c r="F83" t="n">
-        <v>9.779999999999999</v>
+        <v>10</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="n">
-        <v>-2.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -2614,11 +2614,11 @@
         <v>0</v>
       </c>
       <c r="F84" t="n">
-        <v>4.91</v>
+        <v>4.94</v>
       </c>
       <c r="G84" t="inlineStr"/>
       <c r="H84" t="n">
-        <v>-3.73</v>
+        <v>-3.14</v>
       </c>
     </row>
     <row r="85">
@@ -2640,11 +2640,11 @@
         <v>0</v>
       </c>
       <c r="F85" t="n">
-        <v>171.93</v>
+        <v>171</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="n">
-        <v>-0.62</v>
+        <v>-1.16</v>
       </c>
     </row>
     <row r="86">
@@ -2666,11 +2666,11 @@
         <v>0</v>
       </c>
       <c r="F86" t="n">
-        <v>960.7</v>
+        <v>950</v>
       </c>
       <c r="G86" t="inlineStr"/>
       <c r="H86" t="n">
-        <v>-1.46</v>
+        <v>-2.56</v>
       </c>
     </row>
     <row r="87">
@@ -2692,11 +2692,11 @@
         <v>0</v>
       </c>
       <c r="F87" t="n">
-        <v>186.52</v>
+        <v>170</v>
       </c>
       <c r="G87" t="inlineStr"/>
       <c r="H87" t="n">
-        <v>-1.31</v>
+        <v>-10.05</v>
       </c>
     </row>
     <row r="88">
@@ -2718,11 +2718,11 @@
         <v>0</v>
       </c>
       <c r="F88" t="n">
-        <v>610</v>
+        <v>591</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="n">
-        <v>-4.39</v>
+        <v>-7.37</v>
       </c>
     </row>
     <row r="89">
@@ -2744,11 +2744,11 @@
         <v>0</v>
       </c>
       <c r="F89" t="n">
-        <v>840.35</v>
+        <v>808.95</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="n">
-        <v>-8.949999999999999</v>
+        <v>-12.36</v>
       </c>
     </row>
     <row r="90">
@@ -2770,11 +2770,11 @@
         <v>0</v>
       </c>
       <c r="F90" t="n">
-        <v>15.53</v>
+        <v>15.42</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="n">
-        <v>-4.72</v>
+        <v>-5.4</v>
       </c>
     </row>
     <row r="91">
@@ -2796,11 +2796,11 @@
         <v>0</v>
       </c>
       <c r="F91" t="n">
-        <v>27.9</v>
+        <v>26.85</v>
       </c>
       <c r="G91" t="inlineStr"/>
       <c r="H91" t="n">
-        <v>-2.17</v>
+        <v>-5.86</v>
       </c>
     </row>
     <row r="92">
@@ -2822,11 +2822,11 @@
         <v>0</v>
       </c>
       <c r="F92" t="n">
-        <v>29.27</v>
+        <v>29.58</v>
       </c>
       <c r="G92" t="inlineStr"/>
       <c r="H92" t="n">
-        <v>-1.78</v>
+        <v>-0.74</v>
       </c>
     </row>
     <row r="93">
@@ -2848,11 +2848,11 @@
         <v>0</v>
       </c>
       <c r="F93" t="n">
-        <v>1.63</v>
+        <v>1.62</v>
       </c>
       <c r="G93" t="inlineStr"/>
       <c r="H93" t="n">
-        <v>-1.21</v>
+        <v>-1.82</v>
       </c>
     </row>
     <row r="94">
@@ -2874,11 +2874,11 @@
         <v>0</v>
       </c>
       <c r="F94" t="n">
-        <v>715</v>
+        <v>721</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="n">
-        <v>0.03</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="95">
@@ -2900,11 +2900,11 @@
         <v>0</v>
       </c>
       <c r="F95" t="n">
-        <v>14.91</v>
+        <v>14.8</v>
       </c>
       <c r="G95" t="inlineStr"/>
       <c r="H95" t="n">
-        <v>-3.5</v>
+        <v>-4.21</v>
       </c>
     </row>
     <row r="96">
@@ -2926,11 +2926,11 @@
         <v>0</v>
       </c>
       <c r="F96" t="n">
-        <v>6.53</v>
+        <v>6.56</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="n">
-        <v>1.4</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="97">
@@ -2952,11 +2952,11 @@
         <v>0</v>
       </c>
       <c r="F97" t="n">
-        <v>11.69</v>
+        <v>11.46</v>
       </c>
       <c r="G97" t="inlineStr"/>
       <c r="H97" t="n">
-        <v>-1.68</v>
+        <v>-3.62</v>
       </c>
     </row>
     <row r="98">
@@ -3030,11 +3030,11 @@
         <v>0</v>
       </c>
       <c r="F100" t="n">
-        <v>105.75</v>
+        <v>105.2</v>
       </c>
       <c r="G100" t="inlineStr"/>
       <c r="H100" t="n">
-        <v>0.71</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="101">
@@ -3056,11 +3056,11 @@
         <v>0</v>
       </c>
       <c r="F101" t="n">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="G101" t="inlineStr"/>
       <c r="H101" t="n">
-        <v>-1.19</v>
+        <v>-2.99</v>
       </c>
     </row>
     <row r="102">
@@ -3082,11 +3082,11 @@
         <v>0</v>
       </c>
       <c r="F102" t="n">
-        <v>90.53</v>
+        <v>89.40000000000001</v>
       </c>
       <c r="G102" t="inlineStr"/>
       <c r="H102" t="n">
-        <v>-2.14</v>
+        <v>-3.36</v>
       </c>
     </row>
     <row r="103">
@@ -3108,11 +3108,11 @@
         <v>0</v>
       </c>
       <c r="F103" t="n">
-        <v>899.05</v>
+        <v>877.5</v>
       </c>
       <c r="G103" t="inlineStr"/>
       <c r="H103" t="n">
-        <v>1.36</v>
+        <v>-1.07</v>
       </c>
     </row>
     <row r="104">
@@ -3134,11 +3134,11 @@
         <v>0</v>
       </c>
       <c r="F104" t="n">
-        <v>301</v>
+        <v>298.5</v>
       </c>
       <c r="G104" t="inlineStr"/>
       <c r="H104" t="n">
-        <v>-4.64</v>
+        <v>-5.43</v>
       </c>
     </row>
     <row r="105">
@@ -3160,11 +3160,11 @@
         <v>0</v>
       </c>
       <c r="F105" t="n">
-        <v>163</v>
+        <v>164.8</v>
       </c>
       <c r="G105" t="inlineStr"/>
       <c r="H105" t="n">
-        <v>-2.4</v>
+        <v>-1.32</v>
       </c>
     </row>
     <row r="106">
@@ -3186,11 +3186,11 @@
         <v>0</v>
       </c>
       <c r="F106" t="n">
-        <v>81.63</v>
+        <v>80.97</v>
       </c>
       <c r="G106" t="inlineStr"/>
       <c r="H106" t="n">
-        <v>-2.24</v>
+        <v>-3.03</v>
       </c>
     </row>
     <row r="107">
@@ -3212,11 +3212,11 @@
         <v>0</v>
       </c>
       <c r="F107" t="n">
-        <v>32.17</v>
+        <v>31.48</v>
       </c>
       <c r="G107" t="inlineStr"/>
       <c r="H107" t="n">
-        <v>-2.52</v>
+        <v>-4.61</v>
       </c>
     </row>
     <row r="108">
@@ -3238,11 +3238,11 @@
         <v>0</v>
       </c>
       <c r="F108" t="n">
-        <v>26</v>
+        <v>25.09</v>
       </c>
       <c r="G108" t="inlineStr"/>
       <c r="H108" t="n">
-        <v>-1.81</v>
+        <v>-5.25</v>
       </c>
     </row>
     <row r="109">
@@ -3264,11 +3264,11 @@
         <v>0</v>
       </c>
       <c r="F109" t="n">
-        <v>66.73</v>
+        <v>66.88</v>
       </c>
       <c r="G109" t="inlineStr"/>
       <c r="H109" t="n">
-        <v>-0.99</v>
+        <v>-0.77</v>
       </c>
     </row>
     <row r="110">
@@ -3290,11 +3290,11 @@
         <v>0</v>
       </c>
       <c r="F110" t="n">
-        <v>177</v>
+        <v>176.49</v>
       </c>
       <c r="G110" t="inlineStr"/>
       <c r="H110" t="n">
-        <v>-1.12</v>
+        <v>-1.4</v>
       </c>
     </row>
     <row r="111">
@@ -3316,11 +3316,11 @@
         <v>0</v>
       </c>
       <c r="F111" t="n">
-        <v>4.22</v>
+        <v>4.21</v>
       </c>
       <c r="G111" t="inlineStr"/>
       <c r="H111" t="n">
-        <v>-1.63</v>
+        <v>-1.86</v>
       </c>
     </row>
     <row r="112">
@@ -3342,11 +3342,11 @@
         <v>0</v>
       </c>
       <c r="F112" t="n">
-        <v>307.45</v>
+        <v>298</v>
       </c>
       <c r="G112" t="inlineStr"/>
       <c r="H112" t="n">
-        <v>0.65</v>
+        <v>-2.44</v>
       </c>
     </row>
     <row r="113">
@@ -3368,11 +3368,11 @@
         <v>0</v>
       </c>
       <c r="F113" t="n">
-        <v>168.51</v>
+        <v>165</v>
       </c>
       <c r="G113" t="inlineStr"/>
       <c r="H113" t="n">
-        <v>-0.87</v>
+        <v>-2.94</v>
       </c>
     </row>
     <row r="114">
@@ -3394,11 +3394,11 @@
         <v>0</v>
       </c>
       <c r="F114" t="n">
-        <v>22.79</v>
+        <v>23</v>
       </c>
       <c r="G114" t="inlineStr"/>
       <c r="H114" t="n">
-        <v>0.22</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="115">
@@ -3420,11 +3420,11 @@
         <v>0</v>
       </c>
       <c r="F115" t="n">
-        <v>386</v>
+        <v>368</v>
       </c>
       <c r="G115" t="inlineStr"/>
       <c r="H115" t="n">
-        <v>-1.78</v>
+        <v>-6.36</v>
       </c>
     </row>
     <row r="116">
@@ -3446,11 +3446,11 @@
         <v>0</v>
       </c>
       <c r="F116" t="n">
-        <v>139.5</v>
+        <v>144</v>
       </c>
       <c r="G116" t="inlineStr"/>
       <c r="H116" t="n">
-        <v>-2.11</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="117">
@@ -3472,11 +3472,11 @@
         <v>0</v>
       </c>
       <c r="F117" t="n">
-        <v>24.71</v>
+        <v>24.58</v>
       </c>
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="n">
-        <v>-3.02</v>
+        <v>-3.53</v>
       </c>
     </row>
     <row r="118">
@@ -3498,11 +3498,11 @@
         <v>0</v>
       </c>
       <c r="F118" t="n">
-        <v>100.41</v>
+        <v>98.2</v>
       </c>
       <c r="G118" t="inlineStr"/>
       <c r="H118" t="n">
-        <v>-1.85</v>
+        <v>-4.01</v>
       </c>
     </row>
     <row r="119">
@@ -3524,11 +3524,11 @@
         <v>0</v>
       </c>
       <c r="F119" t="n">
-        <v>91.5</v>
+        <v>95.76000000000001</v>
       </c>
       <c r="G119" t="inlineStr"/>
       <c r="H119" t="n">
-        <v>11.59</v>
+        <v>16.78</v>
       </c>
     </row>
     <row r="120">
@@ -3550,11 +3550,11 @@
         <v>0</v>
       </c>
       <c r="F120" t="n">
-        <v>10.05</v>
+        <v>9.93</v>
       </c>
       <c r="G120" t="inlineStr"/>
       <c r="H120" t="n">
-        <v>-4.19</v>
+        <v>-5.34</v>
       </c>
     </row>
     <row r="121">
@@ -3576,11 +3576,11 @@
         <v>0</v>
       </c>
       <c r="F121" t="n">
-        <v>29.36</v>
+        <v>28.1</v>
       </c>
       <c r="G121" t="inlineStr"/>
       <c r="H121" t="n">
-        <v>-1.48</v>
+        <v>-5.7</v>
       </c>
     </row>
     <row r="122">
@@ -3602,11 +3602,11 @@
         <v>0</v>
       </c>
       <c r="F122" t="n">
-        <v>77.84999999999999</v>
+        <v>72.98999999999999</v>
       </c>
       <c r="G122" t="inlineStr"/>
       <c r="H122" t="n">
-        <v>-1.77</v>
+        <v>-7.9</v>
       </c>
     </row>
     <row r="123">
@@ -3628,11 +3628,11 @@
         <v>0</v>
       </c>
       <c r="F123" t="n">
-        <v>4.94</v>
+        <v>4.8</v>
       </c>
       <c r="G123" t="inlineStr"/>
       <c r="H123" t="n">
-        <v>0.2</v>
+        <v>-2.64</v>
       </c>
     </row>
     <row r="124">
@@ -3654,11 +3654,11 @@
         <v>0</v>
       </c>
       <c r="F124" t="n">
-        <v>37.19</v>
+        <v>37.88</v>
       </c>
       <c r="G124" t="inlineStr"/>
       <c r="H124" t="n">
-        <v>-2</v>
+        <v>-0.18</v>
       </c>
     </row>
     <row r="125">
@@ -3680,11 +3680,11 @@
         <v>0</v>
       </c>
       <c r="F125" t="n">
-        <v>229.99</v>
+        <v>230</v>
       </c>
       <c r="G125" t="inlineStr"/>
       <c r="H125" t="n">
-        <v>-1.67</v>
+        <v>-1.66</v>
       </c>
     </row>
     <row r="126">
@@ -3706,11 +3706,11 @@
         <v>0</v>
       </c>
       <c r="F126" t="n">
-        <v>7.82</v>
+        <v>8.4</v>
       </c>
       <c r="G126" t="inlineStr"/>
       <c r="H126" t="n">
-        <v>-2.01</v>
+        <v>5.26</v>
       </c>
     </row>
     <row r="127">
@@ -3732,11 +3732,11 @@
         <v>0</v>
       </c>
       <c r="F127" t="n">
-        <v>2.29</v>
+        <v>2.25</v>
       </c>
       <c r="G127" t="inlineStr"/>
       <c r="H127" t="n">
-        <v>-0.43</v>
+        <v>-2.17</v>
       </c>
     </row>
     <row r="128">
@@ -3758,11 +3758,11 @@
         <v>0</v>
       </c>
       <c r="F128" t="n">
-        <v>28.59</v>
+        <v>28.48</v>
       </c>
       <c r="G128" t="inlineStr"/>
       <c r="H128" t="n">
-        <v>-0.73</v>
+        <v>-1.11</v>
       </c>
     </row>
     <row r="129">
@@ -3784,11 +3784,11 @@
         <v>0</v>
       </c>
       <c r="F129" t="n">
-        <v>22.79</v>
+        <v>22.8</v>
       </c>
       <c r="G129" t="inlineStr"/>
       <c r="H129" t="n">
-        <v>-0.48</v>
+        <v>-0.44</v>
       </c>
     </row>
     <row r="130">
@@ -3810,11 +3810,11 @@
         <v>0</v>
       </c>
       <c r="F130" t="n">
-        <v>43.8</v>
+        <v>43</v>
       </c>
       <c r="G130" t="inlineStr"/>
       <c r="H130" t="n">
-        <v>-2.86</v>
+        <v>-4.64</v>
       </c>
     </row>
     <row r="131">
@@ -3836,11 +3836,11 @@
         <v>0</v>
       </c>
       <c r="F131" t="n">
-        <v>11.22</v>
+        <v>11.1</v>
       </c>
       <c r="G131" t="inlineStr"/>
       <c r="H131" t="n">
-        <v>-4.92</v>
+        <v>-5.93</v>
       </c>
     </row>
     <row r="132">
@@ -3862,11 +3862,11 @@
         <v>0</v>
       </c>
       <c r="F132" t="n">
-        <v>25.56</v>
+        <v>24.33</v>
       </c>
       <c r="G132" t="inlineStr"/>
       <c r="H132" t="n">
-        <v>-0.78</v>
+        <v>-5.55</v>
       </c>
     </row>
     <row r="133">
@@ -3888,11 +3888,11 @@
         <v>0</v>
       </c>
       <c r="F133" t="n">
-        <v>32.82</v>
+        <v>34.5</v>
       </c>
       <c r="G133" t="inlineStr"/>
       <c r="H133" t="n">
-        <v>-3.19</v>
+        <v>1.77</v>
       </c>
     </row>
     <row r="134">
@@ -3914,11 +3914,11 @@
         <v>0</v>
       </c>
       <c r="F134" t="n">
-        <v>24.64</v>
+        <v>25</v>
       </c>
       <c r="G134" t="inlineStr"/>
       <c r="H134" t="n">
-        <v>-5.16</v>
+        <v>-3.77</v>
       </c>
     </row>
     <row r="135">
@@ -3940,11 +3940,11 @@
         <v>0</v>
       </c>
       <c r="F135" t="n">
-        <v>235</v>
+        <v>203.5</v>
       </c>
       <c r="G135" t="inlineStr"/>
       <c r="H135" t="n">
-        <v>-2.85</v>
+        <v>-15.87</v>
       </c>
     </row>
     <row r="136">
@@ -3966,11 +3966,11 @@
         <v>0</v>
       </c>
       <c r="F136" t="n">
-        <v>0.38</v>
+        <v>0.4</v>
       </c>
       <c r="G136" t="inlineStr"/>
       <c r="H136" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137">
@@ -4018,11 +4018,11 @@
         <v>0</v>
       </c>
       <c r="F138" t="n">
-        <v>13.86</v>
+        <v>13.5</v>
       </c>
       <c r="G138" t="inlineStr"/>
       <c r="H138" t="n">
-        <v>-1.63</v>
+        <v>-4.19</v>
       </c>
     </row>
     <row r="139">
@@ -4044,11 +4044,11 @@
         <v>0</v>
       </c>
       <c r="F139" t="n">
-        <v>23.81</v>
+        <v>23.37</v>
       </c>
       <c r="G139" t="inlineStr"/>
       <c r="H139" t="n">
-        <v>-3.21</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="140">
@@ -4070,11 +4070,11 @@
         <v>0</v>
       </c>
       <c r="F140" t="n">
-        <v>5</v>
+        <v>4.98</v>
       </c>
       <c r="G140" t="inlineStr"/>
       <c r="H140" t="n">
-        <v>-4.58</v>
+        <v>-4.96</v>
       </c>
     </row>
     <row r="141">
@@ -4096,11 +4096,11 @@
         <v>0</v>
       </c>
       <c r="F141" t="n">
-        <v>661</v>
+        <v>666</v>
       </c>
       <c r="G141" t="inlineStr"/>
       <c r="H141" t="n">
-        <v>-4.89</v>
+        <v>-4.17</v>
       </c>
     </row>
     <row r="142">
@@ -4122,11 +4122,11 @@
         <v>0</v>
       </c>
       <c r="F142" t="n">
-        <v>247</v>
+        <v>243.7</v>
       </c>
       <c r="G142" t="inlineStr"/>
       <c r="H142" t="n">
-        <v>-1.83</v>
+        <v>-3.14</v>
       </c>
     </row>
     <row r="143">
@@ -4148,11 +4148,11 @@
         <v>0</v>
       </c>
       <c r="F143" t="n">
-        <v>210.62</v>
+        <v>202</v>
       </c>
       <c r="G143" t="inlineStr"/>
       <c r="H143" t="n">
-        <v>-5.89</v>
+        <v>-9.74</v>
       </c>
     </row>
     <row r="144">
@@ -4174,11 +4174,11 @@
         <v>0</v>
       </c>
       <c r="F144" t="n">
-        <v>3</v>
+        <v>2.99</v>
       </c>
       <c r="G144" t="inlineStr"/>
       <c r="H144" t="n">
-        <v>0</v>
+        <v>-0.33</v>
       </c>
     </row>
     <row r="145">
@@ -4200,11 +4200,11 @@
         <v>0</v>
       </c>
       <c r="F145" t="n">
-        <v>22.54</v>
+        <v>20.13</v>
       </c>
       <c r="G145" t="inlineStr"/>
       <c r="H145" t="n">
-        <v>-1.14</v>
+        <v>-11.71</v>
       </c>
     </row>
     <row r="146">
@@ -4226,11 +4226,11 @@
         <v>0</v>
       </c>
       <c r="F146" t="n">
-        <v>65.66</v>
+        <v>63.96</v>
       </c>
       <c r="G146" t="inlineStr"/>
       <c r="H146" t="n">
-        <v>-3.23</v>
+        <v>-5.73</v>
       </c>
     </row>
     <row r="147">
@@ -4252,11 +4252,11 @@
         <v>0</v>
       </c>
       <c r="F147" t="n">
-        <v>1692</v>
+        <v>1641.95</v>
       </c>
       <c r="G147" t="inlineStr"/>
       <c r="H147" t="n">
-        <v>-0.35</v>
+        <v>-3.3</v>
       </c>
     </row>
     <row r="148">
@@ -4278,11 +4278,11 @@
         <v>0</v>
       </c>
       <c r="F148" t="n">
-        <v>352.6</v>
+        <v>338</v>
       </c>
       <c r="G148" t="inlineStr"/>
       <c r="H148" t="n">
-        <v>0.74</v>
+        <v>-3.43</v>
       </c>
     </row>
     <row r="149">
@@ -4304,11 +4304,11 @@
         <v>0</v>
       </c>
       <c r="F149" t="n">
-        <v>1.78</v>
+        <v>1.75</v>
       </c>
       <c r="G149" t="inlineStr"/>
       <c r="H149" t="n">
-        <v>-1.11</v>
+        <v>-2.78</v>
       </c>
     </row>
     <row r="150">
@@ -4356,11 +4356,11 @@
         <v>0</v>
       </c>
       <c r="F151" t="n">
-        <v>1.82</v>
+        <v>1.73</v>
       </c>
       <c r="G151" t="inlineStr"/>
       <c r="H151" t="n">
-        <v>0.55</v>
+        <v>-4.42</v>
       </c>
     </row>
     <row r="152">
@@ -4382,11 +4382,11 @@
         <v>0</v>
       </c>
       <c r="F152" t="n">
-        <v>65.84999999999999</v>
+        <v>59</v>
       </c>
       <c r="G152" t="inlineStr"/>
       <c r="H152" t="n">
-        <v>-0.98</v>
+        <v>-11.28</v>
       </c>
     </row>
     <row r="153">
@@ -4408,11 +4408,11 @@
         <v>0</v>
       </c>
       <c r="F153" t="n">
-        <v>544.7</v>
+        <v>539</v>
       </c>
       <c r="G153" t="inlineStr"/>
       <c r="H153" t="n">
-        <v>0.13</v>
+        <v>-0.92</v>
       </c>
     </row>
     <row r="154">
@@ -4434,11 +4434,11 @@
         <v>0</v>
       </c>
       <c r="F154" t="n">
-        <v>31.33</v>
+        <v>30.27</v>
       </c>
       <c r="G154" t="inlineStr"/>
       <c r="H154" t="n">
-        <v>-2.06</v>
+        <v>-5.38</v>
       </c>
     </row>
     <row r="155">
@@ -4460,11 +4460,11 @@
         <v>0</v>
       </c>
       <c r="F155" t="n">
-        <v>21.46</v>
+        <v>21.07</v>
       </c>
       <c r="G155" t="inlineStr"/>
       <c r="H155" t="n">
-        <v>-2.41</v>
+        <v>-4.18</v>
       </c>
     </row>
     <row r="156">
@@ -4486,11 +4486,11 @@
         <v>0</v>
       </c>
       <c r="F156" t="n">
-        <v>261.7</v>
+        <v>257.2</v>
       </c>
       <c r="G156" t="inlineStr"/>
       <c r="H156" t="n">
-        <v>-3.4</v>
+        <v>-5.06</v>
       </c>
     </row>
     <row r="157">
@@ -4512,11 +4512,11 @@
         <v>0</v>
       </c>
       <c r="F157" t="n">
-        <v>171.92</v>
+        <v>167.2</v>
       </c>
       <c r="G157" t="inlineStr"/>
       <c r="H157" t="n">
-        <v>-3.42</v>
+        <v>-6.07</v>
       </c>
     </row>
     <row r="158">
@@ -4538,11 +4538,11 @@
         <v>0</v>
       </c>
       <c r="F158" t="n">
-        <v>23.29</v>
+        <v>23.05</v>
       </c>
       <c r="G158" t="inlineStr"/>
       <c r="H158" t="n">
-        <v>-3.56</v>
+        <v>-4.55</v>
       </c>
     </row>
     <row r="159">
@@ -4564,11 +4564,11 @@
         <v>0</v>
       </c>
       <c r="F159" t="n">
-        <v>154.89</v>
+        <v>164</v>
       </c>
       <c r="G159" t="inlineStr"/>
       <c r="H159" t="n">
-        <v>0.31</v>
+        <v>6.21</v>
       </c>
     </row>
     <row r="160">
@@ -4590,11 +4590,11 @@
         <v>0</v>
       </c>
       <c r="F160" t="n">
-        <v>116</v>
+        <v>117.97</v>
       </c>
       <c r="G160" t="inlineStr"/>
       <c r="H160" t="n">
-        <v>1.36</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="161">
@@ -4616,11 +4616,11 @@
         <v>0</v>
       </c>
       <c r="F161" t="n">
-        <v>29.18</v>
+        <v>28.64</v>
       </c>
       <c r="G161" t="inlineStr"/>
       <c r="H161" t="n">
-        <v>-2.44</v>
+        <v>-4.25</v>
       </c>
     </row>
     <row r="162">
@@ -4642,11 +4642,11 @@
         <v>0</v>
       </c>
       <c r="F162" t="n">
-        <v>314.65</v>
+        <v>305.1</v>
       </c>
       <c r="G162" t="inlineStr"/>
       <c r="H162" t="n">
-        <v>-1.64</v>
+        <v>-4.63</v>
       </c>
     </row>
     <row r="163">
@@ -4668,11 +4668,11 @@
         <v>0</v>
       </c>
       <c r="F163" t="n">
-        <v>1457.9</v>
+        <v>1410</v>
       </c>
       <c r="G163" t="inlineStr"/>
       <c r="H163" t="n">
-        <v>-1.49</v>
+        <v>-4.73</v>
       </c>
     </row>
     <row r="164">
@@ -4694,11 +4694,11 @@
         <v>0</v>
       </c>
       <c r="F164" t="n">
-        <v>281.6</v>
+        <v>279.15</v>
       </c>
       <c r="G164" t="inlineStr"/>
       <c r="H164" t="n">
-        <v>0.21</v>
+        <v>-0.66</v>
       </c>
     </row>
     <row r="165">
@@ -4720,11 +4720,11 @@
         <v>0</v>
       </c>
       <c r="F165" t="n">
-        <v>224.65</v>
+        <v>228.9</v>
       </c>
       <c r="G165" t="inlineStr"/>
       <c r="H165" t="n">
-        <v>0.33</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="166">
@@ -4746,11 +4746,11 @@
         <v>0</v>
       </c>
       <c r="F166" t="n">
-        <v>237.5</v>
+        <v>230</v>
       </c>
       <c r="G166" t="inlineStr"/>
       <c r="H166" t="n">
-        <v>-0.52</v>
+        <v>-3.66</v>
       </c>
     </row>
     <row r="167">
@@ -4772,11 +4772,11 @@
         <v>0</v>
       </c>
       <c r="F167" t="n">
-        <v>162.24</v>
+        <v>161.6</v>
       </c>
       <c r="G167" t="inlineStr"/>
       <c r="H167" t="n">
-        <v>2.68</v>
+        <v>2.28</v>
       </c>
     </row>
     <row r="168">
@@ -4798,11 +4798,11 @@
         <v>0</v>
       </c>
       <c r="F168" t="n">
-        <v>222</v>
+        <v>218.9</v>
       </c>
       <c r="G168" t="inlineStr"/>
       <c r="H168" t="n">
-        <v>-4.7</v>
+        <v>-6.03</v>
       </c>
     </row>
     <row r="169">
@@ -4824,11 +4824,11 @@
         <v>0</v>
       </c>
       <c r="F169" t="n">
-        <v>2.89</v>
+        <v>2.95</v>
       </c>
       <c r="G169" t="inlineStr"/>
       <c r="H169" t="n">
-        <v>0</v>
+        <v>2.08</v>
       </c>
     </row>
     <row r="170">
@@ -4850,11 +4850,11 @@
         <v>0</v>
       </c>
       <c r="F170" t="n">
-        <v>560.1</v>
+        <v>522.2</v>
       </c>
       <c r="G170" t="inlineStr"/>
       <c r="H170" t="n">
-        <v>1.84</v>
+        <v>-5.05</v>
       </c>
     </row>
     <row r="171">
@@ -4876,11 +4876,11 @@
         <v>0</v>
       </c>
       <c r="F171" t="n">
-        <v>236</v>
+        <v>227.05</v>
       </c>
       <c r="G171" t="inlineStr"/>
       <c r="H171" t="n">
-        <v>-3.28</v>
+        <v>-6.95</v>
       </c>
     </row>
     <row r="172">
@@ -4902,11 +4902,11 @@
         <v>0</v>
       </c>
       <c r="F172" t="n">
-        <v>5.88</v>
+        <v>5.73</v>
       </c>
       <c r="G172" t="inlineStr"/>
       <c r="H172" t="n">
-        <v>0.17</v>
+        <v>-2.39</v>
       </c>
     </row>
     <row r="173">
@@ -4928,11 +4928,11 @@
         <v>0</v>
       </c>
       <c r="F173" t="n">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="G173" t="inlineStr"/>
       <c r="H173" t="n">
-        <v>0</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="174">
@@ -4954,11 +4954,11 @@
         <v>0</v>
       </c>
       <c r="F174" t="n">
-        <v>404.25</v>
+        <v>406.75</v>
       </c>
       <c r="G174" t="inlineStr"/>
       <c r="H174" t="n">
-        <v>-2.32</v>
+        <v>-1.72</v>
       </c>
     </row>
     <row r="175">
@@ -4980,11 +4980,11 @@
         <v>0</v>
       </c>
       <c r="F175" t="n">
-        <v>23.32</v>
+        <v>23.56</v>
       </c>
       <c r="G175" t="inlineStr"/>
       <c r="H175" t="n">
-        <v>-2.83</v>
+        <v>-1.83</v>
       </c>
     </row>
     <row r="176">
@@ -5006,11 +5006,11 @@
         <v>0</v>
       </c>
       <c r="F176" t="n">
-        <v>3.47</v>
+        <v>3.3</v>
       </c>
       <c r="G176" t="inlineStr"/>
       <c r="H176" t="n">
-        <v>-0.57</v>
+        <v>-5.44</v>
       </c>
     </row>
     <row r="177">
@@ -5032,11 +5032,11 @@
         <v>0</v>
       </c>
       <c r="F177" t="n">
-        <v>237.85</v>
+        <v>231.5</v>
       </c>
       <c r="G177" t="inlineStr"/>
       <c r="H177" t="n">
-        <v>-1.69</v>
+        <v>-4.32</v>
       </c>
     </row>
     <row r="178">
@@ -5058,11 +5058,11 @@
         <v>0</v>
       </c>
       <c r="F178" t="n">
-        <v>15.93</v>
+        <v>13.5</v>
       </c>
       <c r="G178" t="inlineStr"/>
       <c r="H178" t="n">
-        <v>17.56</v>
+        <v>-0.37</v>
       </c>
     </row>
     <row r="179">
@@ -5084,11 +5084,11 @@
         <v>0</v>
       </c>
       <c r="F179" t="n">
-        <v>264.8</v>
+        <v>270.8</v>
       </c>
       <c r="G179" t="inlineStr"/>
       <c r="H179" t="n">
-        <v>0.23</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="180">
@@ -5110,11 +5110,11 @@
         <v>0</v>
       </c>
       <c r="F180" t="n">
-        <v>63.52</v>
+        <v>62.3</v>
       </c>
       <c r="G180" t="inlineStr"/>
       <c r="H180" t="n">
-        <v>-1.21</v>
+        <v>-3.11</v>
       </c>
     </row>
     <row r="181">
@@ -5136,11 +5136,11 @@
         <v>0</v>
       </c>
       <c r="F181" t="n">
-        <v>7.19</v>
+        <v>7.1</v>
       </c>
       <c r="G181" t="inlineStr"/>
       <c r="H181" t="n">
-        <v>1.99</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="182">
@@ -5162,11 +5162,11 @@
         <v>0</v>
       </c>
       <c r="F182" t="n">
-        <v>44.84</v>
+        <v>41</v>
       </c>
       <c r="G182" t="inlineStr"/>
       <c r="H182" t="n">
-        <v>-3.05</v>
+        <v>-11.35</v>
       </c>
     </row>
     <row r="183">
@@ -5188,11 +5188,11 @@
         <v>0</v>
       </c>
       <c r="F183" t="n">
-        <v>30.85</v>
+        <v>29.43</v>
       </c>
       <c r="G183" t="inlineStr"/>
       <c r="H183" t="n">
-        <v>2.83</v>
+        <v>-1.9</v>
       </c>
     </row>
     <row r="184">
@@ -5214,11 +5214,11 @@
         <v>0</v>
       </c>
       <c r="F184" t="n">
-        <v>3.02</v>
+        <v>2.94</v>
       </c>
       <c r="G184" t="inlineStr"/>
       <c r="H184" t="n">
-        <v>-0.98</v>
+        <v>-3.61</v>
       </c>
     </row>
     <row r="185">
@@ -5240,11 +5240,11 @@
         <v>0</v>
       </c>
       <c r="F185" t="n">
-        <v>92.70999999999999</v>
+        <v>91.86</v>
       </c>
       <c r="G185" t="inlineStr"/>
       <c r="H185" t="n">
-        <v>-2.05</v>
+        <v>-2.95</v>
       </c>
     </row>
     <row r="186">
@@ -5266,11 +5266,11 @@
         <v>0</v>
       </c>
       <c r="F186" t="n">
-        <v>0.51</v>
+        <v>0.48</v>
       </c>
       <c r="G186" t="inlineStr"/>
       <c r="H186" t="n">
-        <v>0</v>
+        <v>-5.88</v>
       </c>
     </row>
     <row r="187">
@@ -5292,11 +5292,11 @@
         <v>0</v>
       </c>
       <c r="F187" t="n">
-        <v>44.6</v>
+        <v>43.5</v>
       </c>
       <c r="G187" t="inlineStr"/>
       <c r="H187" t="n">
-        <v>-0.67</v>
+        <v>-3.12</v>
       </c>
     </row>
     <row r="188">
@@ -5344,11 +5344,11 @@
         <v>0</v>
       </c>
       <c r="F189" t="n">
-        <v>79.06</v>
+        <v>78</v>
       </c>
       <c r="G189" t="inlineStr"/>
       <c r="H189" t="n">
-        <v>-3.47</v>
+        <v>-4.76</v>
       </c>
     </row>
     <row r="190">
@@ -5370,11 +5370,11 @@
         <v>0</v>
       </c>
       <c r="F190" t="n">
-        <v>261.4</v>
+        <v>250.6</v>
       </c>
       <c r="G190" t="inlineStr"/>
       <c r="H190" t="n">
-        <v>-2.83</v>
+        <v>-6.84</v>
       </c>
     </row>
     <row r="191">
@@ -5396,11 +5396,11 @@
         <v>0</v>
       </c>
       <c r="F191" t="n">
-        <v>14.58</v>
+        <v>14.12</v>
       </c>
       <c r="G191" t="inlineStr"/>
       <c r="H191" t="n">
-        <v>1.25</v>
+        <v>-1.94</v>
       </c>
     </row>
     <row r="192">
@@ -5422,11 +5422,11 @@
         <v>0</v>
       </c>
       <c r="F192" t="n">
-        <v>20.59</v>
+        <v>20.7</v>
       </c>
       <c r="G192" t="inlineStr"/>
       <c r="H192" t="n">
-        <v>-2.51</v>
+        <v>-1.99</v>
       </c>
     </row>
     <row r="193">
@@ -5448,11 +5448,11 @@
         <v>0</v>
       </c>
       <c r="F193" t="n">
-        <v>85.29000000000001</v>
+        <v>81.90000000000001</v>
       </c>
       <c r="G193" t="inlineStr"/>
       <c r="H193" t="n">
-        <v>-0.07000000000000001</v>
+        <v>-4.04</v>
       </c>
     </row>
     <row r="194">
@@ -5474,11 +5474,11 @@
         <v>0</v>
       </c>
       <c r="F194" t="n">
-        <v>45.13</v>
+        <v>40.7</v>
       </c>
       <c r="G194" t="inlineStr"/>
       <c r="H194" t="n">
-        <v>-1.87</v>
+        <v>-11.5</v>
       </c>
     </row>
     <row r="195">
@@ -5500,11 +5500,11 @@
         <v>0</v>
       </c>
       <c r="F195" t="n">
-        <v>170.3</v>
+        <v>165</v>
       </c>
       <c r="G195" t="inlineStr"/>
       <c r="H195" t="n">
-        <v>0.18</v>
+        <v>-2.94</v>
       </c>
     </row>
     <row r="196">
@@ -5526,11 +5526,11 @@
         <v>0</v>
       </c>
       <c r="F196" t="n">
-        <v>2.06</v>
+        <v>2.08</v>
       </c>
       <c r="G196" t="inlineStr"/>
       <c r="H196" t="n">
-        <v>-0.96</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197">
@@ -5552,11 +5552,11 @@
         <v>0</v>
       </c>
       <c r="F197" t="n">
-        <v>155.4</v>
+        <v>152.7</v>
       </c>
       <c r="G197" t="inlineStr"/>
       <c r="H197" t="n">
-        <v>6.44</v>
+        <v>4.59</v>
       </c>
     </row>
     <row r="198">
@@ -5578,11 +5578,11 @@
         <v>0</v>
       </c>
       <c r="F198" t="n">
-        <v>12.17</v>
+        <v>12</v>
       </c>
       <c r="G198" t="inlineStr"/>
       <c r="H198" t="n">
-        <v>-2.48</v>
+        <v>-3.85</v>
       </c>
     </row>
     <row r="199">
@@ -5604,11 +5604,11 @@
         <v>0</v>
       </c>
       <c r="F199" t="n">
-        <v>63.62</v>
+        <v>61.57</v>
       </c>
       <c r="G199" t="inlineStr"/>
       <c r="H199" t="n">
-        <v>-1.82</v>
+        <v>-4.98</v>
       </c>
     </row>
     <row r="200">
@@ -5630,11 +5630,11 @@
         <v>0</v>
       </c>
       <c r="F200" t="n">
-        <v>34.28</v>
+        <v>33.4</v>
       </c>
       <c r="G200" t="inlineStr"/>
       <c r="H200" t="n">
-        <v>-1.49</v>
+        <v>-4.02</v>
       </c>
     </row>
     <row r="201">
@@ -5656,11 +5656,11 @@
         <v>0</v>
       </c>
       <c r="F201" t="n">
-        <v>5.8</v>
+        <v>5.6</v>
       </c>
       <c r="G201" t="inlineStr"/>
       <c r="H201" t="n">
-        <v>0</v>
+        <v>-3.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>